<commit_message>
segundo ejercicio extra cooperativo
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -511,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1348,7 @@
       <c r="B50" s="5">
         <v>11</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="8">
         <v>45110</v>
       </c>
       <c r="D50" s="6">
@@ -2740,18 +2740,18 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="E40:E59"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F57:F58"/>
     <mergeCell ref="E30:E39"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E13:E17"/>
     <mergeCell ref="E19:E26"/>
-    <mergeCell ref="E40:E59"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="F51:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F57:F58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
inicio ej5 extra de la guia
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -121,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +131,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -162,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,6 +210,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -510,8 +519,8 @@
   <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1139,7 @@
       <c r="B37" s="5">
         <v>8</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="15">
         <v>45083</v>
       </c>
       <c r="D37" s="6">
@@ -1366,7 +1375,7 @@
       <c r="B51" s="5">
         <v>12</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="15">
         <v>45111</v>
       </c>
       <c r="D51" s="6">
@@ -1384,7 +1393,7 @@
       <c r="B52" s="5">
         <v>13</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="8">
         <v>45112</v>
       </c>
       <c r="D52" s="6">
@@ -2740,18 +2749,18 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="E30:E39"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="E19:E26"/>
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="F40:F43"/>
     <mergeCell ref="F46:F49"/>
     <mergeCell ref="F51:F54"/>
     <mergeCell ref="F55:F56"/>
     <mergeCell ref="F57:F58"/>
-    <mergeCell ref="E30:E39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E19:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ej 6 extra ahorcado
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -203,6 +203,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -210,9 +213,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,7 +520,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +581,7 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -599,7 +599,7 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -615,7 +615,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5"/>
@@ -633,7 +633,7 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="5"/>
@@ -683,7 +683,7 @@
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -699,7 +699,7 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
       <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,7 +749,7 @@
       <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5"/>
@@ -767,7 +767,7 @@
       <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
       <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
       <c r="D17" s="6">
         <v>4</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5"/>
@@ -867,7 +867,7 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
       <c r="D24" s="6">
         <v>5</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -947,7 +947,7 @@
       <c r="D25" s="6">
         <v>5</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -963,7 +963,7 @@
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
       <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5"/>
@@ -1049,7 +1049,7 @@
       <c r="D31" s="6">
         <v>7</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="13"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
       <c r="D32" s="6">
         <v>7</v>
       </c>
-      <c r="E32" s="12"/>
+      <c r="E32" s="13"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1081,7 +1081,7 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="13"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
       <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="E34" s="12"/>
+      <c r="E34" s="13"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
       <c r="D35" s="6">
         <v>7</v>
       </c>
-      <c r="E35" s="12"/>
+      <c r="E35" s="13"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
       <c r="D36" s="6">
         <v>7</v>
       </c>
-      <c r="E36" s="12"/>
+      <c r="E36" s="13"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1139,13 +1139,13 @@
       <c r="B37" s="5">
         <v>8</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="12">
         <v>45083</v>
       </c>
       <c r="D37" s="6">
         <v>7</v>
       </c>
-      <c r="E37" s="12"/>
+      <c r="E37" s="13"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1161,7 +1161,7 @@
       <c r="D38" s="6">
         <v>7</v>
       </c>
-      <c r="E38" s="12"/>
+      <c r="E38" s="13"/>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1177,7 +1177,7 @@
       <c r="D39" s="6">
         <v>7</v>
       </c>
-      <c r="E39" s="12"/>
+      <c r="E39" s="13"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1193,10 +1193,10 @@
       <c r="D40" s="6">
         <v>8</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="F40" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1213,8 +1213,8 @@
       <c r="D41" s="6">
         <v>8</v>
       </c>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1229,8 +1229,8 @@
       <c r="D42" s="6">
         <v>8</v>
       </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1245,8 +1245,8 @@
       <c r="D43" s="6">
         <v>8</v>
       </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1261,7 +1261,7 @@
       <c r="D44" s="6">
         <v>8</v>
       </c>
-      <c r="E44" s="12"/>
+      <c r="E44" s="13"/>
       <c r="F44" s="11" t="s">
         <v>23</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="12"/>
+      <c r="E45" s="13"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1297,8 +1297,8 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="13" t="s">
+      <c r="E46" s="13"/>
+      <c r="F46" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1315,8 +1315,8 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1331,8 +1331,8 @@
       <c r="D48" s="6">
         <v>8</v>
       </c>
-      <c r="E48" s="12"/>
-      <c r="F48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1347,8 +1347,8 @@
       <c r="D49" s="6">
         <v>8</v>
       </c>
-      <c r="E49" s="12"/>
-      <c r="F49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1363,7 +1363,7 @@
       <c r="D50" s="6">
         <v>8</v>
       </c>
-      <c r="E50" s="12"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1375,14 +1375,14 @@
       <c r="B51" s="5">
         <v>12</v>
       </c>
-      <c r="C51" s="15">
+      <c r="C51" s="12">
         <v>45111</v>
       </c>
       <c r="D51" s="6">
         <v>8</v>
       </c>
-      <c r="E51" s="12"/>
-      <c r="F51" s="14" t="s">
+      <c r="E51" s="13"/>
+      <c r="F51" s="15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1399,8 +1399,8 @@
       <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="14"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="15"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1409,14 +1409,14 @@
       <c r="B53" s="5">
         <v>14</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="8">
         <v>45113</v>
       </c>
       <c r="D53" s="6">
         <v>8</v>
       </c>
-      <c r="E53" s="12"/>
-      <c r="F53" s="14"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="15"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1431,8 +1431,8 @@
       <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E54" s="12"/>
-      <c r="F54" s="14"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="15"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1447,8 +1447,8 @@
       <c r="D55" s="6">
         <v>8</v>
       </c>
-      <c r="E55" s="12"/>
-      <c r="F55" s="13" t="s">
+      <c r="E55" s="13"/>
+      <c r="F55" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1465,8 +1465,8 @@
       <c r="D56" s="6">
         <v>8</v>
       </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1481,8 +1481,8 @@
       <c r="D57" s="6">
         <v>8</v>
       </c>
-      <c r="E57" s="12"/>
-      <c r="F57" s="13" t="s">
+      <c r="E57" s="13"/>
+      <c r="F57" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1499,8 +1499,8 @@
       <c r="D58" s="6">
         <v>8</v>
       </c>
-      <c r="E58" s="12"/>
-      <c r="F58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="14"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1515,7 +1515,7 @@
       <c r="D59" s="6">
         <v>8</v>
       </c>
-      <c r="E59" s="12"/>
+      <c r="E59" s="13"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
ejercicios 1 y 2
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -304,6 +304,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -315,18 +327,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,7 +633,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E62" sqref="E62:E70"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="19" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -714,7 +714,7 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="19" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -752,7 +752,7 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -808,7 +808,7 @@
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -826,7 +826,7 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="22"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -844,7 +844,7 @@
       <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="22"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -882,7 +882,7 @@
       <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -902,7 +902,7 @@
       <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="22"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="22"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="22"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -956,7 +956,7 @@
       <c r="D17" s="6">
         <v>4</v>
       </c>
-      <c r="E17" s="22"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1014,7 +1014,7 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="22"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="22"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="22"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="22"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="D24" s="6">
         <v>5</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="D25" s="6">
         <v>5</v>
       </c>
-      <c r="E25" s="22"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="22"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="19" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1220,7 +1220,7 @@
       <c r="D31" s="6">
         <v>7</v>
       </c>
-      <c r="E31" s="22"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="D32" s="6">
         <v>7</v>
       </c>
-      <c r="E32" s="22"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
-      <c r="E33" s="22"/>
+      <c r="E33" s="19"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="E34" s="22"/>
+      <c r="E34" s="19"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="D35" s="6">
         <v>7</v>
       </c>
-      <c r="E35" s="22"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="D36" s="6">
         <v>7</v>
       </c>
-      <c r="E36" s="22"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="D37" s="6">
         <v>7</v>
       </c>
-      <c r="E37" s="22"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="D38" s="6">
         <v>7</v>
       </c>
-      <c r="E38" s="22"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="D39" s="6">
         <v>7</v>
       </c>
-      <c r="E39" s="22"/>
+      <c r="E39" s="19"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1382,10 +1382,10 @@
       <c r="D40" s="6">
         <v>8</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="22" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1402,8 +1402,8 @@
       <c r="D41" s="6">
         <v>8</v>
       </c>
-      <c r="E41" s="22"/>
-      <c r="F41" s="18"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1418,8 +1418,8 @@
       <c r="D42" s="6">
         <v>8</v>
       </c>
-      <c r="E42" s="22"/>
-      <c r="F42" s="18"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1434,8 +1434,8 @@
       <c r="D43" s="6">
         <v>8</v>
       </c>
-      <c r="E43" s="22"/>
-      <c r="F43" s="18"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1450,7 +1450,7 @@
       <c r="D44" s="6">
         <v>8</v>
       </c>
-      <c r="E44" s="22"/>
+      <c r="E44" s="19"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="22"/>
+      <c r="E45" s="19"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1486,8 +1486,8 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="22"/>
-      <c r="F46" s="18" t="s">
+      <c r="E46" s="19"/>
+      <c r="F46" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1504,8 +1504,8 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-      <c r="E47" s="22"/>
-      <c r="F47" s="18"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1520,8 +1520,8 @@
       <c r="D48" s="6">
         <v>8</v>
       </c>
-      <c r="E48" s="22"/>
-      <c r="F48" s="18"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1536,8 +1536,8 @@
       <c r="D49" s="6">
         <v>8</v>
       </c>
-      <c r="E49" s="22"/>
-      <c r="F49" s="18"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1552,7 +1552,7 @@
       <c r="D50" s="6">
         <v>8</v>
       </c>
-      <c r="E50" s="22"/>
+      <c r="E50" s="19"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1570,8 +1570,8 @@
       <c r="D51" s="6">
         <v>8</v>
       </c>
-      <c r="E51" s="22"/>
-      <c r="F51" s="19" t="s">
+      <c r="E51" s="19"/>
+      <c r="F51" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1588,8 +1588,8 @@
       <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="22"/>
-      <c r="F52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1604,8 +1604,8 @@
       <c r="D53" s="6">
         <v>8</v>
       </c>
-      <c r="E53" s="22"/>
-      <c r="F53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="23"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1620,8 +1620,8 @@
       <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E54" s="22"/>
-      <c r="F54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="23"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1636,8 +1636,8 @@
       <c r="D55" s="6">
         <v>8</v>
       </c>
-      <c r="E55" s="22"/>
-      <c r="F55" s="18" t="s">
+      <c r="E55" s="19"/>
+      <c r="F55" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1654,8 +1654,8 @@
       <c r="D56" s="6">
         <v>8</v>
       </c>
-      <c r="E56" s="22"/>
-      <c r="F56" s="18"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1670,8 +1670,8 @@
       <c r="D57" s="6">
         <v>8</v>
       </c>
-      <c r="E57" s="22"/>
-      <c r="F57" s="18" t="s">
+      <c r="E57" s="19"/>
+      <c r="F57" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1688,8 +1688,8 @@
       <c r="D58" s="6">
         <v>8</v>
       </c>
-      <c r="E58" s="22"/>
-      <c r="F58" s="18"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="22"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1704,7 +1704,7 @@
       <c r="D59" s="6">
         <v>8</v>
       </c>
-      <c r="E59" s="22"/>
+      <c r="E59" s="19"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1722,10 +1722,10 @@
       <c r="D60" s="6">
         <v>9</v>
       </c>
-      <c r="E60" s="20" t="s">
+      <c r="E60" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F60" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1742,8 +1742,8 @@
       <c r="D61" s="6">
         <v>9</v>
       </c>
-      <c r="E61" s="21"/>
-      <c r="F61" s="17"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="21"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1752,13 +1752,13 @@
       <c r="B62" s="5">
         <v>1</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="8">
         <v>45131</v>
       </c>
       <c r="D62" s="6">
         <v>10</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="16" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1770,13 +1770,13 @@
       <c r="B63" s="5">
         <v>2</v>
       </c>
-      <c r="C63" s="9">
+      <c r="C63" s="8">
         <v>45132</v>
       </c>
       <c r="D63" s="6">
         <v>10</v>
       </c>
-      <c r="E63" s="23"/>
+      <c r="E63" s="17"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
       <c r="D64" s="6">
         <v>10</v>
       </c>
-      <c r="E64" s="23"/>
+      <c r="E64" s="17"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
       <c r="D65" s="6">
         <v>10</v>
       </c>
-      <c r="E65" s="23"/>
+      <c r="E65" s="17"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
       <c r="D66" s="6">
         <v>10</v>
       </c>
-      <c r="E66" s="23"/>
+      <c r="E66" s="17"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
       <c r="D67" s="6">
         <v>10</v>
       </c>
-      <c r="E67" s="23"/>
+      <c r="E67" s="17"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
       <c r="D68" s="6">
         <v>10</v>
       </c>
-      <c r="E68" s="23"/>
+      <c r="E68" s="17"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
       <c r="D69" s="6">
         <v>10</v>
       </c>
-      <c r="E69" s="23"/>
+      <c r="E69" s="17"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
       <c r="D70" s="6">
         <v>10</v>
       </c>
-      <c r="E70" s="21"/>
+      <c r="E70" s="18"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -3264,6 +3264,12 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="15">
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F57:F58"/>
     <mergeCell ref="E62:E70"/>
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E30:E39"/>
@@ -3273,12 +3279,6 @@
     <mergeCell ref="E13:E17"/>
     <mergeCell ref="E19:E26"/>
     <mergeCell ref="E40:E59"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="F51:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F57:F58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
iniciando ej 6 colecciones
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -304,6 +304,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -324,9 +327,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,8 +632,8 @@
   <dimension ref="A1:F179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -714,7 +714,7 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -752,7 +752,7 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="16" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -808,7 +808,7 @@
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -826,7 +826,7 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -844,7 +844,7 @@
       <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -882,7 +882,7 @@
       <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -902,7 +902,7 @@
       <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="23"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -956,7 +956,7 @@
       <c r="D17" s="6">
         <v>4</v>
       </c>
-      <c r="E17" s="23"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1014,7 +1014,7 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="23"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="23"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="23"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="23"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="D24" s="6">
         <v>5</v>
       </c>
-      <c r="E24" s="23"/>
+      <c r="E24" s="16"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="D25" s="6">
         <v>5</v>
       </c>
-      <c r="E25" s="23"/>
+      <c r="E25" s="16"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="23"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1220,7 +1220,7 @@
       <c r="D31" s="6">
         <v>7</v>
       </c>
-      <c r="E31" s="23"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="D32" s="6">
         <v>7</v>
       </c>
-      <c r="E32" s="23"/>
+      <c r="E32" s="16"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
-      <c r="E33" s="23"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="E34" s="23"/>
+      <c r="E34" s="16"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="D35" s="6">
         <v>7</v>
       </c>
-      <c r="E35" s="23"/>
+      <c r="E35" s="16"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="D36" s="6">
         <v>7</v>
       </c>
-      <c r="E36" s="23"/>
+      <c r="E36" s="16"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="D37" s="6">
         <v>7</v>
       </c>
-      <c r="E37" s="23"/>
+      <c r="E37" s="16"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="D38" s="6">
         <v>7</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="16"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="D39" s="6">
         <v>7</v>
       </c>
-      <c r="E39" s="23"/>
+      <c r="E39" s="16"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1382,10 +1382,10 @@
       <c r="D40" s="6">
         <v>8</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="22" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1402,8 +1402,8 @@
       <c r="D41" s="6">
         <v>8</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="21"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1418,8 +1418,8 @@
       <c r="D42" s="6">
         <v>8</v>
       </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="21"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1434,8 +1434,8 @@
       <c r="D43" s="6">
         <v>8</v>
       </c>
-      <c r="E43" s="23"/>
-      <c r="F43" s="21"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1450,7 +1450,7 @@
       <c r="D44" s="6">
         <v>8</v>
       </c>
-      <c r="E44" s="23"/>
+      <c r="E44" s="16"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="23"/>
+      <c r="E45" s="16"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1486,8 +1486,8 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="23"/>
-      <c r="F46" s="21" t="s">
+      <c r="E46" s="16"/>
+      <c r="F46" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1504,8 +1504,8 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-      <c r="E47" s="23"/>
-      <c r="F47" s="21"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1520,8 +1520,8 @@
       <c r="D48" s="6">
         <v>8</v>
       </c>
-      <c r="E48" s="23"/>
-      <c r="F48" s="21"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1536,8 +1536,8 @@
       <c r="D49" s="6">
         <v>8</v>
       </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="21"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1552,7 +1552,7 @@
       <c r="D50" s="6">
         <v>8</v>
       </c>
-      <c r="E50" s="23"/>
+      <c r="E50" s="16"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1570,8 +1570,8 @@
       <c r="D51" s="6">
         <v>8</v>
       </c>
-      <c r="E51" s="23"/>
-      <c r="F51" s="22" t="s">
+      <c r="E51" s="16"/>
+      <c r="F51" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1588,8 +1588,8 @@
       <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="23"/>
-      <c r="F52" s="22"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1604,8 +1604,8 @@
       <c r="D53" s="6">
         <v>8</v>
       </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="22"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="23"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1620,8 +1620,8 @@
       <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E54" s="23"/>
-      <c r="F54" s="22"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="23"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1636,8 +1636,8 @@
       <c r="D55" s="6">
         <v>8</v>
       </c>
-      <c r="E55" s="23"/>
-      <c r="F55" s="21" t="s">
+      <c r="E55" s="16"/>
+      <c r="F55" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1654,8 +1654,8 @@
       <c r="D56" s="6">
         <v>8</v>
       </c>
-      <c r="E56" s="23"/>
-      <c r="F56" s="21"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1670,8 +1670,8 @@
       <c r="D57" s="6">
         <v>8</v>
       </c>
-      <c r="E57" s="23"/>
-      <c r="F57" s="21" t="s">
+      <c r="E57" s="16"/>
+      <c r="F57" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1688,8 +1688,8 @@
       <c r="D58" s="6">
         <v>8</v>
       </c>
-      <c r="E58" s="23"/>
-      <c r="F58" s="21"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="22"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1704,7 +1704,7 @@
       <c r="D59" s="6">
         <v>8</v>
       </c>
-      <c r="E59" s="23"/>
+      <c r="E59" s="16"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1722,10 +1722,10 @@
       <c r="D60" s="6">
         <v>9</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E60" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="19" t="s">
+      <c r="F60" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1742,8 +1742,8 @@
       <c r="D61" s="6">
         <v>9</v>
       </c>
-      <c r="E61" s="18"/>
-      <c r="F61" s="20"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="21"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1758,7 +1758,7 @@
       <c r="D62" s="6">
         <v>10</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="17" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1776,7 +1776,7 @@
       <c r="D63" s="6">
         <v>10</v>
       </c>
-      <c r="E63" s="17"/>
+      <c r="E63" s="18"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
       <c r="D64" s="6">
         <v>10</v>
       </c>
-      <c r="E64" s="17"/>
+      <c r="E64" s="18"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
       <c r="D65" s="6">
         <v>10</v>
       </c>
-      <c r="E65" s="17"/>
+      <c r="E65" s="18"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1818,13 +1818,13 @@
       <c r="B66" s="5">
         <v>5</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="8">
         <v>45138</v>
       </c>
       <c r="D66" s="6">
         <v>10</v>
       </c>
-      <c r="E66" s="17"/>
+      <c r="E66" s="18"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
       <c r="D67" s="6">
         <v>10</v>
       </c>
-      <c r="E67" s="17"/>
+      <c r="E67" s="18"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
       <c r="D68" s="6">
         <v>10</v>
       </c>
-      <c r="E68" s="17"/>
+      <c r="E68" s="18"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
       <c r="D69" s="6">
         <v>10</v>
       </c>
-      <c r="E69" s="17"/>
+      <c r="E69" s="18"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
       <c r="D70" s="6">
         <v>10</v>
       </c>
-      <c r="E70" s="18"/>
+      <c r="E70" s="19"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="16" t="s">
+      <c r="E153" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2906,7 +2906,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="17"/>
+      <c r="E154" s="18"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2920,7 +2920,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="17"/>
+      <c r="E155" s="18"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="17"/>
+      <c r="E156" s="18"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2948,7 +2948,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="17"/>
+      <c r="E157" s="18"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -2962,7 +2962,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="17"/>
+      <c r="E158" s="18"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -2976,7 +2976,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="17"/>
+      <c r="E159" s="18"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -2990,7 +2990,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="17"/>
+      <c r="E160" s="18"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,7 +3004,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="17"/>
+      <c r="E161" s="18"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="17"/>
+      <c r="E162" s="18"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="17"/>
+      <c r="E163" s="18"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3046,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="17"/>
+      <c r="E164" s="18"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3060,7 +3060,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="17"/>
+      <c r="E165" s="18"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3074,7 +3074,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="17"/>
+      <c r="E166" s="18"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="17"/>
+      <c r="E167" s="18"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3102,7 +3102,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="17"/>
+      <c r="E168" s="18"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3116,7 +3116,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="17"/>
+      <c r="E169" s="18"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3130,7 +3130,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="17"/>
+      <c r="E170" s="18"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3144,7 +3144,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="17"/>
+      <c r="E171" s="18"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3158,7 +3158,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="17"/>
+      <c r="E172" s="18"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3172,7 +3172,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="17"/>
+      <c r="E173" s="18"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3186,7 +3186,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="17"/>
+      <c r="E174" s="18"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="17"/>
+      <c r="E175" s="18"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3214,7 +3214,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="17"/>
+      <c r="E176" s="18"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3228,7 +3228,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="17"/>
+      <c r="E177" s="18"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="17"/>
+      <c r="E178" s="18"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3256,7 +3256,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="18"/>
+      <c r="E179" s="19"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3264,12 +3264,6 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="E30:E39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E19:E26"/>
     <mergeCell ref="E153:E179"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="F40:F43"/>
@@ -3280,6 +3274,12 @@
     <mergeCell ref="E62:E70"/>
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
+    <mergeCell ref="E30:E39"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="E19:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
colecciones iniciando ejercicio 6
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -304,9 +304,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -327,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,8 +632,8 @@
   <dimension ref="A1:F179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -714,7 +714,7 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -752,7 +752,7 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="16"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -808,7 +808,7 @@
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -826,7 +826,7 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -844,7 +844,7 @@
       <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -882,7 +882,7 @@
       <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -902,7 +902,7 @@
       <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="16"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="16"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -956,7 +956,7 @@
       <c r="D17" s="6">
         <v>4</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1014,7 +1014,7 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="D24" s="6">
         <v>5</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="D25" s="6">
         <v>5</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="16"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="23" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1220,7 +1220,7 @@
       <c r="D31" s="6">
         <v>7</v>
       </c>
-      <c r="E31" s="16"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="D32" s="6">
         <v>7</v>
       </c>
-      <c r="E32" s="16"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
-      <c r="E33" s="16"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="E34" s="16"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="D35" s="6">
         <v>7</v>
       </c>
-      <c r="E35" s="16"/>
+      <c r="E35" s="23"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="D36" s="6">
         <v>7</v>
       </c>
-      <c r="E36" s="16"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="D37" s="6">
         <v>7</v>
       </c>
-      <c r="E37" s="16"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="D38" s="6">
         <v>7</v>
       </c>
-      <c r="E38" s="16"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="D39" s="6">
         <v>7</v>
       </c>
-      <c r="E39" s="16"/>
+      <c r="E39" s="23"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1382,10 +1382,10 @@
       <c r="D40" s="6">
         <v>8</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1402,8 +1402,8 @@
       <c r="D41" s="6">
         <v>8</v>
       </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="22"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1418,8 +1418,8 @@
       <c r="D42" s="6">
         <v>8</v>
       </c>
-      <c r="E42" s="16"/>
-      <c r="F42" s="22"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1434,8 +1434,8 @@
       <c r="D43" s="6">
         <v>8</v>
       </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="22"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1450,7 +1450,7 @@
       <c r="D44" s="6">
         <v>8</v>
       </c>
-      <c r="E44" s="16"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="16"/>
+      <c r="E45" s="23"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1486,8 +1486,8 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="16"/>
-      <c r="F46" s="22" t="s">
+      <c r="E46" s="23"/>
+      <c r="F46" s="21" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1504,8 +1504,8 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-      <c r="E47" s="16"/>
-      <c r="F47" s="22"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1520,8 +1520,8 @@
       <c r="D48" s="6">
         <v>8</v>
       </c>
-      <c r="E48" s="16"/>
-      <c r="F48" s="22"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1536,8 +1536,8 @@
       <c r="D49" s="6">
         <v>8</v>
       </c>
-      <c r="E49" s="16"/>
-      <c r="F49" s="22"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1552,7 +1552,7 @@
       <c r="D50" s="6">
         <v>8</v>
       </c>
-      <c r="E50" s="16"/>
+      <c r="E50" s="23"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1570,8 +1570,8 @@
       <c r="D51" s="6">
         <v>8</v>
       </c>
-      <c r="E51" s="16"/>
-      <c r="F51" s="23" t="s">
+      <c r="E51" s="23"/>
+      <c r="F51" s="22" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1588,8 +1588,8 @@
       <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="22"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1604,8 +1604,8 @@
       <c r="D53" s="6">
         <v>8</v>
       </c>
-      <c r="E53" s="16"/>
-      <c r="F53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="22"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1620,8 +1620,8 @@
       <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E54" s="16"/>
-      <c r="F54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="22"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1636,8 +1636,8 @@
       <c r="D55" s="6">
         <v>8</v>
       </c>
-      <c r="E55" s="16"/>
-      <c r="F55" s="22" t="s">
+      <c r="E55" s="23"/>
+      <c r="F55" s="21" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1654,8 +1654,8 @@
       <c r="D56" s="6">
         <v>8</v>
       </c>
-      <c r="E56" s="16"/>
-      <c r="F56" s="22"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1670,8 +1670,8 @@
       <c r="D57" s="6">
         <v>8</v>
       </c>
-      <c r="E57" s="16"/>
-      <c r="F57" s="22" t="s">
+      <c r="E57" s="23"/>
+      <c r="F57" s="21" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1688,8 +1688,8 @@
       <c r="D58" s="6">
         <v>8</v>
       </c>
-      <c r="E58" s="16"/>
-      <c r="F58" s="22"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="21"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1704,7 +1704,7 @@
       <c r="D59" s="6">
         <v>8</v>
       </c>
-      <c r="E59" s="16"/>
+      <c r="E59" s="23"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1722,10 +1722,10 @@
       <c r="D60" s="6">
         <v>9</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="19" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1742,8 +1742,8 @@
       <c r="D61" s="6">
         <v>9</v>
       </c>
-      <c r="E61" s="19"/>
-      <c r="F61" s="21"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="20"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1758,7 +1758,7 @@
       <c r="D62" s="6">
         <v>10</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E62" s="16" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1776,7 +1776,7 @@
       <c r="D63" s="6">
         <v>10</v>
       </c>
-      <c r="E63" s="18"/>
+      <c r="E63" s="17"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
       <c r="D64" s="6">
         <v>10</v>
       </c>
-      <c r="E64" s="18"/>
+      <c r="E64" s="17"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
       <c r="D65" s="6">
         <v>10</v>
       </c>
-      <c r="E65" s="18"/>
+      <c r="E65" s="17"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
       <c r="D66" s="6">
         <v>10</v>
       </c>
-      <c r="E66" s="18"/>
+      <c r="E66" s="17"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,13 +1834,13 @@
       <c r="B67" s="5">
         <v>6</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="11">
         <v>45139</v>
       </c>
       <c r="D67" s="6">
         <v>10</v>
       </c>
-      <c r="E67" s="18"/>
+      <c r="E67" s="17"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1850,13 +1850,13 @@
       <c r="B68" s="5">
         <v>7</v>
       </c>
-      <c r="C68" s="9">
+      <c r="C68" s="8">
         <v>45140</v>
       </c>
       <c r="D68" s="6">
         <v>10</v>
       </c>
-      <c r="E68" s="18"/>
+      <c r="E68" s="17"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
       <c r="D69" s="6">
         <v>10</v>
       </c>
-      <c r="E69" s="18"/>
+      <c r="E69" s="17"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
       <c r="D70" s="6">
         <v>10</v>
       </c>
-      <c r="E70" s="19"/>
+      <c r="E70" s="18"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="17" t="s">
+      <c r="E153" s="16" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2906,7 +2906,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="18"/>
+      <c r="E154" s="17"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2920,7 +2920,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="18"/>
+      <c r="E155" s="17"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="18"/>
+      <c r="E156" s="17"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2948,7 +2948,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="18"/>
+      <c r="E157" s="17"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -2962,7 +2962,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="18"/>
+      <c r="E158" s="17"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -2976,7 +2976,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="18"/>
+      <c r="E159" s="17"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -2990,7 +2990,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="18"/>
+      <c r="E160" s="17"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,7 +3004,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="18"/>
+      <c r="E161" s="17"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="18"/>
+      <c r="E162" s="17"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="18"/>
+      <c r="E163" s="17"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3046,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="18"/>
+      <c r="E164" s="17"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3060,7 +3060,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="18"/>
+      <c r="E165" s="17"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3074,7 +3074,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="18"/>
+      <c r="E166" s="17"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="18"/>
+      <c r="E167" s="17"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3102,7 +3102,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="18"/>
+      <c r="E168" s="17"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3116,7 +3116,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="18"/>
+      <c r="E169" s="17"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3130,7 +3130,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="18"/>
+      <c r="E170" s="17"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3144,7 +3144,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="18"/>
+      <c r="E171" s="17"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3158,7 +3158,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="18"/>
+      <c r="E172" s="17"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3172,7 +3172,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="18"/>
+      <c r="E173" s="17"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3186,7 +3186,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="18"/>
+      <c r="E174" s="17"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="18"/>
+      <c r="E175" s="17"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3214,7 +3214,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="18"/>
+      <c r="E176" s="17"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3228,7 +3228,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="18"/>
+      <c r="E177" s="17"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="18"/>
+      <c r="E178" s="17"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3256,7 +3256,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="19"/>
+      <c r="E179" s="18"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3264,6 +3264,12 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="16">
+    <mergeCell ref="E30:E39"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="E19:E26"/>
     <mergeCell ref="E153:E179"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="F40:F43"/>
@@ -3274,12 +3280,6 @@
     <mergeCell ref="E62:E70"/>
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
-    <mergeCell ref="E30:E39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E19:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
iniciando ej extra 2
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -304,6 +304,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -324,9 +327,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,8 +632,8 @@
   <dimension ref="A1:F179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -714,7 +714,7 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -752,7 +752,7 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="16" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -808,7 +808,7 @@
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -826,7 +826,7 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -844,7 +844,7 @@
       <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -882,7 +882,7 @@
       <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -902,7 +902,7 @@
       <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="23"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -956,7 +956,7 @@
       <c r="D17" s="6">
         <v>4</v>
       </c>
-      <c r="E17" s="23"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1014,7 +1014,7 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="23"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="23"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="23"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="23"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="D24" s="6">
         <v>5</v>
       </c>
-      <c r="E24" s="23"/>
+      <c r="E24" s="16"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="D25" s="6">
         <v>5</v>
       </c>
-      <c r="E25" s="23"/>
+      <c r="E25" s="16"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="23"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1220,7 +1220,7 @@
       <c r="D31" s="6">
         <v>7</v>
       </c>
-      <c r="E31" s="23"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="D32" s="6">
         <v>7</v>
       </c>
-      <c r="E32" s="23"/>
+      <c r="E32" s="16"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
-      <c r="E33" s="23"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="E34" s="23"/>
+      <c r="E34" s="16"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="D35" s="6">
         <v>7</v>
       </c>
-      <c r="E35" s="23"/>
+      <c r="E35" s="16"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="D36" s="6">
         <v>7</v>
       </c>
-      <c r="E36" s="23"/>
+      <c r="E36" s="16"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="D37" s="6">
         <v>7</v>
       </c>
-      <c r="E37" s="23"/>
+      <c r="E37" s="16"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="D38" s="6">
         <v>7</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="16"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="D39" s="6">
         <v>7</v>
       </c>
-      <c r="E39" s="23"/>
+      <c r="E39" s="16"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1382,10 +1382,10 @@
       <c r="D40" s="6">
         <v>8</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="22" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1402,8 +1402,8 @@
       <c r="D41" s="6">
         <v>8</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="21"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1418,8 +1418,8 @@
       <c r="D42" s="6">
         <v>8</v>
       </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="21"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1434,8 +1434,8 @@
       <c r="D43" s="6">
         <v>8</v>
       </c>
-      <c r="E43" s="23"/>
-      <c r="F43" s="21"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1450,7 +1450,7 @@
       <c r="D44" s="6">
         <v>8</v>
       </c>
-      <c r="E44" s="23"/>
+      <c r="E44" s="16"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="23"/>
+      <c r="E45" s="16"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1486,8 +1486,8 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="23"/>
-      <c r="F46" s="21" t="s">
+      <c r="E46" s="16"/>
+      <c r="F46" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1504,8 +1504,8 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-      <c r="E47" s="23"/>
-      <c r="F47" s="21"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1520,8 +1520,8 @@
       <c r="D48" s="6">
         <v>8</v>
       </c>
-      <c r="E48" s="23"/>
-      <c r="F48" s="21"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1536,8 +1536,8 @@
       <c r="D49" s="6">
         <v>8</v>
       </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="21"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1552,7 +1552,7 @@
       <c r="D50" s="6">
         <v>8</v>
       </c>
-      <c r="E50" s="23"/>
+      <c r="E50" s="16"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1570,8 +1570,8 @@
       <c r="D51" s="6">
         <v>8</v>
       </c>
-      <c r="E51" s="23"/>
-      <c r="F51" s="22" t="s">
+      <c r="E51" s="16"/>
+      <c r="F51" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1588,8 +1588,8 @@
       <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="23"/>
-      <c r="F52" s="22"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1604,8 +1604,8 @@
       <c r="D53" s="6">
         <v>8</v>
       </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="22"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="23"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1620,8 +1620,8 @@
       <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E54" s="23"/>
-      <c r="F54" s="22"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="23"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1636,8 +1636,8 @@
       <c r="D55" s="6">
         <v>8</v>
       </c>
-      <c r="E55" s="23"/>
-      <c r="F55" s="21" t="s">
+      <c r="E55" s="16"/>
+      <c r="F55" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1654,8 +1654,8 @@
       <c r="D56" s="6">
         <v>8</v>
       </c>
-      <c r="E56" s="23"/>
-      <c r="F56" s="21"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1670,8 +1670,8 @@
       <c r="D57" s="6">
         <v>8</v>
       </c>
-      <c r="E57" s="23"/>
-      <c r="F57" s="21" t="s">
+      <c r="E57" s="16"/>
+      <c r="F57" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1688,8 +1688,8 @@
       <c r="D58" s="6">
         <v>8</v>
       </c>
-      <c r="E58" s="23"/>
-      <c r="F58" s="21"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="22"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1704,7 +1704,7 @@
       <c r="D59" s="6">
         <v>8</v>
       </c>
-      <c r="E59" s="23"/>
+      <c r="E59" s="16"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1722,10 +1722,10 @@
       <c r="D60" s="6">
         <v>9</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E60" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="19" t="s">
+      <c r="F60" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1742,8 +1742,8 @@
       <c r="D61" s="6">
         <v>9</v>
       </c>
-      <c r="E61" s="18"/>
-      <c r="F61" s="20"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="21"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1758,7 +1758,7 @@
       <c r="D62" s="6">
         <v>10</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="17" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1776,7 +1776,7 @@
       <c r="D63" s="6">
         <v>10</v>
       </c>
-      <c r="E63" s="17"/>
+      <c r="E63" s="18"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
       <c r="D64" s="6">
         <v>10</v>
       </c>
-      <c r="E64" s="17"/>
+      <c r="E64" s="18"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
       <c r="D65" s="6">
         <v>10</v>
       </c>
-      <c r="E65" s="17"/>
+      <c r="E65" s="18"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
       <c r="D66" s="6">
         <v>10</v>
       </c>
-      <c r="E66" s="17"/>
+      <c r="E66" s="18"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
       <c r="D67" s="6">
         <v>10</v>
       </c>
-      <c r="E67" s="17"/>
+      <c r="E67" s="18"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
       <c r="D68" s="6">
         <v>10</v>
       </c>
-      <c r="E68" s="17"/>
+      <c r="E68" s="18"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,13 +1866,13 @@
       <c r="B69" s="5">
         <v>8</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C69" s="8">
         <v>45141</v>
       </c>
       <c r="D69" s="6">
         <v>10</v>
       </c>
-      <c r="E69" s="17"/>
+      <c r="E69" s="18"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1883,12 +1883,12 @@
         <v>9</v>
       </c>
       <c r="C70" s="9">
-        <v>45145</v>
+        <v>45146</v>
       </c>
       <c r="D70" s="6">
         <v>10</v>
       </c>
-      <c r="E70" s="18"/>
+      <c r="E70" s="19"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="9">
-        <v>45146</v>
+        <v>45147</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="14"/>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="9">
-        <v>45147</v>
+        <v>45148</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="14"/>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="9">
-        <v>45148</v>
+        <v>45152</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="14"/>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="9">
-        <v>45152</v>
+        <v>45153</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="14"/>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="9">
-        <v>45153</v>
+        <v>45154</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="14"/>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="9">
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="14"/>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="9">
-        <v>45155</v>
+        <v>45160</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="14"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="9">
-        <v>45160</v>
+        <v>45161</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="14"/>
@@ -1993,7 +1993,7 @@
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="9">
-        <v>45161</v>
+        <v>45162</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="14"/>
@@ -2005,7 +2005,7 @@
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="9">
-        <v>45162</v>
+        <v>45166</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="14"/>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="9">
-        <v>45166</v>
+        <v>45167</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="14"/>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="9">
-        <v>45167</v>
+        <v>45168</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="14"/>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="9">
-        <v>45168</v>
+        <v>45169</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="14"/>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="9">
-        <v>45169</v>
+        <v>45173</v>
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="14"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="9">
-        <v>45173</v>
+        <v>45174</v>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="14"/>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="9">
-        <v>45174</v>
+        <v>45175</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="14"/>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="9">
-        <v>45175</v>
+        <v>45176</v>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="14"/>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="9">
-        <v>45176</v>
+        <v>45180</v>
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="14"/>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="9">
-        <v>45180</v>
+        <v>45181</v>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="14"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="9">
-        <v>45181</v>
+        <v>45182</v>
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="14"/>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="9">
-        <v>45182</v>
+        <v>45183</v>
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="14"/>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="9">
-        <v>45183</v>
+        <v>45187</v>
       </c>
       <c r="D92" s="6"/>
       <c r="E92" s="14"/>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="9">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="D93" s="6"/>
       <c r="E93" s="14"/>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="9">
-        <v>45188</v>
+        <v>45189</v>
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="14"/>
@@ -2185,7 +2185,7 @@
       </c>
       <c r="B95" s="5"/>
       <c r="C95" s="9">
-        <v>45189</v>
+        <v>45190</v>
       </c>
       <c r="D95" s="6"/>
       <c r="E95" s="14"/>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B96" s="5"/>
       <c r="C96" s="9">
-        <v>45190</v>
+        <v>45194</v>
       </c>
       <c r="D96" s="6"/>
       <c r="E96" s="14"/>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B97" s="5"/>
       <c r="C97" s="9">
-        <v>45194</v>
+        <v>45195</v>
       </c>
       <c r="D97" s="6"/>
       <c r="E97" s="14"/>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B98" s="5"/>
       <c r="C98" s="9">
-        <v>45195</v>
+        <v>45196</v>
       </c>
       <c r="D98" s="6"/>
       <c r="E98" s="14"/>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B99" s="5"/>
       <c r="C99" s="9">
-        <v>45196</v>
+        <v>45197</v>
       </c>
       <c r="D99" s="6"/>
       <c r="E99" s="14"/>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B100" s="5"/>
       <c r="C100" s="9">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="14"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="B101" s="5"/>
       <c r="C101" s="9">
-        <v>45201</v>
+        <v>45202</v>
       </c>
       <c r="D101" s="6"/>
       <c r="E101" s="14"/>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B102" s="5"/>
       <c r="C102" s="9">
-        <v>45202</v>
+        <v>45203</v>
       </c>
       <c r="D102" s="6"/>
       <c r="E102" s="14"/>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="B103" s="5"/>
       <c r="C103" s="9">
-        <v>45203</v>
+        <v>45204</v>
       </c>
       <c r="D103" s="6"/>
       <c r="E103" s="14"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="B104" s="5"/>
       <c r="C104" s="9">
-        <v>45204</v>
+        <v>45208</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="14"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="B105" s="5"/>
       <c r="C105" s="9">
-        <v>45208</v>
+        <v>45209</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="14"/>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B106" s="5"/>
       <c r="C106" s="9">
-        <v>45209</v>
+        <v>45210</v>
       </c>
       <c r="D106" s="6"/>
       <c r="E106" s="14"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="B107" s="5"/>
       <c r="C107" s="9">
-        <v>45210</v>
+        <v>45211</v>
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="14"/>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B108" s="5"/>
       <c r="C108" s="9">
-        <v>45211</v>
+        <v>45216</v>
       </c>
       <c r="D108" s="6"/>
       <c r="E108" s="14"/>
@@ -2353,7 +2353,7 @@
       </c>
       <c r="B109" s="5"/>
       <c r="C109" s="9">
-        <v>45216</v>
+        <v>45217</v>
       </c>
       <c r="D109" s="6"/>
       <c r="E109" s="14"/>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B110" s="5"/>
       <c r="C110" s="9">
-        <v>45217</v>
+        <v>45218</v>
       </c>
       <c r="D110" s="6"/>
       <c r="E110" s="14"/>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="B111" s="5"/>
       <c r="C111" s="9">
-        <v>45218</v>
+        <v>45222</v>
       </c>
       <c r="D111" s="6"/>
       <c r="E111" s="14"/>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="B112" s="5"/>
       <c r="C112" s="9">
-        <v>45222</v>
+        <v>45223</v>
       </c>
       <c r="D112" s="6"/>
       <c r="E112" s="14"/>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="9">
-        <v>45223</v>
+        <v>45224</v>
       </c>
       <c r="D113" s="6"/>
       <c r="E113" s="14"/>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B114" s="5"/>
       <c r="C114" s="9">
-        <v>45224</v>
+        <v>45225</v>
       </c>
       <c r="D114" s="6"/>
       <c r="E114" s="14"/>
@@ -2425,7 +2425,7 @@
       </c>
       <c r="B115" s="5"/>
       <c r="C115" s="9">
-        <v>45225</v>
+        <v>45229</v>
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="14"/>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="B116" s="5"/>
       <c r="C116" s="9">
-        <v>45229</v>
+        <v>45230</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="14"/>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="B117" s="5"/>
       <c r="C117" s="9">
-        <v>45230</v>
+        <v>45231</v>
       </c>
       <c r="D117" s="6"/>
       <c r="E117" s="14"/>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="B118" s="5"/>
       <c r="C118" s="9">
-        <v>45231</v>
+        <v>45232</v>
       </c>
       <c r="D118" s="6"/>
       <c r="E118" s="14"/>
@@ -2473,7 +2473,7 @@
       </c>
       <c r="B119" s="5"/>
       <c r="C119" s="9">
-        <v>45232</v>
+        <v>45236</v>
       </c>
       <c r="D119" s="6"/>
       <c r="E119" s="14"/>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="B120" s="5"/>
       <c r="C120" s="9">
-        <v>45236</v>
+        <v>45237</v>
       </c>
       <c r="D120" s="6"/>
       <c r="E120" s="14"/>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="B121" s="5"/>
       <c r="C121" s="9">
-        <v>45237</v>
+        <v>45238</v>
       </c>
       <c r="D121" s="6"/>
       <c r="E121" s="14"/>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="B122" s="5"/>
       <c r="C122" s="9">
-        <v>45238</v>
+        <v>45239</v>
       </c>
       <c r="D122" s="6"/>
       <c r="E122" s="14"/>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B123" s="5"/>
       <c r="C123" s="9">
-        <v>45239</v>
+        <v>45243</v>
       </c>
       <c r="D123" s="6"/>
       <c r="E123" s="14"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="B124" s="5"/>
       <c r="C124" s="9">
-        <v>45243</v>
+        <v>45244</v>
       </c>
       <c r="D124" s="6"/>
       <c r="E124" s="14"/>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B125" s="5"/>
       <c r="C125" s="9">
-        <v>45244</v>
+        <v>45245</v>
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="14"/>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B126" s="5"/>
       <c r="C126" s="9">
-        <v>45245</v>
+        <v>45246</v>
       </c>
       <c r="D126" s="6"/>
       <c r="E126" s="14"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="B127" s="5"/>
       <c r="C127" s="9">
-        <v>45246</v>
+        <v>45251</v>
       </c>
       <c r="D127" s="6"/>
       <c r="E127" s="14"/>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="B128" s="5"/>
       <c r="C128" s="9">
-        <v>45251</v>
+        <v>45252</v>
       </c>
       <c r="D128" s="6"/>
       <c r="E128" s="14"/>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="B129" s="5"/>
       <c r="C129" s="9">
-        <v>45252</v>
+        <v>45253</v>
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="14"/>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="B130" s="5"/>
       <c r="C130" s="9">
-        <v>45253</v>
+        <v>45257</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="14"/>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B131" s="5"/>
       <c r="C131" s="9">
-        <v>45257</v>
+        <v>45258</v>
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="14"/>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B132" s="5"/>
       <c r="C132" s="9">
-        <v>45258</v>
+        <v>45259</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="14"/>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="B133" s="5"/>
       <c r="C133" s="9">
-        <v>45259</v>
+        <v>45260</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="14"/>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="B134" s="5"/>
       <c r="C134" s="9">
-        <v>45260</v>
+        <v>45264</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="14"/>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B135" s="5"/>
       <c r="C135" s="9">
-        <v>45264</v>
+        <v>45265</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="14"/>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B136" s="5"/>
       <c r="C136" s="9">
-        <v>45265</v>
+        <v>45266</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="14"/>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="B137" s="5"/>
       <c r="C137" s="9">
-        <v>45266</v>
+        <v>45267</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="14"/>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="B138" s="5"/>
       <c r="C138" s="9">
-        <v>45267</v>
+        <v>45271</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="14"/>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B139" s="5"/>
       <c r="C139" s="9">
-        <v>45271</v>
+        <v>45272</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="14"/>
@@ -2725,7 +2725,7 @@
       </c>
       <c r="B140" s="5"/>
       <c r="C140" s="9">
-        <v>45272</v>
+        <v>45273</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="14"/>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="B141" s="5"/>
       <c r="C141" s="9">
-        <v>45273</v>
+        <v>45274</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="14"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="B142" s="5"/>
       <c r="C142" s="9">
-        <v>45274</v>
+        <v>45278</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="14"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B143" s="5"/>
       <c r="C143" s="9">
-        <v>45278</v>
+        <v>45279</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="14"/>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="B144" s="5"/>
       <c r="C144" s="9">
-        <v>45279</v>
+        <v>45280</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="14"/>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="B145" s="5"/>
       <c r="C145" s="9">
-        <v>45280</v>
+        <v>45281</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="14" t="s">
@@ -2798,9 +2798,6 @@
         <v>145</v>
       </c>
       <c r="B146" s="5"/>
-      <c r="C146" s="9">
-        <v>45281</v>
-      </c>
       <c r="D146" s="6"/>
       <c r="E146" s="14" t="s">
         <v>29</v>
@@ -2890,7 +2887,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="16" t="s">
+      <c r="E153" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2906,7 +2903,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="17"/>
+      <c r="E154" s="18"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2920,7 +2917,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="17"/>
+      <c r="E155" s="18"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2934,7 +2931,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="17"/>
+      <c r="E156" s="18"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2948,7 +2945,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="17"/>
+      <c r="E157" s="18"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -2962,7 +2959,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="17"/>
+      <c r="E158" s="18"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -2976,7 +2973,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="17"/>
+      <c r="E159" s="18"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -2990,7 +2987,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="17"/>
+      <c r="E160" s="18"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,7 +3001,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="17"/>
+      <c r="E161" s="18"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3018,7 +3015,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="17"/>
+      <c r="E162" s="18"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3032,7 +3029,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="17"/>
+      <c r="E163" s="18"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3043,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="17"/>
+      <c r="E164" s="18"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3060,7 +3057,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="17"/>
+      <c r="E165" s="18"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3074,7 +3071,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="17"/>
+      <c r="E166" s="18"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3088,7 +3085,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="17"/>
+      <c r="E167" s="18"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3102,7 +3099,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="17"/>
+      <c r="E168" s="18"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3116,7 +3113,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="17"/>
+      <c r="E169" s="18"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3130,7 +3127,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="17"/>
+      <c r="E170" s="18"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3144,7 +3141,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="17"/>
+      <c r="E171" s="18"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3158,7 +3155,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="17"/>
+      <c r="E172" s="18"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3172,7 +3169,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="17"/>
+      <c r="E173" s="18"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3186,7 +3183,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="17"/>
+      <c r="E174" s="18"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3200,7 +3197,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="17"/>
+      <c r="E175" s="18"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3214,7 +3211,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="17"/>
+      <c r="E176" s="18"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3228,7 +3225,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="17"/>
+      <c r="E177" s="18"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3242,7 +3239,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="17"/>
+      <c r="E178" s="18"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3256,7 +3253,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="18"/>
+      <c r="E179" s="19"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3264,12 +3261,6 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="E30:E39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E19:E26"/>
     <mergeCell ref="E153:E179"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="F40:F43"/>
@@ -3280,6 +3271,12 @@
     <mergeCell ref="E62:E70"/>
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
+    <mergeCell ref="E30:E39"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="E19:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
salteo el 3, empiezo el 4
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -632,8 +632,8 @@
   <dimension ref="A1:F179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,25 +1882,29 @@
       <c r="B70" s="5">
         <v>9</v>
       </c>
-      <c r="C70" s="9">
+      <c r="C70" s="8">
         <v>45146</v>
       </c>
       <c r="D70" s="6">
         <v>10</v>
       </c>
-      <c r="E70" s="19"/>
+      <c r="E70" s="18"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>70</v>
       </c>
-      <c r="B71" s="5"/>
+      <c r="B71" s="5">
+        <v>10</v>
+      </c>
       <c r="C71" s="9">
         <v>45147</v>
       </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="14"/>
+      <c r="D71" s="6">
+        <v>10</v>
+      </c>
+      <c r="E71" s="19"/>
       <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3268,9 +3272,9 @@
     <mergeCell ref="F51:F54"/>
     <mergeCell ref="F55:F56"/>
     <mergeCell ref="F57:F58"/>
-    <mergeCell ref="E62:E70"/>
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
+    <mergeCell ref="E62:E71"/>
     <mergeCell ref="E30:E39"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E5:E7"/>

</xml_diff>

<commit_message>
iniciando ejercicio 3 de naipes
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -313,9 +313,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -336,6 +333,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,7 +642,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
+      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +705,7 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="24" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -723,7 +723,7 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="24" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -761,7 +761,7 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -797,7 +797,7 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -817,7 +817,7 @@
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -835,7 +835,7 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="17"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -853,7 +853,7 @@
       <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -891,7 +891,7 @@
       <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="24" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -911,7 +911,7 @@
       <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -929,7 +929,7 @@
       <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -947,7 +947,7 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="D17" s="6">
         <v>4</v>
       </c>
-      <c r="E17" s="17"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1023,7 +1023,7 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="17"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1041,7 +1041,7 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1077,7 +1077,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1095,7 +1095,7 @@
       <c r="D24" s="6">
         <v>5</v>
       </c>
-      <c r="E24" s="17"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="D25" s="6">
         <v>5</v>
       </c>
-      <c r="E25" s="17"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="17"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1209,7 +1209,7 @@
       <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="24" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1229,7 +1229,7 @@
       <c r="D31" s="6">
         <v>7</v>
       </c>
-      <c r="E31" s="17"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1247,7 +1247,7 @@
       <c r="D32" s="6">
         <v>7</v>
       </c>
-      <c r="E32" s="17"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
-      <c r="E33" s="17"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="D35" s="6">
         <v>7</v>
       </c>
-      <c r="E35" s="17"/>
+      <c r="E35" s="24"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="D36" s="6">
         <v>7</v>
       </c>
-      <c r="E36" s="17"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1337,7 +1337,7 @@
       <c r="D37" s="6">
         <v>7</v>
       </c>
-      <c r="E37" s="17"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="D38" s="6">
         <v>7</v>
       </c>
-      <c r="E38" s="17"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="D39" s="6">
         <v>7</v>
       </c>
-      <c r="E39" s="17"/>
+      <c r="E39" s="24"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1391,10 +1391,10 @@
       <c r="D40" s="6">
         <v>8</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="22" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1411,8 +1411,8 @@
       <c r="D41" s="6">
         <v>8</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="23"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1427,8 +1427,8 @@
       <c r="D42" s="6">
         <v>8</v>
       </c>
-      <c r="E42" s="17"/>
-      <c r="F42" s="23"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1443,8 +1443,8 @@
       <c r="D43" s="6">
         <v>8</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="23"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1459,7 +1459,7 @@
       <c r="D44" s="6">
         <v>8</v>
       </c>
-      <c r="E44" s="17"/>
+      <c r="E44" s="24"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="17"/>
+      <c r="E45" s="24"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1495,8 +1495,8 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="23" t="s">
+      <c r="E46" s="24"/>
+      <c r="F46" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1513,8 +1513,8 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="23"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1529,8 +1529,8 @@
       <c r="D48" s="6">
         <v>8</v>
       </c>
-      <c r="E48" s="17"/>
-      <c r="F48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1545,8 +1545,8 @@
       <c r="D49" s="6">
         <v>8</v>
       </c>
-      <c r="E49" s="17"/>
-      <c r="F49" s="23"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1561,7 +1561,7 @@
       <c r="D50" s="6">
         <v>8</v>
       </c>
-      <c r="E50" s="17"/>
+      <c r="E50" s="24"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1579,8 +1579,8 @@
       <c r="D51" s="6">
         <v>8</v>
       </c>
-      <c r="E51" s="17"/>
-      <c r="F51" s="24" t="s">
+      <c r="E51" s="24"/>
+      <c r="F51" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1597,8 +1597,8 @@
       <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="17"/>
-      <c r="F52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1613,8 +1613,8 @@
       <c r="D53" s="6">
         <v>8</v>
       </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="23"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1629,8 +1629,8 @@
       <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E54" s="17"/>
-      <c r="F54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="23"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1645,8 +1645,8 @@
       <c r="D55" s="6">
         <v>8</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="23" t="s">
+      <c r="E55" s="24"/>
+      <c r="F55" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1663,8 +1663,8 @@
       <c r="D56" s="6">
         <v>8</v>
       </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="23"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1679,8 +1679,8 @@
       <c r="D57" s="6">
         <v>8</v>
       </c>
-      <c r="E57" s="17"/>
-      <c r="F57" s="23" t="s">
+      <c r="E57" s="24"/>
+      <c r="F57" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1697,8 +1697,8 @@
       <c r="D58" s="6">
         <v>8</v>
       </c>
-      <c r="E58" s="17"/>
-      <c r="F58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="22"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1713,7 +1713,7 @@
       <c r="D59" s="6">
         <v>8</v>
       </c>
-      <c r="E59" s="17"/>
+      <c r="E59" s="24"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1731,10 +1731,10 @@
       <c r="D60" s="6">
         <v>9</v>
       </c>
-      <c r="E60" s="18" t="s">
+      <c r="E60" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="21" t="s">
+      <c r="F60" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1751,8 +1751,8 @@
       <c r="D61" s="6">
         <v>9</v>
       </c>
-      <c r="E61" s="20"/>
-      <c r="F61" s="22"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="21"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1767,7 +1767,7 @@
       <c r="D62" s="6">
         <v>10</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E62" s="17" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1785,7 +1785,7 @@
       <c r="D63" s="6">
         <v>10</v>
       </c>
-      <c r="E63" s="19"/>
+      <c r="E63" s="18"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
       <c r="D64" s="6">
         <v>10</v>
       </c>
-      <c r="E64" s="19"/>
+      <c r="E64" s="18"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
       <c r="D65" s="6">
         <v>10</v>
       </c>
-      <c r="E65" s="19"/>
+      <c r="E65" s="18"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
       <c r="D66" s="6">
         <v>10</v>
       </c>
-      <c r="E66" s="19"/>
+      <c r="E66" s="18"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
       <c r="D67" s="6">
         <v>10</v>
       </c>
-      <c r="E67" s="19"/>
+      <c r="E67" s="18"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,7 +1865,7 @@
       <c r="D68" s="6">
         <v>10</v>
       </c>
-      <c r="E68" s="19"/>
+      <c r="E68" s="18"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1881,7 +1881,7 @@
       <c r="D69" s="6">
         <v>10</v>
       </c>
-      <c r="E69" s="19"/>
+      <c r="E69" s="18"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
       <c r="D70" s="6">
         <v>10</v>
       </c>
-      <c r="E70" s="19"/>
+      <c r="E70" s="18"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
       <c r="D71" s="6">
         <v>11</v>
       </c>
-      <c r="E71" s="18" t="s">
+      <c r="E71" s="17" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1931,7 +1931,7 @@
       <c r="D72" s="6">
         <v>11</v>
       </c>
-      <c r="E72" s="19"/>
+      <c r="E72" s="18"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
       <c r="D73" s="6">
         <v>11</v>
       </c>
-      <c r="E73" s="19"/>
+      <c r="E73" s="18"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
       <c r="D74" s="6">
         <v>11</v>
       </c>
-      <c r="E74" s="19"/>
+      <c r="E74" s="18"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -1975,13 +1975,13 @@
       <c r="B75" s="16">
         <v>5</v>
       </c>
-      <c r="C75" s="9">
+      <c r="C75" s="8">
         <v>45154</v>
       </c>
       <c r="D75" s="6">
         <v>11</v>
       </c>
-      <c r="E75" s="19"/>
+      <c r="E75" s="18"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1997,7 +1997,7 @@
       <c r="D76" s="6">
         <v>11</v>
       </c>
-      <c r="E76" s="19"/>
+      <c r="E76" s="18"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2013,7 +2013,7 @@
       <c r="D77" s="6">
         <v>11</v>
       </c>
-      <c r="E77" s="19"/>
+      <c r="E77" s="18"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2029,7 +2029,7 @@
       <c r="D78" s="6">
         <v>11</v>
       </c>
-      <c r="E78" s="19"/>
+      <c r="E78" s="18"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
       <c r="D79" s="6">
         <v>11</v>
       </c>
-      <c r="E79" s="19"/>
+      <c r="E79" s="18"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2936,7 +2936,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="18" t="s">
+      <c r="E153" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2952,7 +2952,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="19"/>
+      <c r="E154" s="18"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2966,7 +2966,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="19"/>
+      <c r="E155" s="18"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="19"/>
+      <c r="E156" s="18"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="19"/>
+      <c r="E157" s="18"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="19"/>
+      <c r="E158" s="18"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="19"/>
+      <c r="E159" s="18"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3036,7 +3036,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="19"/>
+      <c r="E160" s="18"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="19"/>
+      <c r="E161" s="18"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="19"/>
+      <c r="E162" s="18"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="19"/>
+      <c r="E163" s="18"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="19"/>
+      <c r="E164" s="18"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3106,7 +3106,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="19"/>
+      <c r="E165" s="18"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="19"/>
+      <c r="E166" s="18"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="19"/>
+      <c r="E167" s="18"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="19"/>
+      <c r="E168" s="18"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="19"/>
+      <c r="E169" s="18"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="19"/>
+      <c r="E170" s="18"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3190,7 +3190,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="19"/>
+      <c r="E171" s="18"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="19"/>
+      <c r="E172" s="18"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="19"/>
+      <c r="E173" s="18"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="19"/>
+      <c r="E174" s="18"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="19"/>
+      <c r="E175" s="18"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="19"/>
+      <c r="E176" s="18"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="19"/>
+      <c r="E177" s="18"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3288,7 +3288,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="19"/>
+      <c r="E178" s="18"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="20"/>
+      <c r="E179" s="19"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3310,6 +3310,12 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="17">
+    <mergeCell ref="E30:E39"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="E19:E26"/>
     <mergeCell ref="E153:E179"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="F40:F43"/>
@@ -3321,12 +3327,6 @@
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="E62:E70"/>
     <mergeCell ref="E71:E79"/>
-    <mergeCell ref="E30:E39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E19:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ejercicio 3 cartas, complicadisimo
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -313,6 +313,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -333,9 +336,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,7 +642,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +705,7 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -723,7 +723,7 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -761,7 +761,7 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -797,7 +797,7 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -817,7 +817,7 @@
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="24"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -835,7 +835,7 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -853,7 +853,7 @@
       <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -891,7 +891,7 @@
       <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="17" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -911,7 +911,7 @@
       <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -929,7 +929,7 @@
       <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="24"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -947,7 +947,7 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="24"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="D17" s="6">
         <v>4</v>
       </c>
-      <c r="E17" s="24"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="17" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1023,7 +1023,7 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1041,7 +1041,7 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="24"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1077,7 +1077,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="24"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1095,7 +1095,7 @@
       <c r="D24" s="6">
         <v>5</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="D25" s="6">
         <v>5</v>
       </c>
-      <c r="E25" s="24"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1209,7 +1209,7 @@
       <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="17" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1229,7 +1229,7 @@
       <c r="D31" s="6">
         <v>7</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1247,7 +1247,7 @@
       <c r="D32" s="6">
         <v>7</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
-      <c r="E33" s="24"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="E34" s="24"/>
+      <c r="E34" s="17"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="D35" s="6">
         <v>7</v>
       </c>
-      <c r="E35" s="24"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="D36" s="6">
         <v>7</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1337,7 +1337,7 @@
       <c r="D37" s="6">
         <v>7</v>
       </c>
-      <c r="E37" s="24"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="D38" s="6">
         <v>7</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="17"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="D39" s="6">
         <v>7</v>
       </c>
-      <c r="E39" s="24"/>
+      <c r="E39" s="17"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1391,10 +1391,10 @@
       <c r="D40" s="6">
         <v>8</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="23" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1411,8 +1411,8 @@
       <c r="D41" s="6">
         <v>8</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="22"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="23"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1427,8 +1427,8 @@
       <c r="D42" s="6">
         <v>8</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="22"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1443,8 +1443,8 @@
       <c r="D43" s="6">
         <v>8</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="22"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="23"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1459,7 +1459,7 @@
       <c r="D44" s="6">
         <v>8</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="17"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="24"/>
+      <c r="E45" s="17"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1495,8 +1495,8 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="22" t="s">
+      <c r="E46" s="17"/>
+      <c r="F46" s="23" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1513,8 +1513,8 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-      <c r="E47" s="24"/>
-      <c r="F47" s="22"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="23"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1529,8 +1529,8 @@
       <c r="D48" s="6">
         <v>8</v>
       </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="22"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="23"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1545,8 +1545,8 @@
       <c r="D49" s="6">
         <v>8</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="22"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="23"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1561,7 +1561,7 @@
       <c r="D50" s="6">
         <v>8</v>
       </c>
-      <c r="E50" s="24"/>
+      <c r="E50" s="17"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1579,8 +1579,8 @@
       <c r="D51" s="6">
         <v>8</v>
       </c>
-      <c r="E51" s="24"/>
-      <c r="F51" s="23" t="s">
+      <c r="E51" s="17"/>
+      <c r="F51" s="24" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1597,8 +1597,8 @@
       <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="23"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="24"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1613,8 +1613,8 @@
       <c r="D53" s="6">
         <v>8</v>
       </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="23"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="24"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1629,8 +1629,8 @@
       <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="23"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="24"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1645,8 +1645,8 @@
       <c r="D55" s="6">
         <v>8</v>
       </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="22" t="s">
+      <c r="E55" s="17"/>
+      <c r="F55" s="23" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1663,8 +1663,8 @@
       <c r="D56" s="6">
         <v>8</v>
       </c>
-      <c r="E56" s="24"/>
-      <c r="F56" s="22"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="23"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1679,8 +1679,8 @@
       <c r="D57" s="6">
         <v>8</v>
       </c>
-      <c r="E57" s="24"/>
-      <c r="F57" s="22" t="s">
+      <c r="E57" s="17"/>
+      <c r="F57" s="23" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1697,8 +1697,8 @@
       <c r="D58" s="6">
         <v>8</v>
       </c>
-      <c r="E58" s="24"/>
-      <c r="F58" s="22"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="23"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1713,7 +1713,7 @@
       <c r="D59" s="6">
         <v>8</v>
       </c>
-      <c r="E59" s="24"/>
+      <c r="E59" s="17"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1731,10 +1731,10 @@
       <c r="D60" s="6">
         <v>9</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1751,8 +1751,8 @@
       <c r="D61" s="6">
         <v>9</v>
       </c>
-      <c r="E61" s="19"/>
-      <c r="F61" s="21"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="22"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1767,7 +1767,7 @@
       <c r="D62" s="6">
         <v>10</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E62" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1785,7 +1785,7 @@
       <c r="D63" s="6">
         <v>10</v>
       </c>
-      <c r="E63" s="18"/>
+      <c r="E63" s="19"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
       <c r="D64" s="6">
         <v>10</v>
       </c>
-      <c r="E64" s="18"/>
+      <c r="E64" s="19"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
       <c r="D65" s="6">
         <v>10</v>
       </c>
-      <c r="E65" s="18"/>
+      <c r="E65" s="19"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
       <c r="D66" s="6">
         <v>10</v>
       </c>
-      <c r="E66" s="18"/>
+      <c r="E66" s="19"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
       <c r="D67" s="6">
         <v>10</v>
       </c>
-      <c r="E67" s="18"/>
+      <c r="E67" s="19"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,7 +1865,7 @@
       <c r="D68" s="6">
         <v>10</v>
       </c>
-      <c r="E68" s="18"/>
+      <c r="E68" s="19"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1881,7 +1881,7 @@
       <c r="D69" s="6">
         <v>10</v>
       </c>
-      <c r="E69" s="18"/>
+      <c r="E69" s="19"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
       <c r="D70" s="6">
         <v>10</v>
       </c>
-      <c r="E70" s="18"/>
+      <c r="E70" s="19"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
       <c r="D71" s="6">
         <v>11</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="E71" s="18" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1931,7 +1931,7 @@
       <c r="D72" s="6">
         <v>11</v>
       </c>
-      <c r="E72" s="18"/>
+      <c r="E72" s="19"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
       <c r="D73" s="6">
         <v>11</v>
       </c>
-      <c r="E73" s="18"/>
+      <c r="E73" s="19"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
       <c r="D74" s="6">
         <v>11</v>
       </c>
-      <c r="E74" s="18"/>
+      <c r="E74" s="19"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -1981,7 +1981,7 @@
       <c r="D75" s="6">
         <v>11</v>
       </c>
-      <c r="E75" s="18"/>
+      <c r="E75" s="19"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1991,13 +1991,13 @@
       <c r="B76" s="16">
         <v>6</v>
       </c>
-      <c r="C76" s="9">
+      <c r="C76" s="8">
         <v>45155</v>
       </c>
       <c r="D76" s="6">
         <v>11</v>
       </c>
-      <c r="E76" s="18"/>
+      <c r="E76" s="19"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2013,7 +2013,7 @@
       <c r="D77" s="6">
         <v>11</v>
       </c>
-      <c r="E77" s="18"/>
+      <c r="E77" s="19"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2029,7 +2029,7 @@
       <c r="D78" s="6">
         <v>11</v>
       </c>
-      <c r="E78" s="18"/>
+      <c r="E78" s="19"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
       <c r="D79" s="6">
         <v>11</v>
       </c>
-      <c r="E79" s="18"/>
+      <c r="E79" s="19"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2936,7 +2936,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="17" t="s">
+      <c r="E153" s="18" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2952,7 +2952,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="18"/>
+      <c r="E154" s="19"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2966,7 +2966,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="18"/>
+      <c r="E155" s="19"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="18"/>
+      <c r="E156" s="19"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="18"/>
+      <c r="E157" s="19"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="18"/>
+      <c r="E158" s="19"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="18"/>
+      <c r="E159" s="19"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3036,7 +3036,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="18"/>
+      <c r="E160" s="19"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="18"/>
+      <c r="E161" s="19"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="18"/>
+      <c r="E162" s="19"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="18"/>
+      <c r="E163" s="19"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="18"/>
+      <c r="E164" s="19"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3106,7 +3106,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="18"/>
+      <c r="E165" s="19"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="18"/>
+      <c r="E166" s="19"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="18"/>
+      <c r="E167" s="19"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="18"/>
+      <c r="E168" s="19"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="18"/>
+      <c r="E169" s="19"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="18"/>
+      <c r="E170" s="19"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3190,7 +3190,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="18"/>
+      <c r="E171" s="19"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="18"/>
+      <c r="E172" s="19"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="18"/>
+      <c r="E173" s="19"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="18"/>
+      <c r="E174" s="19"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="18"/>
+      <c r="E175" s="19"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="18"/>
+      <c r="E176" s="19"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="18"/>
+      <c r="E177" s="19"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3288,7 +3288,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="18"/>
+      <c r="E178" s="19"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="19"/>
+      <c r="E179" s="20"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3310,12 +3310,6 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="E30:E39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E19:E26"/>
     <mergeCell ref="E153:E179"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="F40:F43"/>
@@ -3327,6 +3321,12 @@
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="E62:E70"/>
     <mergeCell ref="E71:E79"/>
+    <mergeCell ref="E30:E39"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="E19:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ej1 extra con chatgpt
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -313,6 +313,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -333,9 +336,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,7 +642,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
+      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +705,7 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -723,7 +723,7 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -761,7 +761,7 @@
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -797,7 +797,7 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -817,7 +817,7 @@
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="24"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -835,7 +835,7 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -853,7 +853,7 @@
       <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -891,7 +891,7 @@
       <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="17" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -911,7 +911,7 @@
       <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -929,7 +929,7 @@
       <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="24"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -947,7 +947,7 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="24"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="D17" s="6">
         <v>4</v>
       </c>
-      <c r="E17" s="24"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="17" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1023,7 +1023,7 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1041,7 +1041,7 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="24"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1077,7 +1077,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="24"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1095,7 +1095,7 @@
       <c r="D24" s="6">
         <v>5</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="D25" s="6">
         <v>5</v>
       </c>
-      <c r="E25" s="24"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="D26" s="6">
         <v>5</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1209,7 +1209,7 @@
       <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="17" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1229,7 +1229,7 @@
       <c r="D31" s="6">
         <v>7</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1247,7 +1247,7 @@
       <c r="D32" s="6">
         <v>7</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="D33" s="6">
         <v>7</v>
       </c>
-      <c r="E33" s="24"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="E34" s="24"/>
+      <c r="E34" s="17"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="D35" s="6">
         <v>7</v>
       </c>
-      <c r="E35" s="24"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="D36" s="6">
         <v>7</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1337,7 +1337,7 @@
       <c r="D37" s="6">
         <v>7</v>
       </c>
-      <c r="E37" s="24"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="D38" s="6">
         <v>7</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="17"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="D39" s="6">
         <v>7</v>
       </c>
-      <c r="E39" s="24"/>
+      <c r="E39" s="17"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1391,10 +1391,10 @@
       <c r="D40" s="6">
         <v>8</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="23" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1411,8 +1411,8 @@
       <c r="D41" s="6">
         <v>8</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="22"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="23"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1427,8 +1427,8 @@
       <c r="D42" s="6">
         <v>8</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="22"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1443,8 +1443,8 @@
       <c r="D43" s="6">
         <v>8</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="22"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="23"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1459,7 +1459,7 @@
       <c r="D44" s="6">
         <v>8</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="17"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="24"/>
+      <c r="E45" s="17"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1495,8 +1495,8 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="22" t="s">
+      <c r="E46" s="17"/>
+      <c r="F46" s="23" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1513,8 +1513,8 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-      <c r="E47" s="24"/>
-      <c r="F47" s="22"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="23"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1529,8 +1529,8 @@
       <c r="D48" s="6">
         <v>8</v>
       </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="22"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="23"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1545,8 +1545,8 @@
       <c r="D49" s="6">
         <v>8</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="22"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="23"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1561,7 +1561,7 @@
       <c r="D50" s="6">
         <v>8</v>
       </c>
-      <c r="E50" s="24"/>
+      <c r="E50" s="17"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1579,8 +1579,8 @@
       <c r="D51" s="6">
         <v>8</v>
       </c>
-      <c r="E51" s="24"/>
-      <c r="F51" s="23" t="s">
+      <c r="E51" s="17"/>
+      <c r="F51" s="24" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1597,8 +1597,8 @@
       <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="23"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="24"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1613,8 +1613,8 @@
       <c r="D53" s="6">
         <v>8</v>
       </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="23"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="24"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1629,8 +1629,8 @@
       <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="23"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="24"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1645,8 +1645,8 @@
       <c r="D55" s="6">
         <v>8</v>
       </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="22" t="s">
+      <c r="E55" s="17"/>
+      <c r="F55" s="23" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1663,8 +1663,8 @@
       <c r="D56" s="6">
         <v>8</v>
       </c>
-      <c r="E56" s="24"/>
-      <c r="F56" s="22"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="23"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1679,8 +1679,8 @@
       <c r="D57" s="6">
         <v>8</v>
       </c>
-      <c r="E57" s="24"/>
-      <c r="F57" s="22" t="s">
+      <c r="E57" s="17"/>
+      <c r="F57" s="23" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1697,8 +1697,8 @@
       <c r="D58" s="6">
         <v>8</v>
       </c>
-      <c r="E58" s="24"/>
-      <c r="F58" s="22"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="23"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1713,7 +1713,7 @@
       <c r="D59" s="6">
         <v>8</v>
       </c>
-      <c r="E59" s="24"/>
+      <c r="E59" s="17"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1731,10 +1731,10 @@
       <c r="D60" s="6">
         <v>9</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1751,8 +1751,8 @@
       <c r="D61" s="6">
         <v>9</v>
       </c>
-      <c r="E61" s="19"/>
-      <c r="F61" s="21"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="22"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1767,7 +1767,7 @@
       <c r="D62" s="6">
         <v>10</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E62" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1785,7 +1785,7 @@
       <c r="D63" s="6">
         <v>10</v>
       </c>
-      <c r="E63" s="18"/>
+      <c r="E63" s="19"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
       <c r="D64" s="6">
         <v>10</v>
       </c>
-      <c r="E64" s="18"/>
+      <c r="E64" s="19"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
       <c r="D65" s="6">
         <v>10</v>
       </c>
-      <c r="E65" s="18"/>
+      <c r="E65" s="19"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
       <c r="D66" s="6">
         <v>10</v>
       </c>
-      <c r="E66" s="18"/>
+      <c r="E66" s="19"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
       <c r="D67" s="6">
         <v>10</v>
       </c>
-      <c r="E67" s="18"/>
+      <c r="E67" s="19"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,7 +1865,7 @@
       <c r="D68" s="6">
         <v>10</v>
       </c>
-      <c r="E68" s="18"/>
+      <c r="E68" s="19"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1881,7 +1881,7 @@
       <c r="D69" s="6">
         <v>10</v>
       </c>
-      <c r="E69" s="18"/>
+      <c r="E69" s="19"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
       <c r="D70" s="6">
         <v>10</v>
       </c>
-      <c r="E70" s="18"/>
+      <c r="E70" s="19"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
       <c r="D71" s="6">
         <v>11</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="E71" s="18" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1931,7 +1931,7 @@
       <c r="D72" s="6">
         <v>11</v>
       </c>
-      <c r="E72" s="18"/>
+      <c r="E72" s="19"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
       <c r="D73" s="6">
         <v>11</v>
       </c>
-      <c r="E73" s="18"/>
+      <c r="E73" s="19"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
       <c r="D74" s="6">
         <v>11</v>
       </c>
-      <c r="E74" s="18"/>
+      <c r="E74" s="19"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -1981,7 +1981,7 @@
       <c r="D75" s="6">
         <v>11</v>
       </c>
-      <c r="E75" s="18"/>
+      <c r="E75" s="19"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1997,7 +1997,7 @@
       <c r="D76" s="6">
         <v>11</v>
       </c>
-      <c r="E76" s="18"/>
+      <c r="E76" s="19"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2013,7 +2013,7 @@
       <c r="D77" s="6">
         <v>11</v>
       </c>
-      <c r="E77" s="18"/>
+      <c r="E77" s="19"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2023,13 +2023,13 @@
       <c r="B78" s="16">
         <v>8</v>
       </c>
-      <c r="C78" s="9">
+      <c r="C78" s="8">
         <v>45161</v>
       </c>
       <c r="D78" s="6">
         <v>11</v>
       </c>
-      <c r="E78" s="18"/>
+      <c r="E78" s="19"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
       <c r="D79" s="6">
         <v>11</v>
       </c>
-      <c r="E79" s="18"/>
+      <c r="E79" s="19"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2936,7 +2936,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="17" t="s">
+      <c r="E153" s="18" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2952,7 +2952,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="18"/>
+      <c r="E154" s="19"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2966,7 +2966,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="18"/>
+      <c r="E155" s="19"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="18"/>
+      <c r="E156" s="19"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="18"/>
+      <c r="E157" s="19"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="18"/>
+      <c r="E158" s="19"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="18"/>
+      <c r="E159" s="19"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3036,7 +3036,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="18"/>
+      <c r="E160" s="19"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="18"/>
+      <c r="E161" s="19"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="18"/>
+      <c r="E162" s="19"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="18"/>
+      <c r="E163" s="19"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="18"/>
+      <c r="E164" s="19"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3106,7 +3106,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="18"/>
+      <c r="E165" s="19"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="18"/>
+      <c r="E166" s="19"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="18"/>
+      <c r="E167" s="19"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="18"/>
+      <c r="E168" s="19"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="18"/>
+      <c r="E169" s="19"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="18"/>
+      <c r="E170" s="19"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3190,7 +3190,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="18"/>
+      <c r="E171" s="19"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="18"/>
+      <c r="E172" s="19"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="18"/>
+      <c r="E173" s="19"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="18"/>
+      <c r="E174" s="19"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="18"/>
+      <c r="E175" s="19"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="18"/>
+      <c r="E176" s="19"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="18"/>
+      <c r="E177" s="19"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3288,7 +3288,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="18"/>
+      <c r="E178" s="19"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="19"/>
+      <c r="E179" s="20"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3310,12 +3310,6 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="E30:E39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E19:E26"/>
     <mergeCell ref="E153:E179"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="F40:F43"/>
@@ -3327,6 +3321,12 @@
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="E62:E70"/>
     <mergeCell ref="E71:E79"/>
+    <mergeCell ref="E30:E39"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="E19:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
herencia ej2 por la mitad
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Fecha</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Herencia</t>
+  </si>
+  <si>
+    <t>Excepciones</t>
+  </si>
+  <si>
+    <t>MySQL</t>
   </si>
 </sst>
 </file>
@@ -266,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -316,22 +322,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -345,6 +339,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -659,11 +662,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F180"/>
+  <dimension ref="A1:F179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,10 +726,10 @@
       <c r="C3" s="8">
         <v>45019</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="23">
         <v>1</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="19" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -741,8 +744,8 @@
       <c r="C4" s="8">
         <v>45020</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -757,10 +760,10 @@
       <c r="C5" s="8">
         <v>45021</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="23">
         <v>2</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="19" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -777,8 +780,8 @@
       <c r="C6" s="8">
         <v>45026</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -793,8 +796,8 @@
       <c r="C7" s="8">
         <v>45027</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -809,10 +812,10 @@
       <c r="C8" s="8">
         <v>45028</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="23">
         <v>3</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -829,8 +832,8 @@
       <c r="C9" s="8">
         <v>45029</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -845,8 +848,8 @@
       <c r="C10" s="8">
         <v>45033</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -861,8 +864,8 @@
       <c r="C11" s="8">
         <v>45034</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -897,10 +900,10 @@
       <c r="C13" s="8">
         <v>45036</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="23">
         <v>4</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -917,8 +920,8 @@
       <c r="C14" s="8">
         <v>45040</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -933,8 +936,8 @@
       <c r="C15" s="8">
         <v>45041</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -949,8 +952,8 @@
       <c r="C16" s="8">
         <v>45042</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -965,8 +968,8 @@
       <c r="C17" s="8">
         <v>45043</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -981,7 +984,7 @@
       <c r="C18" s="8">
         <v>45048</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="14" t="s">
         <v>8</v>
       </c>
@@ -999,10 +1002,10 @@
       <c r="C19" s="8">
         <v>45049</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="23">
         <v>5</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1019,8 +1022,8 @@
       <c r="C20" s="8">
         <v>45050</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1035,8 +1038,8 @@
       <c r="C21" s="8">
         <v>45054</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1051,8 +1054,8 @@
       <c r="C22" s="8">
         <v>45055</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1067,8 +1070,8 @@
       <c r="C23" s="8">
         <v>45056</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1083,8 +1086,8 @@
       <c r="C24" s="8">
         <v>45057</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="23"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1099,8 +1102,8 @@
       <c r="C25" s="8">
         <v>45062</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="23"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1115,8 +1118,8 @@
       <c r="C26" s="8">
         <v>45062</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="23"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1131,7 +1134,7 @@
       <c r="C27" s="8">
         <v>45063</v>
       </c>
-      <c r="D27" s="21"/>
+      <c r="D27" s="24"/>
       <c r="E27" s="14" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1152,7 @@
       <c r="C28" s="8">
         <v>45064</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="14" t="s">
         <v>9</v>
       </c>
@@ -1187,10 +1190,10 @@
       <c r="C30" s="8">
         <v>45069</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="23">
         <v>7</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="19" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1207,8 +1210,8 @@
       <c r="C31" s="8">
         <v>45070</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1223,8 +1226,8 @@
       <c r="C32" s="8">
         <v>45075</v>
       </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1239,8 +1242,8 @@
       <c r="C33" s="8">
         <v>45076</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="19"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1255,8 +1258,8 @@
       <c r="C34" s="8">
         <v>45077</v>
       </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="19"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1271,8 +1274,8 @@
       <c r="C35" s="8">
         <v>45078</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1287,8 +1290,8 @@
       <c r="C36" s="8">
         <v>45082</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1303,8 +1306,8 @@
       <c r="C37" s="8">
         <v>45083</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="23"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1319,8 +1322,8 @@
       <c r="C38" s="8">
         <v>45084</v>
       </c>
-      <c r="D38" s="21"/>
-      <c r="E38" s="23"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1335,8 +1338,8 @@
       <c r="C39" s="8">
         <v>45085</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="23"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="19"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1351,13 +1354,13 @@
       <c r="C40" s="8">
         <v>45089</v>
       </c>
-      <c r="D40" s="20">
+      <c r="D40" s="23">
         <v>8</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="29" t="s">
+      <c r="F40" s="28" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1371,9 +1374,9 @@
       <c r="C41" s="8">
         <v>45090</v>
       </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="29"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1385,9 +1388,9 @@
       <c r="C42" s="8">
         <v>45091</v>
       </c>
-      <c r="D42" s="21"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="29"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="28"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1399,9 +1402,9 @@
       <c r="C43" s="8">
         <v>45092</v>
       </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="29"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1413,8 +1416,8 @@
       <c r="C44" s="8">
         <v>45098</v>
       </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="23"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="19"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1429,8 +1432,8 @@
       <c r="C45" s="8">
         <v>45099</v>
       </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="23"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="19"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1445,9 +1448,9 @@
       <c r="C46" s="8">
         <v>45103</v>
       </c>
-      <c r="D46" s="21"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="29" t="s">
+      <c r="D46" s="24"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="28" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1461,9 +1464,9 @@
       <c r="C47" s="8">
         <v>45104</v>
       </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="29"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="28"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1475,9 +1478,9 @@
       <c r="C48" s="8">
         <v>45105</v>
       </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="29"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="28"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1489,9 +1492,9 @@
       <c r="C49" s="8">
         <v>45106</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="29"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="28"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1503,8 +1506,8 @@
       <c r="C50" s="8">
         <v>45110</v>
       </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="23"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="19"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1519,9 +1522,9 @@
       <c r="C51" s="11">
         <v>45111</v>
       </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="30" t="s">
+      <c r="D51" s="24"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1535,9 +1538,9 @@
       <c r="C52" s="8">
         <v>45112</v>
       </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="30"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="29"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1549,9 +1552,9 @@
       <c r="C53" s="8">
         <v>45113</v>
       </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="30"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="29"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1563,9 +1566,9 @@
       <c r="C54" s="8">
         <v>45117</v>
       </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="30"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="29"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1577,9 +1580,9 @@
       <c r="C55" s="8">
         <v>45118</v>
       </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="29" t="s">
+      <c r="D55" s="24"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="28" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1593,9 +1596,9 @@
       <c r="C56" s="8">
         <v>45119</v>
       </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="29"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="28"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1607,9 +1610,9 @@
       <c r="C57" s="8">
         <v>45120</v>
       </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="29" t="s">
+      <c r="D57" s="24"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="28" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1623,9 +1626,9 @@
       <c r="C58" s="8">
         <v>45124</v>
       </c>
-      <c r="D58" s="21"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="29"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="28"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1637,8 +1640,8 @@
       <c r="C59" s="8">
         <v>45125</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="23"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="19"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1653,13 +1656,13 @@
       <c r="C60" s="8">
         <v>45126</v>
       </c>
-      <c r="D60" s="20">
+      <c r="D60" s="23">
         <v>9</v>
       </c>
-      <c r="E60" s="24" t="s">
+      <c r="E60" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="27" t="s">
+      <c r="F60" s="26" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1673,9 +1676,9 @@
       <c r="C61" s="8">
         <v>45127</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="28"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="27"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1687,10 +1690,10 @@
       <c r="C62" s="8">
         <v>45131</v>
       </c>
-      <c r="D62" s="20">
+      <c r="D62" s="23">
         <v>10</v>
       </c>
-      <c r="E62" s="24" t="s">
+      <c r="E62" s="20" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1705,8 +1708,8 @@
       <c r="C63" s="8">
         <v>45132</v>
       </c>
-      <c r="D63" s="21"/>
-      <c r="E63" s="25"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="21"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1719,8 +1722,8 @@
       <c r="C64" s="8">
         <v>45133</v>
       </c>
-      <c r="D64" s="21"/>
-      <c r="E64" s="25"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="21"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1733,8 +1736,8 @@
       <c r="C65" s="8">
         <v>45134</v>
       </c>
-      <c r="D65" s="21"/>
-      <c r="E65" s="25"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="21"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,8 +1750,8 @@
       <c r="C66" s="8">
         <v>45138</v>
       </c>
-      <c r="D66" s="21"/>
-      <c r="E66" s="25"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="21"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1761,8 +1764,8 @@
       <c r="C67" s="11">
         <v>45139</v>
       </c>
-      <c r="D67" s="21"/>
-      <c r="E67" s="25"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="21"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1775,8 +1778,8 @@
       <c r="C68" s="8">
         <v>45140</v>
       </c>
-      <c r="D68" s="21"/>
-      <c r="E68" s="25"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="21"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,8 +1792,8 @@
       <c r="C69" s="8">
         <v>45141</v>
       </c>
-      <c r="D69" s="21"/>
-      <c r="E69" s="25"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="21"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1803,8 +1806,8 @@
       <c r="C70" s="8">
         <v>45146</v>
       </c>
-      <c r="D70" s="22"/>
-      <c r="E70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="21"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1817,10 +1820,10 @@
       <c r="C71" s="8">
         <v>45147</v>
       </c>
-      <c r="D71" s="20">
+      <c r="D71" s="23">
         <v>11</v>
       </c>
-      <c r="E71" s="24" t="s">
+      <c r="E71" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1835,8 +1838,8 @@
       <c r="C72" s="11">
         <v>45148</v>
       </c>
-      <c r="D72" s="21"/>
-      <c r="E72" s="25"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="21"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1849,8 +1852,8 @@
       <c r="C73" s="8">
         <v>45152</v>
       </c>
-      <c r="D73" s="21"/>
-      <c r="E73" s="25"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="21"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1863,8 +1866,8 @@
       <c r="C74" s="8">
         <v>45153</v>
       </c>
-      <c r="D74" s="21"/>
-      <c r="E74" s="25"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="21"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -1879,8 +1882,8 @@
       <c r="C75" s="8">
         <v>45154</v>
       </c>
-      <c r="D75" s="21"/>
-      <c r="E75" s="25"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="21"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1893,8 +1896,8 @@
       <c r="C76" s="8">
         <v>45155</v>
       </c>
-      <c r="D76" s="21"/>
-      <c r="E76" s="25"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="21"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1907,8 +1910,8 @@
       <c r="C77" s="8">
         <v>45160</v>
       </c>
-      <c r="D77" s="21"/>
-      <c r="E77" s="25"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="21"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1921,8 +1924,8 @@
       <c r="C78" s="8">
         <v>45161</v>
       </c>
-      <c r="D78" s="21"/>
-      <c r="E78" s="25"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="21"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -1935,8 +1938,8 @@
       <c r="C79" s="8">
         <v>45162</v>
       </c>
-      <c r="D79" s="21"/>
-      <c r="E79" s="25"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="21"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -1949,36 +1952,40 @@
       <c r="C80" s="8">
         <v>45166</v>
       </c>
-      <c r="D80" s="22"/>
-      <c r="E80" s="26"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="22"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>80</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="18"/>
+      <c r="B81" s="5">
+        <v>1</v>
+      </c>
+      <c r="C81" s="8">
+        <v>45167</v>
+      </c>
+      <c r="D81" s="18">
+        <v>12</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F81" s="5"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>81</v>
       </c>
       <c r="B82" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C82" s="8">
-        <v>45167</v>
-      </c>
-      <c r="D82" s="20">
-        <v>12</v>
-      </c>
-      <c r="E82" s="24" t="s">
-        <v>46</v>
-      </c>
+        <v>45168</v>
+      </c>
+      <c r="D82" s="18"/>
+      <c r="E82" s="19"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -1986,13 +1993,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C83" s="8">
-        <v>45168</v>
-      </c>
-      <c r="D83" s="21"/>
-      <c r="E83" s="25"/>
+        <v>45169</v>
+      </c>
+      <c r="D83" s="18"/>
+      <c r="E83" s="19"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2000,13 +2007,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C84" s="9">
-        <v>45169</v>
-      </c>
-      <c r="D84" s="21"/>
-      <c r="E84" s="25"/>
+        <v>45173</v>
+      </c>
+      <c r="D84" s="18"/>
+      <c r="E84" s="19"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2014,13 +2021,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C85" s="9">
-        <v>45173</v>
-      </c>
-      <c r="D85" s="21"/>
-      <c r="E85" s="25"/>
+        <v>45174</v>
+      </c>
+      <c r="D85" s="18"/>
+      <c r="E85" s="19"/>
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2028,13 +2035,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C86" s="9">
-        <v>45174</v>
-      </c>
-      <c r="D86" s="21"/>
-      <c r="E86" s="25"/>
+        <v>45175</v>
+      </c>
+      <c r="D86" s="18"/>
+      <c r="E86" s="19"/>
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2042,13 +2049,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C87" s="9">
-        <v>45175</v>
-      </c>
-      <c r="D87" s="21"/>
-      <c r="E87" s="25"/>
+        <v>45176</v>
+      </c>
+      <c r="D87" s="18"/>
+      <c r="E87" s="19"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2056,13 +2063,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C88" s="9">
-        <v>45176</v>
-      </c>
-      <c r="D88" s="21"/>
-      <c r="E88" s="25"/>
+        <v>45180</v>
+      </c>
+      <c r="D88" s="18"/>
+      <c r="E88" s="19"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2070,13 +2077,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C89" s="9">
-        <v>45180</v>
-      </c>
-      <c r="D89" s="21"/>
-      <c r="E89" s="25"/>
+        <v>45181</v>
+      </c>
+      <c r="D89" s="18"/>
+      <c r="E89" s="19"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2084,193 +2091,233 @@
         <v>89</v>
       </c>
       <c r="B90" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C90" s="9">
-        <v>45181</v>
-      </c>
-      <c r="D90" s="22"/>
-      <c r="E90" s="26"/>
+        <v>45182</v>
+      </c>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>90</v>
       </c>
-      <c r="B91" s="5"/>
+      <c r="B91" s="17">
+        <v>11</v>
+      </c>
       <c r="C91" s="9">
-        <v>45182</v>
-      </c>
-      <c r="D91" s="6"/>
-      <c r="E91" s="14"/>
+        <v>45183</v>
+      </c>
+      <c r="D91" s="18"/>
+      <c r="E91" s="19"/>
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>91</v>
       </c>
-      <c r="B92" s="5"/>
+      <c r="B92" s="17">
+        <v>1</v>
+      </c>
       <c r="C92" s="9">
-        <v>45183</v>
-      </c>
-      <c r="D92" s="6"/>
-      <c r="E92" s="14"/>
+        <v>45187</v>
+      </c>
+      <c r="D92" s="18">
+        <v>13</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="F92" s="5"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>92</v>
       </c>
-      <c r="B93" s="5"/>
+      <c r="B93" s="17">
+        <v>2</v>
+      </c>
       <c r="C93" s="9">
-        <v>45187</v>
-      </c>
-      <c r="D93" s="6"/>
-      <c r="E93" s="14"/>
+        <v>45188</v>
+      </c>
+      <c r="D93" s="18"/>
+      <c r="E93" s="19"/>
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>93</v>
       </c>
-      <c r="B94" s="5"/>
+      <c r="B94" s="17">
+        <v>3</v>
+      </c>
       <c r="C94" s="9">
-        <v>45188</v>
-      </c>
-      <c r="D94" s="6"/>
-      <c r="E94" s="14"/>
+        <v>45189</v>
+      </c>
+      <c r="D94" s="18"/>
+      <c r="E94" s="19"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>94</v>
       </c>
-      <c r="B95" s="5"/>
+      <c r="B95" s="17">
+        <v>4</v>
+      </c>
       <c r="C95" s="9">
-        <v>45189</v>
-      </c>
-      <c r="D95" s="6"/>
-      <c r="E95" s="14"/>
+        <v>45194</v>
+      </c>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>95</v>
       </c>
-      <c r="B96" s="5"/>
+      <c r="B96" s="5">
+        <v>1</v>
+      </c>
       <c r="C96" s="9">
-        <v>45190</v>
-      </c>
-      <c r="D96" s="6"/>
-      <c r="E96" s="14"/>
+        <v>45195</v>
+      </c>
+      <c r="D96" s="23">
+        <v>14</v>
+      </c>
+      <c r="E96" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="F96" s="5"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>96</v>
       </c>
-      <c r="B97" s="5"/>
+      <c r="B97" s="5">
+        <v>2</v>
+      </c>
       <c r="C97" s="9">
-        <v>45194</v>
-      </c>
-      <c r="D97" s="6"/>
-      <c r="E97" s="14"/>
+        <v>45196</v>
+      </c>
+      <c r="D97" s="24"/>
+      <c r="E97" s="21"/>
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>97</v>
       </c>
-      <c r="B98" s="5"/>
+      <c r="B98" s="5">
+        <v>3</v>
+      </c>
       <c r="C98" s="9">
-        <v>45195</v>
-      </c>
-      <c r="D98" s="6"/>
-      <c r="E98" s="14"/>
+        <v>45197</v>
+      </c>
+      <c r="D98" s="24"/>
+      <c r="E98" s="21"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>98</v>
       </c>
-      <c r="B99" s="5"/>
+      <c r="B99" s="5">
+        <v>4</v>
+      </c>
       <c r="C99" s="9">
-        <v>45196</v>
-      </c>
-      <c r="D99" s="6"/>
-      <c r="E99" s="14"/>
+        <v>45201</v>
+      </c>
+      <c r="D99" s="24"/>
+      <c r="E99" s="21"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>99</v>
       </c>
-      <c r="B100" s="5"/>
+      <c r="B100" s="5">
+        <v>5</v>
+      </c>
       <c r="C100" s="9">
-        <v>45197</v>
-      </c>
-      <c r="D100" s="6"/>
-      <c r="E100" s="14"/>
+        <v>45202</v>
+      </c>
+      <c r="D100" s="24"/>
+      <c r="E100" s="21"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>100</v>
       </c>
-      <c r="B101" s="5"/>
+      <c r="B101" s="5">
+        <v>6</v>
+      </c>
       <c r="C101" s="9">
-        <v>45201</v>
-      </c>
-      <c r="D101" s="6"/>
-      <c r="E101" s="14"/>
+        <v>45203</v>
+      </c>
+      <c r="D101" s="24"/>
+      <c r="E101" s="21"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>101</v>
       </c>
-      <c r="B102" s="5"/>
+      <c r="B102" s="5">
+        <v>7</v>
+      </c>
       <c r="C102" s="9">
-        <v>45202</v>
-      </c>
-      <c r="D102" s="6"/>
-      <c r="E102" s="14"/>
+        <v>45204</v>
+      </c>
+      <c r="D102" s="24"/>
+      <c r="E102" s="21"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>102</v>
       </c>
-      <c r="B103" s="5"/>
+      <c r="B103" s="5">
+        <v>8</v>
+      </c>
       <c r="C103" s="9">
-        <v>45203</v>
-      </c>
-      <c r="D103" s="6"/>
-      <c r="E103" s="14"/>
+        <v>45208</v>
+      </c>
+      <c r="D103" s="24"/>
+      <c r="E103" s="21"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>103</v>
       </c>
-      <c r="B104" s="5"/>
+      <c r="B104" s="5">
+        <v>9</v>
+      </c>
       <c r="C104" s="9">
-        <v>45204</v>
-      </c>
-      <c r="D104" s="6"/>
-      <c r="E104" s="14"/>
+        <v>45209</v>
+      </c>
+      <c r="D104" s="25"/>
+      <c r="E104" s="22"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>104</v>
       </c>
-      <c r="B105" s="5"/>
+      <c r="B105" s="5">
+        <v>1</v>
+      </c>
       <c r="C105" s="9">
-        <v>45208</v>
+        <v>45210</v>
       </c>
       <c r="D105" s="6"/>
-      <c r="E105" s="14"/>
+      <c r="E105" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="F105" s="5"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -2279,7 +2326,7 @@
       </c>
       <c r="B106" s="5"/>
       <c r="C106" s="9">
-        <v>45209</v>
+        <v>45211</v>
       </c>
       <c r="D106" s="6"/>
       <c r="E106" s="14"/>
@@ -2291,7 +2338,7 @@
       </c>
       <c r="B107" s="5"/>
       <c r="C107" s="9">
-        <v>45210</v>
+        <v>45216</v>
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="14"/>
@@ -2303,7 +2350,7 @@
       </c>
       <c r="B108" s="5"/>
       <c r="C108" s="9">
-        <v>45211</v>
+        <v>45217</v>
       </c>
       <c r="D108" s="6"/>
       <c r="E108" s="14"/>
@@ -2315,7 +2362,7 @@
       </c>
       <c r="B109" s="5"/>
       <c r="C109" s="9">
-        <v>45216</v>
+        <v>45218</v>
       </c>
       <c r="D109" s="6"/>
       <c r="E109" s="14"/>
@@ -2327,7 +2374,7 @@
       </c>
       <c r="B110" s="5"/>
       <c r="C110" s="9">
-        <v>45217</v>
+        <v>45222</v>
       </c>
       <c r="D110" s="6"/>
       <c r="E110" s="14"/>
@@ -2339,7 +2386,7 @@
       </c>
       <c r="B111" s="5"/>
       <c r="C111" s="9">
-        <v>45218</v>
+        <v>45223</v>
       </c>
       <c r="D111" s="6"/>
       <c r="E111" s="14"/>
@@ -2351,7 +2398,7 @@
       </c>
       <c r="B112" s="5"/>
       <c r="C112" s="9">
-        <v>45222</v>
+        <v>45224</v>
       </c>
       <c r="D112" s="6"/>
       <c r="E112" s="14"/>
@@ -2363,7 +2410,7 @@
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="9">
-        <v>45223</v>
+        <v>45225</v>
       </c>
       <c r="D113" s="6"/>
       <c r="E113" s="14"/>
@@ -2375,7 +2422,7 @@
       </c>
       <c r="B114" s="5"/>
       <c r="C114" s="9">
-        <v>45224</v>
+        <v>45229</v>
       </c>
       <c r="D114" s="6"/>
       <c r="E114" s="14"/>
@@ -2387,7 +2434,7 @@
       </c>
       <c r="B115" s="5"/>
       <c r="C115" s="9">
-        <v>45225</v>
+        <v>45230</v>
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="14"/>
@@ -2399,7 +2446,7 @@
       </c>
       <c r="B116" s="5"/>
       <c r="C116" s="9">
-        <v>45229</v>
+        <v>45231</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="14"/>
@@ -2411,7 +2458,7 @@
       </c>
       <c r="B117" s="5"/>
       <c r="C117" s="9">
-        <v>45230</v>
+        <v>45232</v>
       </c>
       <c r="D117" s="6"/>
       <c r="E117" s="14"/>
@@ -2423,7 +2470,7 @@
       </c>
       <c r="B118" s="5"/>
       <c r="C118" s="9">
-        <v>45231</v>
+        <v>45236</v>
       </c>
       <c r="D118" s="6"/>
       <c r="E118" s="14"/>
@@ -2435,7 +2482,7 @@
       </c>
       <c r="B119" s="5"/>
       <c r="C119" s="9">
-        <v>45232</v>
+        <v>45237</v>
       </c>
       <c r="D119" s="6"/>
       <c r="E119" s="14"/>
@@ -2447,7 +2494,7 @@
       </c>
       <c r="B120" s="5"/>
       <c r="C120" s="9">
-        <v>45236</v>
+        <v>45238</v>
       </c>
       <c r="D120" s="6"/>
       <c r="E120" s="14"/>
@@ -2459,7 +2506,7 @@
       </c>
       <c r="B121" s="5"/>
       <c r="C121" s="9">
-        <v>45237</v>
+        <v>45239</v>
       </c>
       <c r="D121" s="6"/>
       <c r="E121" s="14"/>
@@ -2471,7 +2518,7 @@
       </c>
       <c r="B122" s="5"/>
       <c r="C122" s="9">
-        <v>45238</v>
+        <v>45243</v>
       </c>
       <c r="D122" s="6"/>
       <c r="E122" s="14"/>
@@ -2483,7 +2530,7 @@
       </c>
       <c r="B123" s="5"/>
       <c r="C123" s="9">
-        <v>45239</v>
+        <v>45244</v>
       </c>
       <c r="D123" s="6"/>
       <c r="E123" s="14"/>
@@ -2495,7 +2542,7 @@
       </c>
       <c r="B124" s="5"/>
       <c r="C124" s="9">
-        <v>45243</v>
+        <v>45245</v>
       </c>
       <c r="D124" s="6"/>
       <c r="E124" s="14"/>
@@ -2507,7 +2554,7 @@
       </c>
       <c r="B125" s="5"/>
       <c r="C125" s="9">
-        <v>45244</v>
+        <v>45246</v>
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="14"/>
@@ -2519,7 +2566,7 @@
       </c>
       <c r="B126" s="5"/>
       <c r="C126" s="9">
-        <v>45245</v>
+        <v>45251</v>
       </c>
       <c r="D126" s="6"/>
       <c r="E126" s="14"/>
@@ -2531,7 +2578,7 @@
       </c>
       <c r="B127" s="5"/>
       <c r="C127" s="9">
-        <v>45246</v>
+        <v>45252</v>
       </c>
       <c r="D127" s="6"/>
       <c r="E127" s="14"/>
@@ -2543,7 +2590,7 @@
       </c>
       <c r="B128" s="5"/>
       <c r="C128" s="9">
-        <v>45251</v>
+        <v>45253</v>
       </c>
       <c r="D128" s="6"/>
       <c r="E128" s="14"/>
@@ -2555,7 +2602,7 @@
       </c>
       <c r="B129" s="5"/>
       <c r="C129" s="9">
-        <v>45252</v>
+        <v>45257</v>
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="14"/>
@@ -2567,7 +2614,7 @@
       </c>
       <c r="B130" s="5"/>
       <c r="C130" s="9">
-        <v>45253</v>
+        <v>45258</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="14"/>
@@ -2579,7 +2626,7 @@
       </c>
       <c r="B131" s="5"/>
       <c r="C131" s="9">
-        <v>45257</v>
+        <v>45259</v>
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="14"/>
@@ -2591,7 +2638,7 @@
       </c>
       <c r="B132" s="5"/>
       <c r="C132" s="9">
-        <v>45258</v>
+        <v>45260</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="14"/>
@@ -2603,7 +2650,7 @@
       </c>
       <c r="B133" s="5"/>
       <c r="C133" s="9">
-        <v>45259</v>
+        <v>45264</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="14"/>
@@ -2615,7 +2662,7 @@
       </c>
       <c r="B134" s="5"/>
       <c r="C134" s="9">
-        <v>45260</v>
+        <v>45265</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="14"/>
@@ -2627,7 +2674,7 @@
       </c>
       <c r="B135" s="5"/>
       <c r="C135" s="9">
-        <v>45264</v>
+        <v>45266</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="14"/>
@@ -2639,7 +2686,7 @@
       </c>
       <c r="B136" s="5"/>
       <c r="C136" s="9">
-        <v>45265</v>
+        <v>45267</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="14"/>
@@ -2651,7 +2698,7 @@
       </c>
       <c r="B137" s="5"/>
       <c r="C137" s="9">
-        <v>45266</v>
+        <v>45271</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="14"/>
@@ -2663,7 +2710,7 @@
       </c>
       <c r="B138" s="5"/>
       <c r="C138" s="9">
-        <v>45267</v>
+        <v>45272</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="14"/>
@@ -2675,7 +2722,7 @@
       </c>
       <c r="B139" s="5"/>
       <c r="C139" s="9">
-        <v>45271</v>
+        <v>45273</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="14"/>
@@ -2687,7 +2734,7 @@
       </c>
       <c r="B140" s="5"/>
       <c r="C140" s="9">
-        <v>45272</v>
+        <v>45274</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="14"/>
@@ -2699,7 +2746,7 @@
       </c>
       <c r="B141" s="5"/>
       <c r="C141" s="9">
-        <v>45273</v>
+        <v>45278</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="14"/>
@@ -2711,7 +2758,7 @@
       </c>
       <c r="B142" s="5"/>
       <c r="C142" s="9">
-        <v>45274</v>
+        <v>45279</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="14"/>
@@ -2723,7 +2770,7 @@
       </c>
       <c r="B143" s="5"/>
       <c r="C143" s="9">
-        <v>45278</v>
+        <v>45280</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="14"/>
@@ -2735,7 +2782,7 @@
       </c>
       <c r="B144" s="5"/>
       <c r="C144" s="9">
-        <v>45279</v>
+        <v>45281</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="14"/>
@@ -2746,11 +2793,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="5"/>
-      <c r="C145" s="9">
-        <v>45280</v>
-      </c>
       <c r="D145" s="6"/>
-      <c r="E145" s="14"/>
+      <c r="E145" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F145" s="5"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -2759,17 +2805,20 @@
       </c>
       <c r="B146" s="5"/>
       <c r="C146" s="9">
-        <v>45281</v>
+        <v>45286</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F146" s="5"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="5"/>
+      <c r="C147" s="9">
+        <v>45287</v>
+      </c>
       <c r="D147" s="6"/>
       <c r="E147" s="14" t="s">
         <v>29</v>
@@ -2780,7 +2829,7 @@
       <c r="A148" s="5"/>
       <c r="B148" s="5"/>
       <c r="C148" s="9">
-        <v>45286</v>
+        <v>45288</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="14" t="s">
@@ -2792,11 +2841,11 @@
       <c r="A149" s="5"/>
       <c r="B149" s="5"/>
       <c r="C149" s="9">
-        <v>45287</v>
+        <v>45293</v>
       </c>
       <c r="D149" s="6"/>
       <c r="E149" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F149" s="5"/>
     </row>
@@ -2804,7 +2853,7 @@
       <c r="A150" s="5"/>
       <c r="B150" s="5"/>
       <c r="C150" s="9">
-        <v>45288</v>
+        <v>45294</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="14" t="s">
@@ -2816,7 +2865,7 @@
       <c r="A151" s="5"/>
       <c r="B151" s="5"/>
       <c r="C151" s="9">
-        <v>45293</v>
+        <v>45295</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="14" t="s">
@@ -2828,7 +2877,7 @@
       <c r="A152" s="5"/>
       <c r="B152" s="5"/>
       <c r="C152" s="9">
-        <v>45294</v>
+        <v>45299</v>
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="14" t="s">
@@ -2840,13 +2889,15 @@
       <c r="A153" s="5">
         <v>146</v>
       </c>
-      <c r="B153" s="5"/>
+      <c r="B153" s="5">
+        <v>1</v>
+      </c>
       <c r="C153" s="9">
-        <v>45295</v>
+        <v>45300</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="14" t="s">
-        <v>27</v>
+      <c r="E153" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="F153" s="5"/>
     </row>
@@ -2855,15 +2906,13 @@
         <v>147</v>
       </c>
       <c r="B154" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C154" s="9">
-        <v>45299</v>
+        <v>45301</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="24" t="s">
-        <v>26</v>
-      </c>
+      <c r="E154" s="21"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2871,13 +2920,13 @@
         <v>148</v>
       </c>
       <c r="B155" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C155" s="9">
-        <v>45300</v>
+        <v>45302</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="25"/>
+      <c r="E155" s="21"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2885,13 +2934,13 @@
         <v>149</v>
       </c>
       <c r="B156" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C156" s="9">
-        <v>45301</v>
+        <v>45306</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="25"/>
+      <c r="E156" s="21"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2899,13 +2948,13 @@
         <v>150</v>
       </c>
       <c r="B157" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C157" s="9">
-        <v>45302</v>
+        <v>45307</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="25"/>
+      <c r="E157" s="21"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -2913,13 +2962,13 @@
         <v>151</v>
       </c>
       <c r="B158" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C158" s="9">
-        <v>45306</v>
+        <v>45308</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="25"/>
+      <c r="E158" s="21"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -2927,27 +2976,27 @@
         <v>152</v>
       </c>
       <c r="B159" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C159" s="9">
-        <v>45307</v>
+        <v>45309</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="25"/>
+      <c r="E159" s="21"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="12">
         <v>153</v>
       </c>
-      <c r="B160" s="5">
-        <v>7</v>
+      <c r="B160" s="12">
+        <v>8</v>
       </c>
       <c r="C160" s="9">
-        <v>45308</v>
+        <v>45313</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="25"/>
+      <c r="E160" s="21"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -2955,13 +3004,13 @@
         <v>154</v>
       </c>
       <c r="B161" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C161" s="9">
-        <v>45309</v>
+        <v>45314</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="25"/>
+      <c r="E161" s="21"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -2969,27 +3018,27 @@
         <v>155</v>
       </c>
       <c r="B162" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C162" s="9">
-        <v>45313</v>
+        <v>45315</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="25"/>
-      <c r="F162" s="5"/>
+      <c r="E162" s="21"/>
+      <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="12">
         <v>156</v>
       </c>
       <c r="B163" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C163" s="9">
-        <v>45314</v>
+        <v>45316</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="25"/>
+      <c r="E163" s="21"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -2997,13 +3046,13 @@
         <v>157</v>
       </c>
       <c r="B164" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C164" s="9">
-        <v>45315</v>
+        <v>45320</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="25"/>
+      <c r="E164" s="21"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3011,13 +3060,13 @@
         <v>158</v>
       </c>
       <c r="B165" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C165" s="9">
-        <v>45316</v>
+        <v>45321</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="25"/>
+      <c r="E165" s="21"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3025,13 +3074,13 @@
         <v>159</v>
       </c>
       <c r="B166" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C166" s="9">
-        <v>45320</v>
+        <v>45322</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="25"/>
+      <c r="E166" s="21"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3039,13 +3088,13 @@
         <v>160</v>
       </c>
       <c r="B167" s="12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C167" s="9">
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="25"/>
+      <c r="E167" s="21"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3053,13 +3102,13 @@
         <v>161</v>
       </c>
       <c r="B168" s="12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C168" s="9">
-        <v>45322</v>
+        <v>45327</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="25"/>
+      <c r="E168" s="21"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3067,13 +3116,13 @@
         <v>162</v>
       </c>
       <c r="B169" s="12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C169" s="9">
-        <v>45323</v>
+        <v>45328</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="25"/>
+      <c r="E169" s="21"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3081,13 +3130,13 @@
         <v>163</v>
       </c>
       <c r="B170" s="12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C170" s="9">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="25"/>
+      <c r="E170" s="21"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3095,13 +3144,13 @@
         <v>164</v>
       </c>
       <c r="B171" s="12">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C171" s="9">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="25"/>
+      <c r="E171" s="21"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3109,13 +3158,13 @@
         <v>165</v>
       </c>
       <c r="B172" s="12">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C172" s="9">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="25"/>
+      <c r="E172" s="21"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3123,13 +3172,13 @@
         <v>166</v>
       </c>
       <c r="B173" s="12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C173" s="9">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="25"/>
+      <c r="E173" s="21"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3137,13 +3186,13 @@
         <v>167</v>
       </c>
       <c r="B174" s="12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C174" s="9">
-        <v>45334</v>
+        <v>45336</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="25"/>
+      <c r="E174" s="21"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3151,13 +3200,13 @@
         <v>168</v>
       </c>
       <c r="B175" s="12">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C175" s="9">
-        <v>45335</v>
+        <v>45337</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="25"/>
+      <c r="E175" s="21"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3165,13 +3214,13 @@
         <v>169</v>
       </c>
       <c r="B176" s="12">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C176" s="9">
-        <v>45336</v>
+        <v>45341</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="25"/>
+      <c r="E176" s="21"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3179,13 +3228,13 @@
         <v>170</v>
       </c>
       <c r="B177" s="12">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C177" s="9">
-        <v>45337</v>
+        <v>45342</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="25"/>
+      <c r="E177" s="21"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3193,13 +3242,13 @@
         <v>171</v>
       </c>
       <c r="B178" s="12">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C178" s="9">
-        <v>45341</v>
+        <v>45343</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="25"/>
+      <c r="E178" s="21"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3207,60 +3256,50 @@
         <v>172</v>
       </c>
       <c r="B179" s="12">
-        <v>26</v>
-      </c>
-      <c r="C179" s="9">
-        <v>45342</v>
+        <v>27</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="25"/>
+      <c r="E179" s="22"/>
       <c r="F179" s="12"/>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B180" s="12">
-        <v>27</v>
-      </c>
-      <c r="C180" s="9">
-        <v>45343</v>
-      </c>
-      <c r="D180" s="6"/>
-      <c r="E180" s="26"/>
-      <c r="F180" s="12"/>
     </row>
   </sheetData>
   <sortState columnSort="1" ref="D3:J3">
     <sortCondition ref="D3:J3"/>
   </sortState>
-  <mergeCells count="29">
+  <mergeCells count="33">
+    <mergeCell ref="D71:D80"/>
+    <mergeCell ref="D81:D91"/>
+    <mergeCell ref="D30:D39"/>
+    <mergeCell ref="D40:D59"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E30:E39"/>
     <mergeCell ref="D62:D70"/>
-    <mergeCell ref="E154:E180"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D13:D18"/>
+    <mergeCell ref="D19:D28"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="E19:E26"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="E40:E59"/>
+    <mergeCell ref="E62:E70"/>
+    <mergeCell ref="E71:E80"/>
+    <mergeCell ref="E81:E91"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="F40:F43"/>
     <mergeCell ref="F46:F49"/>
     <mergeCell ref="F51:F54"/>
     <mergeCell ref="F55:F56"/>
     <mergeCell ref="F57:F58"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="E40:E59"/>
-    <mergeCell ref="E62:E70"/>
-    <mergeCell ref="E71:E80"/>
-    <mergeCell ref="E82:E90"/>
-    <mergeCell ref="D82:D90"/>
-    <mergeCell ref="E30:E39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="D71:D80"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D13:D18"/>
-    <mergeCell ref="D19:D28"/>
-    <mergeCell ref="D30:D39"/>
-    <mergeCell ref="D40:D59"/>
-    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="E96:E104"/>
+    <mergeCell ref="D96:D104"/>
+    <mergeCell ref="E153:E179"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
iniciando ej 3, check listo
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -325,15 +325,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -343,11 +334,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -666,7 +666,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B104" sqref="B104"/>
+      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,10 +726,10 @@
       <c r="C3" s="8">
         <v>45019</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="23">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="19" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -744,8 +744,8 @@
       <c r="C4" s="8">
         <v>45020</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="22"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -760,10 +760,10 @@
       <c r="C5" s="8">
         <v>45021</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="23">
         <v>2</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="19" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -780,8 +780,8 @@
       <c r="C6" s="8">
         <v>45026</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -796,8 +796,8 @@
       <c r="C7" s="8">
         <v>45027</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -812,10 +812,10 @@
       <c r="C8" s="8">
         <v>45028</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="23">
         <v>3</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -832,8 +832,8 @@
       <c r="C9" s="8">
         <v>45029</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -848,8 +848,8 @@
       <c r="C10" s="8">
         <v>45033</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="22"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -864,8 +864,8 @@
       <c r="C11" s="8">
         <v>45034</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -900,10 +900,10 @@
       <c r="C13" s="8">
         <v>45036</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="23">
         <v>4</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -920,8 +920,8 @@
       <c r="C14" s="8">
         <v>45040</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="22"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -936,8 +936,8 @@
       <c r="C15" s="8">
         <v>45041</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="22"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -952,8 +952,8 @@
       <c r="C16" s="8">
         <v>45042</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="22"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -968,8 +968,8 @@
       <c r="C17" s="8">
         <v>45043</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="22"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="C18" s="8">
         <v>45048</v>
       </c>
-      <c r="D18" s="20"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="14" t="s">
         <v>8</v>
       </c>
@@ -1002,10 +1002,10 @@
       <c r="C19" s="8">
         <v>45049</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="23">
         <v>5</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1022,8 +1022,8 @@
       <c r="C20" s="8">
         <v>45050</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1038,8 +1038,8 @@
       <c r="C21" s="8">
         <v>45054</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1054,8 +1054,8 @@
       <c r="C22" s="8">
         <v>45055</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="22"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1070,8 +1070,8 @@
       <c r="C23" s="8">
         <v>45056</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1086,8 +1086,8 @@
       <c r="C24" s="8">
         <v>45057</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="22"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1102,8 +1102,8 @@
       <c r="C25" s="8">
         <v>45062</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="22"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1118,8 +1118,8 @@
       <c r="C26" s="8">
         <v>45062</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="22"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="C27" s="8">
         <v>45063</v>
       </c>
-      <c r="D27" s="19"/>
+      <c r="D27" s="24"/>
       <c r="E27" s="14" t="s">
         <v>8</v>
       </c>
@@ -1152,7 +1152,7 @@
       <c r="C28" s="8">
         <v>45064</v>
       </c>
-      <c r="D28" s="20"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="14" t="s">
         <v>9</v>
       </c>
@@ -1190,10 +1190,10 @@
       <c r="C30" s="8">
         <v>45069</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="23">
         <v>7</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="19" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1210,8 +1210,8 @@
       <c r="C31" s="8">
         <v>45070</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="22"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1226,8 +1226,8 @@
       <c r="C32" s="8">
         <v>45075</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="22"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1242,8 +1242,8 @@
       <c r="C33" s="8">
         <v>45076</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="22"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="19"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1258,8 +1258,8 @@
       <c r="C34" s="8">
         <v>45077</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="22"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="19"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1274,8 +1274,8 @@
       <c r="C35" s="8">
         <v>45078</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="22"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1290,8 +1290,8 @@
       <c r="C36" s="8">
         <v>45082</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="22"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1306,8 +1306,8 @@
       <c r="C37" s="8">
         <v>45083</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="22"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1322,8 +1322,8 @@
       <c r="C38" s="8">
         <v>45084</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="22"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1338,8 +1338,8 @@
       <c r="C39" s="8">
         <v>45085</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="22"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="19"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1354,10 +1354,10 @@
       <c r="C40" s="8">
         <v>45089</v>
       </c>
-      <c r="D40" s="18">
+      <c r="D40" s="23">
         <v>8</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="19" t="s">
         <v>3</v>
       </c>
       <c r="F40" s="28" t="s">
@@ -1374,8 +1374,8 @@
       <c r="C41" s="8">
         <v>45090</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="22"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="19"/>
       <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1388,8 +1388,8 @@
       <c r="C42" s="8">
         <v>45091</v>
       </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="22"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="19"/>
       <c r="F42" s="28"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,8 +1402,8 @@
       <c r="C43" s="8">
         <v>45092</v>
       </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="22"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="19"/>
       <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1416,8 +1416,8 @@
       <c r="C44" s="8">
         <v>45098</v>
       </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="22"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="19"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1432,8 +1432,8 @@
       <c r="C45" s="8">
         <v>45099</v>
       </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="22"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="19"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1448,8 +1448,8 @@
       <c r="C46" s="8">
         <v>45103</v>
       </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="22"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="19"/>
       <c r="F46" s="28" t="s">
         <v>20</v>
       </c>
@@ -1464,8 +1464,8 @@
       <c r="C47" s="8">
         <v>45104</v>
       </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="22"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="19"/>
       <c r="F47" s="28"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1478,8 +1478,8 @@
       <c r="C48" s="8">
         <v>45105</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="22"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="19"/>
       <c r="F48" s="28"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,8 +1492,8 @@
       <c r="C49" s="8">
         <v>45106</v>
       </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="22"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="19"/>
       <c r="F49" s="28"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1506,8 +1506,8 @@
       <c r="C50" s="8">
         <v>45110</v>
       </c>
-      <c r="D50" s="19"/>
-      <c r="E50" s="22"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="19"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1522,8 +1522,8 @@
       <c r="C51" s="11">
         <v>45111</v>
       </c>
-      <c r="D51" s="19"/>
-      <c r="E51" s="22"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="19"/>
       <c r="F51" s="29" t="s">
         <v>18</v>
       </c>
@@ -1538,8 +1538,8 @@
       <c r="C52" s="8">
         <v>45112</v>
       </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="22"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="19"/>
       <c r="F52" s="29"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,8 +1552,8 @@
       <c r="C53" s="8">
         <v>45113</v>
       </c>
-      <c r="D53" s="19"/>
-      <c r="E53" s="22"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="19"/>
       <c r="F53" s="29"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1566,8 +1566,8 @@
       <c r="C54" s="8">
         <v>45117</v>
       </c>
-      <c r="D54" s="19"/>
-      <c r="E54" s="22"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="19"/>
       <c r="F54" s="29"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1580,8 +1580,8 @@
       <c r="C55" s="8">
         <v>45118</v>
       </c>
-      <c r="D55" s="19"/>
-      <c r="E55" s="22"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="19"/>
       <c r="F55" s="28" t="s">
         <v>15</v>
       </c>
@@ -1596,8 +1596,8 @@
       <c r="C56" s="8">
         <v>45119</v>
       </c>
-      <c r="D56" s="19"/>
-      <c r="E56" s="22"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="19"/>
       <c r="F56" s="28"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1610,8 +1610,8 @@
       <c r="C57" s="8">
         <v>45120</v>
       </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="22"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="19"/>
       <c r="F57" s="28" t="s">
         <v>16</v>
       </c>
@@ -1626,8 +1626,8 @@
       <c r="C58" s="8">
         <v>45124</v>
       </c>
-      <c r="D58" s="19"/>
-      <c r="E58" s="22"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="19"/>
       <c r="F58" s="28"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1640,8 +1640,8 @@
       <c r="C59" s="8">
         <v>45125</v>
       </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="22"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="19"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1656,10 +1656,10 @@
       <c r="C60" s="8">
         <v>45126</v>
       </c>
-      <c r="D60" s="18">
+      <c r="D60" s="23">
         <v>9</v>
       </c>
-      <c r="E60" s="23" t="s">
+      <c r="E60" s="20" t="s">
         <v>41</v>
       </c>
       <c r="F60" s="26" t="s">
@@ -1676,8 +1676,8 @@
       <c r="C61" s="8">
         <v>45127</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="24"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="22"/>
       <c r="F61" s="27"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1690,10 +1690,10 @@
       <c r="C62" s="8">
         <v>45131</v>
       </c>
-      <c r="D62" s="18">
+      <c r="D62" s="23">
         <v>10</v>
       </c>
-      <c r="E62" s="23" t="s">
+      <c r="E62" s="20" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1708,8 +1708,8 @@
       <c r="C63" s="8">
         <v>45132</v>
       </c>
-      <c r="D63" s="19"/>
-      <c r="E63" s="25"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="21"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,8 +1722,8 @@
       <c r="C64" s="8">
         <v>45133</v>
       </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="25"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="21"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1736,8 +1736,8 @@
       <c r="C65" s="8">
         <v>45134</v>
       </c>
-      <c r="D65" s="19"/>
-      <c r="E65" s="25"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="21"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1750,8 +1750,8 @@
       <c r="C66" s="8">
         <v>45138</v>
       </c>
-      <c r="D66" s="19"/>
-      <c r="E66" s="25"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="21"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1764,8 +1764,8 @@
       <c r="C67" s="11">
         <v>45139</v>
       </c>
-      <c r="D67" s="19"/>
-      <c r="E67" s="25"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="21"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1778,8 +1778,8 @@
       <c r="C68" s="8">
         <v>45140</v>
       </c>
-      <c r="D68" s="19"/>
-      <c r="E68" s="25"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="21"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,8 +1792,8 @@
       <c r="C69" s="8">
         <v>45141</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="25"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="21"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1806,8 +1806,8 @@
       <c r="C70" s="8">
         <v>45146</v>
       </c>
-      <c r="D70" s="20"/>
-      <c r="E70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="21"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1820,10 +1820,10 @@
       <c r="C71" s="8">
         <v>45147</v>
       </c>
-      <c r="D71" s="18">
+      <c r="D71" s="23">
         <v>11</v>
       </c>
-      <c r="E71" s="23" t="s">
+      <c r="E71" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1838,8 +1838,8 @@
       <c r="C72" s="11">
         <v>45148</v>
       </c>
-      <c r="D72" s="19"/>
-      <c r="E72" s="25"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="21"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,8 +1852,8 @@
       <c r="C73" s="8">
         <v>45152</v>
       </c>
-      <c r="D73" s="19"/>
-      <c r="E73" s="25"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="21"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,8 +1866,8 @@
       <c r="C74" s="8">
         <v>45153</v>
       </c>
-      <c r="D74" s="19"/>
-      <c r="E74" s="25"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="21"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -1882,8 +1882,8 @@
       <c r="C75" s="8">
         <v>45154</v>
       </c>
-      <c r="D75" s="19"/>
-      <c r="E75" s="25"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="21"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1896,8 +1896,8 @@
       <c r="C76" s="8">
         <v>45155</v>
       </c>
-      <c r="D76" s="19"/>
-      <c r="E76" s="25"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="21"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1910,8 +1910,8 @@
       <c r="C77" s="8">
         <v>45160</v>
       </c>
-      <c r="D77" s="19"/>
-      <c r="E77" s="25"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="21"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1924,8 +1924,8 @@
       <c r="C78" s="8">
         <v>45161</v>
       </c>
-      <c r="D78" s="19"/>
-      <c r="E78" s="25"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="21"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -1938,8 +1938,8 @@
       <c r="C79" s="8">
         <v>45162</v>
       </c>
-      <c r="D79" s="19"/>
-      <c r="E79" s="25"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="21"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -1952,8 +1952,8 @@
       <c r="C80" s="8">
         <v>45166</v>
       </c>
-      <c r="D80" s="20"/>
-      <c r="E80" s="24"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="22"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -1966,10 +1966,10 @@
       <c r="C81" s="8">
         <v>45167</v>
       </c>
-      <c r="D81" s="21">
+      <c r="D81" s="18">
         <v>12</v>
       </c>
-      <c r="E81" s="22" t="s">
+      <c r="E81" s="19" t="s">
         <v>46</v>
       </c>
       <c r="F81" s="5"/>
@@ -1984,8 +1984,8 @@
       <c r="C82" s="8">
         <v>45168</v>
       </c>
-      <c r="D82" s="21"/>
-      <c r="E82" s="22"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="19"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,8 +1998,8 @@
       <c r="C83" s="8">
         <v>45169</v>
       </c>
-      <c r="D83" s="21"/>
-      <c r="E83" s="22"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="19"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,8 +2012,8 @@
       <c r="C84" s="8">
         <v>45173</v>
       </c>
-      <c r="D84" s="21"/>
-      <c r="E84" s="22"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="19"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,8 +2026,8 @@
       <c r="C85" s="8">
         <v>45174</v>
       </c>
-      <c r="D85" s="21"/>
-      <c r="E85" s="22"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="19"/>
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,8 +2040,8 @@
       <c r="C86" s="8">
         <v>45175</v>
       </c>
-      <c r="D86" s="21"/>
-      <c r="E86" s="22"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="19"/>
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2054,8 +2054,8 @@
       <c r="C87" s="8">
         <v>45176</v>
       </c>
-      <c r="D87" s="21"/>
-      <c r="E87" s="22"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="19"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2068,8 +2068,8 @@
       <c r="C88" s="8">
         <v>45180</v>
       </c>
-      <c r="D88" s="21"/>
-      <c r="E88" s="22"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="19"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2079,11 +2079,11 @@
       <c r="B89" s="5">
         <v>9</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C89" s="8">
         <v>45181</v>
       </c>
-      <c r="D89" s="21"/>
-      <c r="E89" s="22"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="19"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2096,8 +2096,8 @@
       <c r="C90" s="9">
         <v>45182</v>
       </c>
-      <c r="D90" s="21"/>
-      <c r="E90" s="22"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2110,8 +2110,8 @@
       <c r="C91" s="9">
         <v>45183</v>
       </c>
-      <c r="D91" s="21"/>
-      <c r="E91" s="22"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="19"/>
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,10 +2124,10 @@
       <c r="C92" s="9">
         <v>45187</v>
       </c>
-      <c r="D92" s="21">
+      <c r="D92" s="18">
         <v>13</v>
       </c>
-      <c r="E92" s="22" t="s">
+      <c r="E92" s="19" t="s">
         <v>47</v>
       </c>
       <c r="F92" s="5"/>
@@ -2142,8 +2142,8 @@
       <c r="C93" s="9">
         <v>45188</v>
       </c>
-      <c r="D93" s="21"/>
-      <c r="E93" s="22"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="19"/>
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2156,8 +2156,8 @@
       <c r="C94" s="9">
         <v>45189</v>
       </c>
-      <c r="D94" s="21"/>
-      <c r="E94" s="22"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="19"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2170,8 +2170,8 @@
       <c r="C95" s="9">
         <v>45190</v>
       </c>
-      <c r="D95" s="21"/>
-      <c r="E95" s="22"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2184,10 +2184,10 @@
       <c r="C96" s="9">
         <v>45194</v>
       </c>
-      <c r="D96" s="18">
+      <c r="D96" s="23">
         <v>14</v>
       </c>
-      <c r="E96" s="23" t="s">
+      <c r="E96" s="20" t="s">
         <v>48</v>
       </c>
       <c r="F96" s="5"/>
@@ -2202,8 +2202,8 @@
       <c r="C97" s="9">
         <v>45195</v>
       </c>
-      <c r="D97" s="19"/>
-      <c r="E97" s="25"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="21"/>
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2216,8 +2216,8 @@
       <c r="C98" s="9">
         <v>45196</v>
       </c>
-      <c r="D98" s="19"/>
-      <c r="E98" s="25"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="21"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2230,8 +2230,8 @@
       <c r="C99" s="9">
         <v>45197</v>
       </c>
-      <c r="D99" s="19"/>
-      <c r="E99" s="25"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="21"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2244,8 +2244,8 @@
       <c r="C100" s="9">
         <v>45201</v>
       </c>
-      <c r="D100" s="19"/>
-      <c r="E100" s="25"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="21"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2258,8 +2258,8 @@
       <c r="C101" s="9">
         <v>45202</v>
       </c>
-      <c r="D101" s="19"/>
-      <c r="E101" s="25"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="21"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2272,8 +2272,8 @@
       <c r="C102" s="9">
         <v>45203</v>
       </c>
-      <c r="D102" s="19"/>
-      <c r="E102" s="25"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="21"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2286,8 +2286,8 @@
       <c r="C103" s="9">
         <v>45204</v>
       </c>
-      <c r="D103" s="19"/>
-      <c r="E103" s="25"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="21"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2300,8 +2300,8 @@
       <c r="C104" s="9">
         <v>45208</v>
       </c>
-      <c r="D104" s="20"/>
-      <c r="E104" s="24"/>
+      <c r="D104" s="25"/>
+      <c r="E104" s="22"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="23" t="s">
+      <c r="E153" s="20" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2912,7 +2912,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="25"/>
+      <c r="E154" s="21"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2926,7 +2926,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="25"/>
+      <c r="E155" s="21"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2940,7 +2940,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="25"/>
+      <c r="E156" s="21"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2954,7 +2954,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="25"/>
+      <c r="E157" s="21"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -2968,7 +2968,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="25"/>
+      <c r="E158" s="21"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -2982,7 +2982,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="25"/>
+      <c r="E159" s="21"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="25"/>
+      <c r="E160" s="21"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3010,7 +3010,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="25"/>
+      <c r="E161" s="21"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="25"/>
+      <c r="E162" s="21"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3038,7 +3038,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="25"/>
+      <c r="E163" s="21"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3052,7 +3052,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="25"/>
+      <c r="E164" s="21"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="25"/>
+      <c r="E165" s="21"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="25"/>
+      <c r="E166" s="21"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3094,7 +3094,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="25"/>
+      <c r="E167" s="21"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="25"/>
+      <c r="E168" s="21"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3122,7 +3122,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="25"/>
+      <c r="E169" s="21"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="25"/>
+      <c r="E170" s="21"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3150,7 +3150,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="25"/>
+      <c r="E171" s="21"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3164,7 +3164,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="25"/>
+      <c r="E172" s="21"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3178,7 +3178,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="25"/>
+      <c r="E173" s="21"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3192,7 +3192,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="25"/>
+      <c r="E174" s="21"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3206,7 +3206,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="25"/>
+      <c r="E175" s="21"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="25"/>
+      <c r="E176" s="21"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3234,7 +3234,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="25"/>
+      <c r="E177" s="21"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3248,7 +3248,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="25"/>
+      <c r="E178" s="21"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3262,7 +3262,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="24"/>
+      <c r="E179" s="22"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3270,19 +3270,11 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="33">
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="E96:E104"/>
-    <mergeCell ref="D96:D104"/>
-    <mergeCell ref="E153:E179"/>
-    <mergeCell ref="E71:E80"/>
-    <mergeCell ref="E81:E91"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="F51:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="D71:D80"/>
+    <mergeCell ref="D81:D91"/>
+    <mergeCell ref="D30:D39"/>
+    <mergeCell ref="D40:D59"/>
+    <mergeCell ref="D60:D61"/>
     <mergeCell ref="E30:E39"/>
     <mergeCell ref="D62:D70"/>
     <mergeCell ref="D3:D4"/>
@@ -3298,11 +3290,19 @@
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="E62:E70"/>
-    <mergeCell ref="D71:D80"/>
-    <mergeCell ref="D81:D91"/>
-    <mergeCell ref="D30:D39"/>
-    <mergeCell ref="D40:D59"/>
-    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E71:E80"/>
+    <mergeCell ref="E81:E91"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="E96:E104"/>
+    <mergeCell ref="D96:D104"/>
+    <mergeCell ref="E153:E179"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ej4 extra empezado en clase
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -666,7 +666,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2093,7 @@
       <c r="B90" s="5">
         <v>10</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C90" s="8">
         <v>45182</v>
       </c>
       <c r="D90" s="18"/>

</xml_diff>

<commit_message>
herencia iniciando ejercicio 4 extra
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -325,6 +325,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -334,20 +343,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -666,7 +666,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,10 +726,10 @@
       <c r="C3" s="8">
         <v>45019</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="18">
         <v>1</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -744,8 +744,8 @@
       <c r="C4" s="8">
         <v>45020</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -760,10 +760,10 @@
       <c r="C5" s="8">
         <v>45021</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="18">
         <v>2</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="22" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -780,8 +780,8 @@
       <c r="C6" s="8">
         <v>45026</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -796,8 +796,8 @@
       <c r="C7" s="8">
         <v>45027</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -812,10 +812,10 @@
       <c r="C8" s="8">
         <v>45028</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="18">
         <v>3</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -832,8 +832,8 @@
       <c r="C9" s="8">
         <v>45029</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -848,8 +848,8 @@
       <c r="C10" s="8">
         <v>45033</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -864,8 +864,8 @@
       <c r="C11" s="8">
         <v>45034</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -900,10 +900,10 @@
       <c r="C13" s="8">
         <v>45036</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="18">
         <v>4</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="22" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -920,8 +920,8 @@
       <c r="C14" s="8">
         <v>45040</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -936,8 +936,8 @@
       <c r="C15" s="8">
         <v>45041</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -952,8 +952,8 @@
       <c r="C16" s="8">
         <v>45042</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -968,8 +968,8 @@
       <c r="C17" s="8">
         <v>45043</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="C18" s="8">
         <v>45048</v>
       </c>
-      <c r="D18" s="25"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="14" t="s">
         <v>8</v>
       </c>
@@ -1002,10 +1002,10 @@
       <c r="C19" s="8">
         <v>45049</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="18">
         <v>5</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="22" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1022,8 +1022,8 @@
       <c r="C20" s="8">
         <v>45050</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1038,8 +1038,8 @@
       <c r="C21" s="8">
         <v>45054</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1054,8 +1054,8 @@
       <c r="C22" s="8">
         <v>45055</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1070,8 +1070,8 @@
       <c r="C23" s="8">
         <v>45056</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1086,8 +1086,8 @@
       <c r="C24" s="8">
         <v>45057</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1102,8 +1102,8 @@
       <c r="C25" s="8">
         <v>45062</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1118,8 +1118,8 @@
       <c r="C26" s="8">
         <v>45062</v>
       </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="C27" s="8">
         <v>45063</v>
       </c>
-      <c r="D27" s="24"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="14" t="s">
         <v>8</v>
       </c>
@@ -1152,7 +1152,7 @@
       <c r="C28" s="8">
         <v>45064</v>
       </c>
-      <c r="D28" s="25"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="14" t="s">
         <v>9</v>
       </c>
@@ -1190,10 +1190,10 @@
       <c r="C30" s="8">
         <v>45069</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="18">
         <v>7</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1210,8 +1210,8 @@
       <c r="C31" s="8">
         <v>45070</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1226,8 +1226,8 @@
       <c r="C32" s="8">
         <v>45075</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="22"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1242,8 +1242,8 @@
       <c r="C33" s="8">
         <v>45076</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1258,8 +1258,8 @@
       <c r="C34" s="8">
         <v>45077</v>
       </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1274,8 +1274,8 @@
       <c r="C35" s="8">
         <v>45078</v>
       </c>
-      <c r="D35" s="24"/>
-      <c r="E35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1290,8 +1290,8 @@
       <c r="C36" s="8">
         <v>45082</v>
       </c>
-      <c r="D36" s="24"/>
-      <c r="E36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="22"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1306,8 +1306,8 @@
       <c r="C37" s="8">
         <v>45083</v>
       </c>
-      <c r="D37" s="24"/>
-      <c r="E37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="22"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1322,8 +1322,8 @@
       <c r="C38" s="8">
         <v>45084</v>
       </c>
-      <c r="D38" s="24"/>
-      <c r="E38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="22"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1338,8 +1338,8 @@
       <c r="C39" s="8">
         <v>45085</v>
       </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="19"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="22"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1354,10 +1354,10 @@
       <c r="C40" s="8">
         <v>45089</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="18">
         <v>8</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="22" t="s">
         <v>3</v>
       </c>
       <c r="F40" s="28" t="s">
@@ -1374,8 +1374,8 @@
       <c r="C41" s="8">
         <v>45090</v>
       </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="22"/>
       <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1388,8 +1388,8 @@
       <c r="C42" s="8">
         <v>45091</v>
       </c>
-      <c r="D42" s="24"/>
-      <c r="E42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="22"/>
       <c r="F42" s="28"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,8 +1402,8 @@
       <c r="C43" s="8">
         <v>45092</v>
       </c>
-      <c r="D43" s="24"/>
-      <c r="E43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="22"/>
       <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1416,8 +1416,8 @@
       <c r="C44" s="8">
         <v>45098</v>
       </c>
-      <c r="D44" s="24"/>
-      <c r="E44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="22"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1432,8 +1432,8 @@
       <c r="C45" s="8">
         <v>45099</v>
       </c>
-      <c r="D45" s="24"/>
-      <c r="E45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="22"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1448,8 +1448,8 @@
       <c r="C46" s="8">
         <v>45103</v>
       </c>
-      <c r="D46" s="24"/>
-      <c r="E46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="22"/>
       <c r="F46" s="28" t="s">
         <v>20</v>
       </c>
@@ -1464,8 +1464,8 @@
       <c r="C47" s="8">
         <v>45104</v>
       </c>
-      <c r="D47" s="24"/>
-      <c r="E47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="22"/>
       <c r="F47" s="28"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1478,8 +1478,8 @@
       <c r="C48" s="8">
         <v>45105</v>
       </c>
-      <c r="D48" s="24"/>
-      <c r="E48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="22"/>
       <c r="F48" s="28"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,8 +1492,8 @@
       <c r="C49" s="8">
         <v>45106</v>
       </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="22"/>
       <c r="F49" s="28"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1506,8 +1506,8 @@
       <c r="C50" s="8">
         <v>45110</v>
       </c>
-      <c r="D50" s="24"/>
-      <c r="E50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="22"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1522,8 +1522,8 @@
       <c r="C51" s="11">
         <v>45111</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="E51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="22"/>
       <c r="F51" s="29" t="s">
         <v>18</v>
       </c>
@@ -1538,8 +1538,8 @@
       <c r="C52" s="8">
         <v>45112</v>
       </c>
-      <c r="D52" s="24"/>
-      <c r="E52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="22"/>
       <c r="F52" s="29"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,8 +1552,8 @@
       <c r="C53" s="8">
         <v>45113</v>
       </c>
-      <c r="D53" s="24"/>
-      <c r="E53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="22"/>
       <c r="F53" s="29"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1566,8 +1566,8 @@
       <c r="C54" s="8">
         <v>45117</v>
       </c>
-      <c r="D54" s="24"/>
-      <c r="E54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="22"/>
       <c r="F54" s="29"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1580,8 +1580,8 @@
       <c r="C55" s="8">
         <v>45118</v>
       </c>
-      <c r="D55" s="24"/>
-      <c r="E55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="22"/>
       <c r="F55" s="28" t="s">
         <v>15</v>
       </c>
@@ -1596,8 +1596,8 @@
       <c r="C56" s="8">
         <v>45119</v>
       </c>
-      <c r="D56" s="24"/>
-      <c r="E56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="22"/>
       <c r="F56" s="28"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1610,8 +1610,8 @@
       <c r="C57" s="8">
         <v>45120</v>
       </c>
-      <c r="D57" s="24"/>
-      <c r="E57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="22"/>
       <c r="F57" s="28" t="s">
         <v>16</v>
       </c>
@@ -1626,8 +1626,8 @@
       <c r="C58" s="8">
         <v>45124</v>
       </c>
-      <c r="D58" s="24"/>
-      <c r="E58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="22"/>
       <c r="F58" s="28"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1640,8 +1640,8 @@
       <c r="C59" s="8">
         <v>45125</v>
       </c>
-      <c r="D59" s="25"/>
-      <c r="E59" s="19"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="22"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1656,10 +1656,10 @@
       <c r="C60" s="8">
         <v>45126</v>
       </c>
-      <c r="D60" s="23">
+      <c r="D60" s="18">
         <v>9</v>
       </c>
-      <c r="E60" s="20" t="s">
+      <c r="E60" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F60" s="26" t="s">
@@ -1676,8 +1676,8 @@
       <c r="C61" s="8">
         <v>45127</v>
       </c>
-      <c r="D61" s="25"/>
-      <c r="E61" s="22"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="24"/>
       <c r="F61" s="27"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1690,10 +1690,10 @@
       <c r="C62" s="8">
         <v>45131</v>
       </c>
-      <c r="D62" s="23">
+      <c r="D62" s="18">
         <v>10</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="23" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1708,8 +1708,8 @@
       <c r="C63" s="8">
         <v>45132</v>
       </c>
-      <c r="D63" s="24"/>
-      <c r="E63" s="21"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="25"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,8 +1722,8 @@
       <c r="C64" s="8">
         <v>45133</v>
       </c>
-      <c r="D64" s="24"/>
-      <c r="E64" s="21"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="25"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1736,8 +1736,8 @@
       <c r="C65" s="8">
         <v>45134</v>
       </c>
-      <c r="D65" s="24"/>
-      <c r="E65" s="21"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="25"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1750,8 +1750,8 @@
       <c r="C66" s="8">
         <v>45138</v>
       </c>
-      <c r="D66" s="24"/>
-      <c r="E66" s="21"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="25"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1764,8 +1764,8 @@
       <c r="C67" s="11">
         <v>45139</v>
       </c>
-      <c r="D67" s="24"/>
-      <c r="E67" s="21"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="25"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1778,8 +1778,8 @@
       <c r="C68" s="8">
         <v>45140</v>
       </c>
-      <c r="D68" s="24"/>
-      <c r="E68" s="21"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="25"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,8 +1792,8 @@
       <c r="C69" s="8">
         <v>45141</v>
       </c>
-      <c r="D69" s="24"/>
-      <c r="E69" s="21"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="25"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1806,8 +1806,8 @@
       <c r="C70" s="8">
         <v>45146</v>
       </c>
-      <c r="D70" s="25"/>
-      <c r="E70" s="21"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="25"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1820,10 +1820,10 @@
       <c r="C71" s="8">
         <v>45147</v>
       </c>
-      <c r="D71" s="23">
+      <c r="D71" s="18">
         <v>11</v>
       </c>
-      <c r="E71" s="20" t="s">
+      <c r="E71" s="23" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1838,8 +1838,8 @@
       <c r="C72" s="11">
         <v>45148</v>
       </c>
-      <c r="D72" s="24"/>
-      <c r="E72" s="21"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="25"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,8 +1852,8 @@
       <c r="C73" s="8">
         <v>45152</v>
       </c>
-      <c r="D73" s="24"/>
-      <c r="E73" s="21"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="25"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,8 +1866,8 @@
       <c r="C74" s="8">
         <v>45153</v>
       </c>
-      <c r="D74" s="24"/>
-      <c r="E74" s="21"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="25"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -1882,8 +1882,8 @@
       <c r="C75" s="8">
         <v>45154</v>
       </c>
-      <c r="D75" s="24"/>
-      <c r="E75" s="21"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="25"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1896,8 +1896,8 @@
       <c r="C76" s="8">
         <v>45155</v>
       </c>
-      <c r="D76" s="24"/>
-      <c r="E76" s="21"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="25"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1910,8 +1910,8 @@
       <c r="C77" s="8">
         <v>45160</v>
       </c>
-      <c r="D77" s="24"/>
-      <c r="E77" s="21"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="25"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1924,8 +1924,8 @@
       <c r="C78" s="8">
         <v>45161</v>
       </c>
-      <c r="D78" s="24"/>
-      <c r="E78" s="21"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="25"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -1938,8 +1938,8 @@
       <c r="C79" s="8">
         <v>45162</v>
       </c>
-      <c r="D79" s="24"/>
-      <c r="E79" s="21"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="25"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -1952,8 +1952,8 @@
       <c r="C80" s="8">
         <v>45166</v>
       </c>
-      <c r="D80" s="25"/>
-      <c r="E80" s="22"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="24"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -1966,10 +1966,10 @@
       <c r="C81" s="8">
         <v>45167</v>
       </c>
-      <c r="D81" s="18">
+      <c r="D81" s="21">
         <v>12</v>
       </c>
-      <c r="E81" s="19" t="s">
+      <c r="E81" s="22" t="s">
         <v>46</v>
       </c>
       <c r="F81" s="5"/>
@@ -1984,8 +1984,8 @@
       <c r="C82" s="8">
         <v>45168</v>
       </c>
-      <c r="D82" s="18"/>
-      <c r="E82" s="19"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="22"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,8 +1998,8 @@
       <c r="C83" s="8">
         <v>45169</v>
       </c>
-      <c r="D83" s="18"/>
-      <c r="E83" s="19"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="22"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,8 +2012,8 @@
       <c r="C84" s="8">
         <v>45173</v>
       </c>
-      <c r="D84" s="18"/>
-      <c r="E84" s="19"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="22"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,8 +2026,8 @@
       <c r="C85" s="8">
         <v>45174</v>
       </c>
-      <c r="D85" s="18"/>
-      <c r="E85" s="19"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="22"/>
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,8 +2040,8 @@
       <c r="C86" s="8">
         <v>45175</v>
       </c>
-      <c r="D86" s="18"/>
-      <c r="E86" s="19"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="22"/>
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2054,8 +2054,8 @@
       <c r="C87" s="8">
         <v>45176</v>
       </c>
-      <c r="D87" s="18"/>
-      <c r="E87" s="19"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="22"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2068,8 +2068,8 @@
       <c r="C88" s="8">
         <v>45180</v>
       </c>
-      <c r="D88" s="18"/>
-      <c r="E88" s="19"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="22"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,8 +2082,8 @@
       <c r="C89" s="8">
         <v>45181</v>
       </c>
-      <c r="D89" s="18"/>
-      <c r="E89" s="19"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="22"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2096,8 +2096,8 @@
       <c r="C90" s="8">
         <v>45182</v>
       </c>
-      <c r="D90" s="18"/>
-      <c r="E90" s="19"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="22"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,11 +2107,11 @@
       <c r="B91" s="17">
         <v>11</v>
       </c>
-      <c r="C91" s="9">
+      <c r="C91" s="8">
         <v>45183</v>
       </c>
-      <c r="D91" s="18"/>
-      <c r="E91" s="19"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="22"/>
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,10 +2124,10 @@
       <c r="C92" s="9">
         <v>45187</v>
       </c>
-      <c r="D92" s="18">
+      <c r="D92" s="21">
         <v>13</v>
       </c>
-      <c r="E92" s="19" t="s">
+      <c r="E92" s="22" t="s">
         <v>47</v>
       </c>
       <c r="F92" s="5"/>
@@ -2142,8 +2142,8 @@
       <c r="C93" s="9">
         <v>45188</v>
       </c>
-      <c r="D93" s="18"/>
-      <c r="E93" s="19"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="22"/>
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2156,8 +2156,8 @@
       <c r="C94" s="9">
         <v>45189</v>
       </c>
-      <c r="D94" s="18"/>
-      <c r="E94" s="19"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="22"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2170,8 +2170,8 @@
       <c r="C95" s="9">
         <v>45190</v>
       </c>
-      <c r="D95" s="18"/>
-      <c r="E95" s="19"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="22"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2184,10 +2184,10 @@
       <c r="C96" s="9">
         <v>45194</v>
       </c>
-      <c r="D96" s="23">
+      <c r="D96" s="18">
         <v>14</v>
       </c>
-      <c r="E96" s="20" t="s">
+      <c r="E96" s="23" t="s">
         <v>48</v>
       </c>
       <c r="F96" s="5"/>
@@ -2202,8 +2202,8 @@
       <c r="C97" s="9">
         <v>45195</v>
       </c>
-      <c r="D97" s="24"/>
-      <c r="E97" s="21"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="25"/>
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2216,8 +2216,8 @@
       <c r="C98" s="9">
         <v>45196</v>
       </c>
-      <c r="D98" s="24"/>
-      <c r="E98" s="21"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="25"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2230,8 +2230,8 @@
       <c r="C99" s="9">
         <v>45197</v>
       </c>
-      <c r="D99" s="24"/>
-      <c r="E99" s="21"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="25"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2244,8 +2244,8 @@
       <c r="C100" s="9">
         <v>45201</v>
       </c>
-      <c r="D100" s="24"/>
-      <c r="E100" s="21"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="25"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2258,8 +2258,8 @@
       <c r="C101" s="9">
         <v>45202</v>
       </c>
-      <c r="D101" s="24"/>
-      <c r="E101" s="21"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="25"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2272,8 +2272,8 @@
       <c r="C102" s="9">
         <v>45203</v>
       </c>
-      <c r="D102" s="24"/>
-      <c r="E102" s="21"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="25"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2286,8 +2286,8 @@
       <c r="C103" s="9">
         <v>45204</v>
       </c>
-      <c r="D103" s="24"/>
-      <c r="E103" s="21"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="25"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2300,8 +2300,8 @@
       <c r="C104" s="9">
         <v>45208</v>
       </c>
-      <c r="D104" s="25"/>
-      <c r="E104" s="22"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="24"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="20" t="s">
+      <c r="E153" s="23" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2912,7 +2912,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="21"/>
+      <c r="E154" s="25"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2926,7 +2926,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="21"/>
+      <c r="E155" s="25"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2940,7 +2940,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="21"/>
+      <c r="E156" s="25"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2954,7 +2954,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="21"/>
+      <c r="E157" s="25"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -2968,7 +2968,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="21"/>
+      <c r="E158" s="25"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -2982,7 +2982,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="21"/>
+      <c r="E159" s="25"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="21"/>
+      <c r="E160" s="25"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3010,7 +3010,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="21"/>
+      <c r="E161" s="25"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="21"/>
+      <c r="E162" s="25"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3038,7 +3038,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="21"/>
+      <c r="E163" s="25"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3052,7 +3052,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="21"/>
+      <c r="E164" s="25"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="21"/>
+      <c r="E165" s="25"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="21"/>
+      <c r="E166" s="25"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3094,7 +3094,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="21"/>
+      <c r="E167" s="25"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="21"/>
+      <c r="E168" s="25"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3122,7 +3122,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="21"/>
+      <c r="E169" s="25"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="21"/>
+      <c r="E170" s="25"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3150,7 +3150,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="21"/>
+      <c r="E171" s="25"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3164,7 +3164,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="21"/>
+      <c r="E172" s="25"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3178,7 +3178,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="21"/>
+      <c r="E173" s="25"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3192,7 +3192,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="21"/>
+      <c r="E174" s="25"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3206,7 +3206,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="21"/>
+      <c r="E175" s="25"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="21"/>
+      <c r="E176" s="25"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3234,7 +3234,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="21"/>
+      <c r="E177" s="25"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3248,7 +3248,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="21"/>
+      <c r="E178" s="25"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3262,7 +3262,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="22"/>
+      <c r="E179" s="24"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3270,11 +3270,19 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="33">
-    <mergeCell ref="D71:D80"/>
-    <mergeCell ref="D81:D91"/>
-    <mergeCell ref="D30:D39"/>
-    <mergeCell ref="D40:D59"/>
-    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="E96:E104"/>
+    <mergeCell ref="D96:D104"/>
+    <mergeCell ref="E153:E179"/>
+    <mergeCell ref="E71:E80"/>
+    <mergeCell ref="E81:E91"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F57:F58"/>
     <mergeCell ref="E30:E39"/>
     <mergeCell ref="D62:D70"/>
     <mergeCell ref="D3:D4"/>
@@ -3290,19 +3298,11 @@
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="E62:E70"/>
-    <mergeCell ref="E71:E80"/>
-    <mergeCell ref="E81:E91"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="F51:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="E96:E104"/>
-    <mergeCell ref="D96:D104"/>
-    <mergeCell ref="E153:E179"/>
+    <mergeCell ref="D71:D80"/>
+    <mergeCell ref="D81:D91"/>
+    <mergeCell ref="D30:D39"/>
+    <mergeCell ref="D40:D59"/>
+    <mergeCell ref="D60:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
sql ej extra 2 avanzando
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -332,6 +332,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -341,20 +350,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -673,7 +673,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
+      <selection pane="bottomLeft" activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,10 +733,10 @@
       <c r="C3" s="8">
         <v>45019</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="19">
         <v>1</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -751,8 +751,8 @@
       <c r="C4" s="8">
         <v>45020</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -767,10 +767,10 @@
       <c r="C5" s="8">
         <v>45021</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="19">
         <v>2</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -787,8 +787,8 @@
       <c r="C6" s="8">
         <v>45026</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -803,8 +803,8 @@
       <c r="C7" s="8">
         <v>45027</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -819,10 +819,10 @@
       <c r="C8" s="8">
         <v>45028</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="19">
         <v>3</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -839,8 +839,8 @@
       <c r="C9" s="8">
         <v>45029</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -855,8 +855,8 @@
       <c r="C10" s="8">
         <v>45033</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -871,8 +871,8 @@
       <c r="C11" s="8">
         <v>45034</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -907,10 +907,10 @@
       <c r="C13" s="8">
         <v>45036</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="19">
         <v>4</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -927,8 +927,8 @@
       <c r="C14" s="8">
         <v>45040</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -943,8 +943,8 @@
       <c r="C15" s="8">
         <v>45041</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -959,8 +959,8 @@
       <c r="C16" s="8">
         <v>45042</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -975,8 +975,8 @@
       <c r="C17" s="8">
         <v>45043</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -991,7 +991,7 @@
       <c r="C18" s="8">
         <v>45048</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="14" t="s">
         <v>8</v>
       </c>
@@ -1009,10 +1009,10 @@
       <c r="C19" s="8">
         <v>45049</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="19">
         <v>5</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1029,8 +1029,8 @@
       <c r="C20" s="8">
         <v>45050</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1045,8 +1045,8 @@
       <c r="C21" s="8">
         <v>45054</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1061,8 +1061,8 @@
       <c r="C22" s="8">
         <v>45055</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1077,8 +1077,8 @@
       <c r="C23" s="8">
         <v>45056</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1093,8 +1093,8 @@
       <c r="C24" s="8">
         <v>45057</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1109,8 +1109,8 @@
       <c r="C25" s="8">
         <v>45062</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1125,8 +1125,8 @@
       <c r="C26" s="8">
         <v>45062</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="C27" s="8">
         <v>45063</v>
       </c>
-      <c r="D27" s="25"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="14" t="s">
         <v>8</v>
       </c>
@@ -1159,7 +1159,7 @@
       <c r="C28" s="8">
         <v>45064</v>
       </c>
-      <c r="D28" s="26"/>
+      <c r="D28" s="21"/>
       <c r="E28" s="14" t="s">
         <v>9</v>
       </c>
@@ -1197,10 +1197,10 @@
       <c r="C30" s="8">
         <v>45069</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="19">
         <v>7</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="23" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1217,8 +1217,8 @@
       <c r="C31" s="8">
         <v>45070</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1233,8 +1233,8 @@
       <c r="C32" s="8">
         <v>45075</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1249,8 +1249,8 @@
       <c r="C33" s="8">
         <v>45076</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1265,8 +1265,8 @@
       <c r="C34" s="8">
         <v>45077</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1281,8 +1281,8 @@
       <c r="C35" s="8">
         <v>45078</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="23"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1297,8 +1297,8 @@
       <c r="C36" s="8">
         <v>45082</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1313,8 +1313,8 @@
       <c r="C37" s="8">
         <v>45083</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1329,8 +1329,8 @@
       <c r="C38" s="8">
         <v>45084</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1345,8 +1345,8 @@
       <c r="C39" s="8">
         <v>45085</v>
       </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="20"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="23"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1361,10 +1361,10 @@
       <c r="C40" s="8">
         <v>45089</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D40" s="19">
         <v>8</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F40" s="29" t="s">
@@ -1381,8 +1381,8 @@
       <c r="C41" s="8">
         <v>45090</v>
       </c>
-      <c r="D41" s="25"/>
-      <c r="E41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1395,8 +1395,8 @@
       <c r="C42" s="8">
         <v>45091</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="29"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1409,8 +1409,8 @@
       <c r="C43" s="8">
         <v>45092</v>
       </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="23"/>
       <c r="F43" s="29"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1423,8 +1423,8 @@
       <c r="C44" s="8">
         <v>45098</v>
       </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1439,8 +1439,8 @@
       <c r="C45" s="8">
         <v>45099</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="23"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1455,8 +1455,8 @@
       <c r="C46" s="8">
         <v>45103</v>
       </c>
-      <c r="D46" s="25"/>
-      <c r="E46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="29" t="s">
         <v>20</v>
       </c>
@@ -1471,8 +1471,8 @@
       <c r="C47" s="8">
         <v>45104</v>
       </c>
-      <c r="D47" s="25"/>
-      <c r="E47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="23"/>
       <c r="F47" s="29"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,8 +1485,8 @@
       <c r="C48" s="8">
         <v>45105</v>
       </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="23"/>
       <c r="F48" s="29"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1499,8 +1499,8 @@
       <c r="C49" s="8">
         <v>45106</v>
       </c>
-      <c r="D49" s="25"/>
-      <c r="E49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="23"/>
       <c r="F49" s="29"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1513,8 +1513,8 @@
       <c r="C50" s="8">
         <v>45110</v>
       </c>
-      <c r="D50" s="25"/>
-      <c r="E50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="23"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1529,8 +1529,8 @@
       <c r="C51" s="11">
         <v>45111</v>
       </c>
-      <c r="D51" s="25"/>
-      <c r="E51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="23"/>
       <c r="F51" s="30" t="s">
         <v>18</v>
       </c>
@@ -1545,8 +1545,8 @@
       <c r="C52" s="8">
         <v>45112</v>
       </c>
-      <c r="D52" s="25"/>
-      <c r="E52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="23"/>
       <c r="F52" s="30"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1559,8 +1559,8 @@
       <c r="C53" s="8">
         <v>45113</v>
       </c>
-      <c r="D53" s="25"/>
-      <c r="E53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="23"/>
       <c r="F53" s="30"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1573,8 +1573,8 @@
       <c r="C54" s="8">
         <v>45117</v>
       </c>
-      <c r="D54" s="25"/>
-      <c r="E54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="23"/>
       <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,8 +1587,8 @@
       <c r="C55" s="8">
         <v>45118</v>
       </c>
-      <c r="D55" s="25"/>
-      <c r="E55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="23"/>
       <c r="F55" s="29" t="s">
         <v>15</v>
       </c>
@@ -1603,8 +1603,8 @@
       <c r="C56" s="8">
         <v>45119</v>
       </c>
-      <c r="D56" s="25"/>
-      <c r="E56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="23"/>
       <c r="F56" s="29"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1617,8 +1617,8 @@
       <c r="C57" s="8">
         <v>45120</v>
       </c>
-      <c r="D57" s="25"/>
-      <c r="E57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="23"/>
       <c r="F57" s="29" t="s">
         <v>16</v>
       </c>
@@ -1633,8 +1633,8 @@
       <c r="C58" s="8">
         <v>45124</v>
       </c>
-      <c r="D58" s="25"/>
-      <c r="E58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="23"/>
       <c r="F58" s="29"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1647,8 +1647,8 @@
       <c r="C59" s="8">
         <v>45125</v>
       </c>
-      <c r="D59" s="26"/>
-      <c r="E59" s="20"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="23"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1663,10 +1663,10 @@
       <c r="C60" s="8">
         <v>45126</v>
       </c>
-      <c r="D60" s="24">
+      <c r="D60" s="19">
         <v>9</v>
       </c>
-      <c r="E60" s="21" t="s">
+      <c r="E60" s="24" t="s">
         <v>41</v>
       </c>
       <c r="F60" s="27" t="s">
@@ -1683,8 +1683,8 @@
       <c r="C61" s="8">
         <v>45127</v>
       </c>
-      <c r="D61" s="26"/>
-      <c r="E61" s="23"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="25"/>
       <c r="F61" s="28"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1697,10 +1697,10 @@
       <c r="C62" s="8">
         <v>45131</v>
       </c>
-      <c r="D62" s="24">
+      <c r="D62" s="19">
         <v>10</v>
       </c>
-      <c r="E62" s="21" t="s">
+      <c r="E62" s="24" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1715,8 +1715,8 @@
       <c r="C63" s="8">
         <v>45132</v>
       </c>
-      <c r="D63" s="25"/>
-      <c r="E63" s="22"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="26"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1729,8 +1729,8 @@
       <c r="C64" s="8">
         <v>45133</v>
       </c>
-      <c r="D64" s="25"/>
-      <c r="E64" s="22"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="26"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1743,8 +1743,8 @@
       <c r="C65" s="8">
         <v>45134</v>
       </c>
-      <c r="D65" s="25"/>
-      <c r="E65" s="22"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="26"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,8 +1757,8 @@
       <c r="C66" s="8">
         <v>45138</v>
       </c>
-      <c r="D66" s="25"/>
-      <c r="E66" s="22"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="26"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1771,8 +1771,8 @@
       <c r="C67" s="11">
         <v>45139</v>
       </c>
-      <c r="D67" s="25"/>
-      <c r="E67" s="22"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="26"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1785,8 +1785,8 @@
       <c r="C68" s="8">
         <v>45140</v>
       </c>
-      <c r="D68" s="25"/>
-      <c r="E68" s="22"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="26"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1799,8 +1799,8 @@
       <c r="C69" s="8">
         <v>45141</v>
       </c>
-      <c r="D69" s="25"/>
-      <c r="E69" s="22"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="26"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1813,8 +1813,8 @@
       <c r="C70" s="8">
         <v>45146</v>
       </c>
-      <c r="D70" s="26"/>
-      <c r="E70" s="22"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="26"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1827,10 +1827,10 @@
       <c r="C71" s="8">
         <v>45147</v>
       </c>
-      <c r="D71" s="24">
+      <c r="D71" s="19">
         <v>11</v>
       </c>
-      <c r="E71" s="21" t="s">
+      <c r="E71" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1845,8 +1845,8 @@
       <c r="C72" s="11">
         <v>45148</v>
       </c>
-      <c r="D72" s="25"/>
-      <c r="E72" s="22"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="26"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1859,8 +1859,8 @@
       <c r="C73" s="8">
         <v>45152</v>
       </c>
-      <c r="D73" s="25"/>
-      <c r="E73" s="22"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="26"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1873,8 +1873,8 @@
       <c r="C74" s="8">
         <v>45153</v>
       </c>
-      <c r="D74" s="25"/>
-      <c r="E74" s="22"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="26"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -1889,8 +1889,8 @@
       <c r="C75" s="8">
         <v>45154</v>
       </c>
-      <c r="D75" s="25"/>
-      <c r="E75" s="22"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="26"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1903,8 +1903,8 @@
       <c r="C76" s="8">
         <v>45155</v>
       </c>
-      <c r="D76" s="25"/>
-      <c r="E76" s="22"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="26"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,8 +1917,8 @@
       <c r="C77" s="8">
         <v>45160</v>
       </c>
-      <c r="D77" s="25"/>
-      <c r="E77" s="22"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="26"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1931,8 +1931,8 @@
       <c r="C78" s="8">
         <v>45161</v>
       </c>
-      <c r="D78" s="25"/>
-      <c r="E78" s="22"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="26"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -1945,8 +1945,8 @@
       <c r="C79" s="8">
         <v>45162</v>
       </c>
-      <c r="D79" s="25"/>
-      <c r="E79" s="22"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="26"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -1959,8 +1959,8 @@
       <c r="C80" s="8">
         <v>45166</v>
       </c>
-      <c r="D80" s="26"/>
-      <c r="E80" s="23"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="25"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -1973,10 +1973,10 @@
       <c r="C81" s="8">
         <v>45167</v>
       </c>
-      <c r="D81" s="19">
+      <c r="D81" s="22">
         <v>12</v>
       </c>
-      <c r="E81" s="20" t="s">
+      <c r="E81" s="23" t="s">
         <v>46</v>
       </c>
       <c r="F81" s="5"/>
@@ -1991,8 +1991,8 @@
       <c r="C82" s="8">
         <v>45168</v>
       </c>
-      <c r="D82" s="19"/>
-      <c r="E82" s="20"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="23"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2005,8 +2005,8 @@
       <c r="C83" s="8">
         <v>45169</v>
       </c>
-      <c r="D83" s="19"/>
-      <c r="E83" s="20"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="23"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,8 +2019,8 @@
       <c r="C84" s="8">
         <v>45173</v>
       </c>
-      <c r="D84" s="19"/>
-      <c r="E84" s="20"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="23"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2033,8 +2033,8 @@
       <c r="C85" s="8">
         <v>45174</v>
       </c>
-      <c r="D85" s="19"/>
-      <c r="E85" s="20"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="23"/>
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2047,8 +2047,8 @@
       <c r="C86" s="8">
         <v>45175</v>
       </c>
-      <c r="D86" s="19"/>
-      <c r="E86" s="20"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="23"/>
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2061,8 +2061,8 @@
       <c r="C87" s="8">
         <v>45176</v>
       </c>
-      <c r="D87" s="19"/>
-      <c r="E87" s="20"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="23"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2075,8 +2075,8 @@
       <c r="C88" s="8">
         <v>45180</v>
       </c>
-      <c r="D88" s="19"/>
-      <c r="E88" s="20"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="23"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2089,8 +2089,8 @@
       <c r="C89" s="8">
         <v>45181</v>
       </c>
-      <c r="D89" s="19"/>
-      <c r="E89" s="20"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="23"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2103,8 +2103,8 @@
       <c r="C90" s="8">
         <v>45182</v>
       </c>
-      <c r="D90" s="19"/>
-      <c r="E90" s="20"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="23"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2117,8 +2117,8 @@
       <c r="C91" s="8">
         <v>45183</v>
       </c>
-      <c r="D91" s="19"/>
-      <c r="E91" s="20"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="23"/>
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2131,10 +2131,10 @@
       <c r="C92" s="8">
         <v>45187</v>
       </c>
-      <c r="D92" s="19">
+      <c r="D92" s="22">
         <v>13</v>
       </c>
-      <c r="E92" s="20" t="s">
+      <c r="E92" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F92" s="5"/>
@@ -2149,8 +2149,8 @@
       <c r="C93" s="8">
         <v>45188</v>
       </c>
-      <c r="D93" s="19"/>
-      <c r="E93" s="20"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="23"/>
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2163,8 +2163,8 @@
       <c r="C94" s="8">
         <v>45189</v>
       </c>
-      <c r="D94" s="19"/>
-      <c r="E94" s="20"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="23"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2177,8 +2177,8 @@
       <c r="C95" s="8">
         <v>45190</v>
       </c>
-      <c r="D95" s="19"/>
-      <c r="E95" s="20"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="23"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2191,10 +2191,10 @@
       <c r="C96" s="8">
         <v>45194</v>
       </c>
-      <c r="D96" s="24">
+      <c r="D96" s="19">
         <v>14</v>
       </c>
-      <c r="E96" s="21" t="s">
+      <c r="E96" s="24" t="s">
         <v>48</v>
       </c>
       <c r="F96" s="5"/>
@@ -2209,8 +2209,8 @@
       <c r="C97" s="8">
         <v>45195</v>
       </c>
-      <c r="D97" s="25"/>
-      <c r="E97" s="22"/>
+      <c r="D97" s="20"/>
+      <c r="E97" s="26"/>
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2223,8 +2223,8 @@
       <c r="C98" s="11">
         <v>45196</v>
       </c>
-      <c r="D98" s="25"/>
-      <c r="E98" s="22"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="26"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,8 +2237,8 @@
       <c r="C99" s="8">
         <v>45197</v>
       </c>
-      <c r="D99" s="25"/>
-      <c r="E99" s="22"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="26"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2251,8 +2251,8 @@
       <c r="C100" s="8">
         <v>45201</v>
       </c>
-      <c r="D100" s="25"/>
-      <c r="E100" s="22"/>
+      <c r="D100" s="20"/>
+      <c r="E100" s="26"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2265,8 +2265,8 @@
       <c r="C101" s="8">
         <v>45202</v>
       </c>
-      <c r="D101" s="25"/>
-      <c r="E101" s="22"/>
+      <c r="D101" s="20"/>
+      <c r="E101" s="26"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2279,8 +2279,8 @@
       <c r="C102" s="8">
         <v>45203</v>
       </c>
-      <c r="D102" s="25"/>
-      <c r="E102" s="22"/>
+      <c r="D102" s="20"/>
+      <c r="E102" s="26"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2293,8 +2293,8 @@
       <c r="C103" s="8">
         <v>45204</v>
       </c>
-      <c r="D103" s="25"/>
-      <c r="E103" s="22"/>
+      <c r="D103" s="20"/>
+      <c r="E103" s="26"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2304,11 +2304,11 @@
       <c r="B104" s="5">
         <v>9</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C104" s="8">
         <v>45208</v>
       </c>
-      <c r="D104" s="26"/>
-      <c r="E104" s="23"/>
+      <c r="D104" s="21"/>
+      <c r="E104" s="25"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="21" t="s">
+      <c r="E153" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2921,7 +2921,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="22"/>
+      <c r="E154" s="26"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="22"/>
+      <c r="E155" s="26"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2949,7 +2949,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="22"/>
+      <c r="E156" s="26"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -2963,7 +2963,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="22"/>
+      <c r="E157" s="26"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -2977,7 +2977,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="22"/>
+      <c r="E158" s="26"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -2991,7 +2991,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="22"/>
+      <c r="E159" s="26"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3005,7 +3005,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="22"/>
+      <c r="E160" s="26"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3019,7 +3019,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="22"/>
+      <c r="E161" s="26"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="22"/>
+      <c r="E162" s="26"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="22"/>
+      <c r="E163" s="26"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="22"/>
+      <c r="E164" s="26"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3075,7 +3075,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="22"/>
+      <c r="E165" s="26"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3089,7 +3089,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="22"/>
+      <c r="E166" s="26"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3103,7 +3103,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="22"/>
+      <c r="E167" s="26"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3117,7 +3117,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="22"/>
+      <c r="E168" s="26"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="22"/>
+      <c r="E169" s="26"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3145,7 +3145,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="22"/>
+      <c r="E170" s="26"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3159,7 +3159,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="22"/>
+      <c r="E171" s="26"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3173,7 +3173,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="22"/>
+      <c r="E172" s="26"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3187,7 +3187,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="22"/>
+      <c r="E173" s="26"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3201,7 +3201,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="22"/>
+      <c r="E174" s="26"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3215,7 +3215,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="22"/>
+      <c r="E175" s="26"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3229,7 +3229,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="22"/>
+      <c r="E176" s="26"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3243,7 +3243,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="22"/>
+      <c r="E177" s="26"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3257,7 +3257,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="22"/>
+      <c r="E178" s="26"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3271,7 +3271,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="23"/>
+      <c r="E179" s="25"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3279,11 +3279,19 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="33">
-    <mergeCell ref="D71:D80"/>
-    <mergeCell ref="D81:D91"/>
-    <mergeCell ref="D30:D39"/>
-    <mergeCell ref="D40:D59"/>
-    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="E96:E104"/>
+    <mergeCell ref="D96:D104"/>
+    <mergeCell ref="E153:E179"/>
+    <mergeCell ref="E71:E80"/>
+    <mergeCell ref="E81:E91"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F57:F58"/>
     <mergeCell ref="E30:E39"/>
     <mergeCell ref="D62:D70"/>
     <mergeCell ref="D3:D4"/>
@@ -3299,19 +3307,11 @@
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="E62:E70"/>
-    <mergeCell ref="E71:E80"/>
-    <mergeCell ref="E81:E91"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="F51:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="E96:E104"/>
-    <mergeCell ref="D96:D104"/>
-    <mergeCell ref="E153:E179"/>
+    <mergeCell ref="D71:D80"/>
+    <mergeCell ref="D81:D91"/>
+    <mergeCell ref="D30:D39"/>
+    <mergeCell ref="D40:D59"/>
+    <mergeCell ref="D60:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ejercicio 1 - cerebro derretido
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Fecha</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>JDBC</t>
+  </si>
+  <si>
+    <t>JPA</t>
   </si>
 </sst>
 </file>
@@ -676,7 +679,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E106" sqref="E106:E109"/>
+      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,7 +2342,7 @@
       <c r="B106" s="5">
         <v>1</v>
       </c>
-      <c r="C106" s="9">
+      <c r="C106" s="8">
         <v>45210</v>
       </c>
       <c r="D106" s="19">
@@ -2357,7 +2360,7 @@
       <c r="B107" s="5">
         <v>2</v>
       </c>
-      <c r="C107" s="9">
+      <c r="C107" s="8">
         <v>45211</v>
       </c>
       <c r="D107" s="20"/>
@@ -2371,7 +2374,7 @@
       <c r="B108" s="5">
         <v>3</v>
       </c>
-      <c r="C108" s="9">
+      <c r="C108" s="8">
         <v>45216</v>
       </c>
       <c r="D108" s="20"/>
@@ -2385,7 +2388,7 @@
       <c r="B109" s="5">
         <v>4</v>
       </c>
-      <c r="C109" s="9">
+      <c r="C109" s="8">
         <v>45217</v>
       </c>
       <c r="D109" s="21"/>
@@ -2396,12 +2399,18 @@
       <c r="A110" s="5">
         <v>109</v>
       </c>
-      <c r="B110" s="5"/>
+      <c r="B110" s="5">
+        <v>1</v>
+      </c>
       <c r="C110" s="9">
         <v>45218</v>
       </c>
-      <c r="D110" s="6"/>
-      <c r="E110" s="14"/>
+      <c r="D110" s="6">
+        <v>16</v>
+      </c>
+      <c r="E110" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="F110" s="5"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
jpa masterclass juan manuel
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Fecha</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>JPA</t>
+  </si>
+  <si>
+    <t>Masterclass con JuanMa a las 20:00 hs.</t>
+  </si>
+  <si>
+    <t>Sprint</t>
   </si>
 </sst>
 </file>
@@ -338,15 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,11 +353,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -679,7 +685,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C119" sqref="C119"/>
+      <selection pane="bottomLeft" activeCell="E119" sqref="E119:E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,10 +745,10 @@
       <c r="C3" s="8">
         <v>45019</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="24">
         <v>1</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -757,8 +763,8 @@
       <c r="C4" s="8">
         <v>45020</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -773,10 +779,10 @@
       <c r="C5" s="8">
         <v>45021</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="24">
         <v>2</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -793,8 +799,8 @@
       <c r="C6" s="8">
         <v>45026</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -809,8 +815,8 @@
       <c r="C7" s="8">
         <v>45027</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -825,10 +831,10 @@
       <c r="C8" s="8">
         <v>45028</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="24">
         <v>3</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -845,8 +851,8 @@
       <c r="C9" s="8">
         <v>45029</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -861,8 +867,8 @@
       <c r="C10" s="8">
         <v>45033</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -877,8 +883,8 @@
       <c r="C11" s="8">
         <v>45034</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="23"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -913,10 +919,10 @@
       <c r="C13" s="8">
         <v>45036</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="24">
         <v>4</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="20" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -933,8 +939,8 @@
       <c r="C14" s="8">
         <v>45040</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="23"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -949,8 +955,8 @@
       <c r="C15" s="8">
         <v>45041</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="23"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -965,8 +971,8 @@
       <c r="C16" s="8">
         <v>45042</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="23"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -981,8 +987,8 @@
       <c r="C17" s="8">
         <v>45043</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -997,7 +1003,7 @@
       <c r="C18" s="8">
         <v>45048</v>
       </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="26"/>
       <c r="E18" s="14" t="s">
         <v>8</v>
       </c>
@@ -1015,10 +1021,10 @@
       <c r="C19" s="8">
         <v>45049</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="24">
         <v>5</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="20" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1035,8 +1041,8 @@
       <c r="C20" s="8">
         <v>45050</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1051,8 +1057,8 @@
       <c r="C21" s="8">
         <v>45054</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="23"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1067,8 +1073,8 @@
       <c r="C22" s="8">
         <v>45055</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="23"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1083,8 +1089,8 @@
       <c r="C23" s="8">
         <v>45056</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="23"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1099,8 +1105,8 @@
       <c r="C24" s="8">
         <v>45057</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="23"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1115,8 +1121,8 @@
       <c r="C25" s="8">
         <v>45062</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="23"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1131,8 +1137,8 @@
       <c r="C26" s="8">
         <v>45062</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="23"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="20"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1147,7 +1153,7 @@
       <c r="C27" s="8">
         <v>45063</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="14" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1171,7 @@
       <c r="C28" s="8">
         <v>45064</v>
       </c>
-      <c r="D28" s="21"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="14" t="s">
         <v>9</v>
       </c>
@@ -1203,10 +1209,10 @@
       <c r="C30" s="8">
         <v>45069</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="24">
         <v>7</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="20" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1223,8 +1229,8 @@
       <c r="C31" s="8">
         <v>45070</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="23"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1239,8 +1245,8 @@
       <c r="C32" s="8">
         <v>45075</v>
       </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="23"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1255,8 +1261,8 @@
       <c r="C33" s="8">
         <v>45076</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="23"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="20"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1271,8 +1277,8 @@
       <c r="C34" s="8">
         <v>45077</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="23"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1287,8 +1293,8 @@
       <c r="C35" s="8">
         <v>45078</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="23"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="20"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1303,8 +1309,8 @@
       <c r="C36" s="8">
         <v>45082</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="23"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="20"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1319,8 +1325,8 @@
       <c r="C37" s="8">
         <v>45083</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="23"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1335,8 +1341,8 @@
       <c r="C38" s="8">
         <v>45084</v>
       </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="23"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1351,8 +1357,8 @@
       <c r="C39" s="8">
         <v>45085</v>
       </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="23"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="20"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1367,10 +1373,10 @@
       <c r="C40" s="8">
         <v>45089</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="24">
         <v>8</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="20" t="s">
         <v>3</v>
       </c>
       <c r="F40" s="29" t="s">
@@ -1387,8 +1393,8 @@
       <c r="C41" s="8">
         <v>45090</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="23"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="20"/>
       <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1401,8 +1407,8 @@
       <c r="C42" s="8">
         <v>45091</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="23"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="20"/>
       <c r="F42" s="29"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1415,8 +1421,8 @@
       <c r="C43" s="8">
         <v>45092</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="23"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="20"/>
       <c r="F43" s="29"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1429,8 +1435,8 @@
       <c r="C44" s="8">
         <v>45098</v>
       </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="23"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="20"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1445,8 +1451,8 @@
       <c r="C45" s="8">
         <v>45099</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="23"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1461,8 +1467,8 @@
       <c r="C46" s="8">
         <v>45103</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="23"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="20"/>
       <c r="F46" s="29" t="s">
         <v>20</v>
       </c>
@@ -1477,8 +1483,8 @@
       <c r="C47" s="8">
         <v>45104</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="23"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="20"/>
       <c r="F47" s="29"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1491,8 +1497,8 @@
       <c r="C48" s="8">
         <v>45105</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="23"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="20"/>
       <c r="F48" s="29"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,8 +1511,8 @@
       <c r="C49" s="8">
         <v>45106</v>
       </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="23"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="20"/>
       <c r="F49" s="29"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1519,8 +1525,8 @@
       <c r="C50" s="8">
         <v>45110</v>
       </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="23"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="20"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1535,8 +1541,8 @@
       <c r="C51" s="11">
         <v>45111</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="23"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="20"/>
       <c r="F51" s="30" t="s">
         <v>18</v>
       </c>
@@ -1551,8 +1557,8 @@
       <c r="C52" s="8">
         <v>45112</v>
       </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="23"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="20"/>
       <c r="F52" s="30"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1565,8 +1571,8 @@
       <c r="C53" s="8">
         <v>45113</v>
       </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="23"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="20"/>
       <c r="F53" s="30"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1579,8 +1585,8 @@
       <c r="C54" s="8">
         <v>45117</v>
       </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="23"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="20"/>
       <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1593,8 +1599,8 @@
       <c r="C55" s="8">
         <v>45118</v>
       </c>
-      <c r="D55" s="20"/>
-      <c r="E55" s="23"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="20"/>
       <c r="F55" s="29" t="s">
         <v>15</v>
       </c>
@@ -1609,8 +1615,8 @@
       <c r="C56" s="8">
         <v>45119</v>
       </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="23"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="20"/>
       <c r="F56" s="29"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1623,8 +1629,8 @@
       <c r="C57" s="8">
         <v>45120</v>
       </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="23"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="20"/>
       <c r="F57" s="29" t="s">
         <v>16</v>
       </c>
@@ -1639,8 +1645,8 @@
       <c r="C58" s="8">
         <v>45124</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="23"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="20"/>
       <c r="F58" s="29"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1653,8 +1659,8 @@
       <c r="C59" s="8">
         <v>45125</v>
       </c>
-      <c r="D59" s="21"/>
-      <c r="E59" s="23"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="20"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1669,10 +1675,10 @@
       <c r="C60" s="8">
         <v>45126</v>
       </c>
-      <c r="D60" s="19">
+      <c r="D60" s="24">
         <v>9</v>
       </c>
-      <c r="E60" s="24" t="s">
+      <c r="E60" s="21" t="s">
         <v>41</v>
       </c>
       <c r="F60" s="27" t="s">
@@ -1689,8 +1695,8 @@
       <c r="C61" s="8">
         <v>45127</v>
       </c>
-      <c r="D61" s="21"/>
-      <c r="E61" s="25"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="23"/>
       <c r="F61" s="28"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1703,10 +1709,10 @@
       <c r="C62" s="8">
         <v>45131</v>
       </c>
-      <c r="D62" s="19">
+      <c r="D62" s="24">
         <v>10</v>
       </c>
-      <c r="E62" s="24" t="s">
+      <c r="E62" s="21" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1721,8 +1727,8 @@
       <c r="C63" s="8">
         <v>45132</v>
       </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="26"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="22"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1735,8 +1741,8 @@
       <c r="C64" s="8">
         <v>45133</v>
       </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="26"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="22"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1749,8 +1755,8 @@
       <c r="C65" s="8">
         <v>45134</v>
       </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="26"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="22"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1763,8 +1769,8 @@
       <c r="C66" s="8">
         <v>45138</v>
       </c>
-      <c r="D66" s="20"/>
-      <c r="E66" s="26"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="22"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1777,8 +1783,8 @@
       <c r="C67" s="11">
         <v>45139</v>
       </c>
-      <c r="D67" s="20"/>
-      <c r="E67" s="26"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="22"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1791,8 +1797,8 @@
       <c r="C68" s="8">
         <v>45140</v>
       </c>
-      <c r="D68" s="20"/>
-      <c r="E68" s="26"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="22"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1805,8 +1811,8 @@
       <c r="C69" s="8">
         <v>45141</v>
       </c>
-      <c r="D69" s="20"/>
-      <c r="E69" s="26"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="22"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1819,8 +1825,8 @@
       <c r="C70" s="8">
         <v>45146</v>
       </c>
-      <c r="D70" s="21"/>
-      <c r="E70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="22"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1833,10 +1839,10 @@
       <c r="C71" s="8">
         <v>45147</v>
       </c>
-      <c r="D71" s="19">
+      <c r="D71" s="24">
         <v>11</v>
       </c>
-      <c r="E71" s="24" t="s">
+      <c r="E71" s="21" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1851,8 +1857,8 @@
       <c r="C72" s="11">
         <v>45148</v>
       </c>
-      <c r="D72" s="20"/>
-      <c r="E72" s="26"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="22"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,8 +1871,8 @@
       <c r="C73" s="8">
         <v>45152</v>
       </c>
-      <c r="D73" s="20"/>
-      <c r="E73" s="26"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="22"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1879,8 +1885,8 @@
       <c r="C74" s="8">
         <v>45153</v>
       </c>
-      <c r="D74" s="20"/>
-      <c r="E74" s="26"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="22"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -1895,8 +1901,8 @@
       <c r="C75" s="8">
         <v>45154</v>
       </c>
-      <c r="D75" s="20"/>
-      <c r="E75" s="26"/>
+      <c r="D75" s="25"/>
+      <c r="E75" s="22"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1909,8 +1915,8 @@
       <c r="C76" s="8">
         <v>45155</v>
       </c>
-      <c r="D76" s="20"/>
-      <c r="E76" s="26"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="22"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1923,8 +1929,8 @@
       <c r="C77" s="8">
         <v>45160</v>
       </c>
-      <c r="D77" s="20"/>
-      <c r="E77" s="26"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="22"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1937,8 +1943,8 @@
       <c r="C78" s="8">
         <v>45161</v>
       </c>
-      <c r="D78" s="20"/>
-      <c r="E78" s="26"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="22"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -1951,8 +1957,8 @@
       <c r="C79" s="8">
         <v>45162</v>
       </c>
-      <c r="D79" s="20"/>
-      <c r="E79" s="26"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="22"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,8 +1971,8 @@
       <c r="C80" s="8">
         <v>45166</v>
       </c>
-      <c r="D80" s="21"/>
-      <c r="E80" s="25"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="23"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -1979,10 +1985,10 @@
       <c r="C81" s="8">
         <v>45167</v>
       </c>
-      <c r="D81" s="22">
+      <c r="D81" s="19">
         <v>12</v>
       </c>
-      <c r="E81" s="23" t="s">
+      <c r="E81" s="20" t="s">
         <v>46</v>
       </c>
       <c r="F81" s="5"/>
@@ -1997,8 +2003,8 @@
       <c r="C82" s="8">
         <v>45168</v>
       </c>
-      <c r="D82" s="22"/>
-      <c r="E82" s="23"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="20"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2011,8 +2017,8 @@
       <c r="C83" s="8">
         <v>45169</v>
       </c>
-      <c r="D83" s="22"/>
-      <c r="E83" s="23"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="20"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2025,8 +2031,8 @@
       <c r="C84" s="8">
         <v>45173</v>
       </c>
-      <c r="D84" s="22"/>
-      <c r="E84" s="23"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="20"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,8 +2045,8 @@
       <c r="C85" s="8">
         <v>45174</v>
       </c>
-      <c r="D85" s="22"/>
-      <c r="E85" s="23"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="20"/>
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2053,8 +2059,8 @@
       <c r="C86" s="8">
         <v>45175</v>
       </c>
-      <c r="D86" s="22"/>
-      <c r="E86" s="23"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="20"/>
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2067,8 +2073,8 @@
       <c r="C87" s="8">
         <v>45176</v>
       </c>
-      <c r="D87" s="22"/>
-      <c r="E87" s="23"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="20"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2081,8 +2087,8 @@
       <c r="C88" s="8">
         <v>45180</v>
       </c>
-      <c r="D88" s="22"/>
-      <c r="E88" s="23"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="20"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2095,8 +2101,8 @@
       <c r="C89" s="8">
         <v>45181</v>
       </c>
-      <c r="D89" s="22"/>
-      <c r="E89" s="23"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="20"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2109,8 +2115,8 @@
       <c r="C90" s="8">
         <v>45182</v>
       </c>
-      <c r="D90" s="22"/>
-      <c r="E90" s="23"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="20"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2123,8 +2129,8 @@
       <c r="C91" s="8">
         <v>45183</v>
       </c>
-      <c r="D91" s="22"/>
-      <c r="E91" s="23"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="20"/>
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2137,10 +2143,10 @@
       <c r="C92" s="8">
         <v>45187</v>
       </c>
-      <c r="D92" s="22">
+      <c r="D92" s="19">
         <v>13</v>
       </c>
-      <c r="E92" s="23" t="s">
+      <c r="E92" s="20" t="s">
         <v>47</v>
       </c>
       <c r="F92" s="5"/>
@@ -2155,8 +2161,8 @@
       <c r="C93" s="8">
         <v>45188</v>
       </c>
-      <c r="D93" s="22"/>
-      <c r="E93" s="23"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="20"/>
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2169,8 +2175,8 @@
       <c r="C94" s="8">
         <v>45189</v>
       </c>
-      <c r="D94" s="22"/>
-      <c r="E94" s="23"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="20"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2183,8 +2189,8 @@
       <c r="C95" s="8">
         <v>45190</v>
       </c>
-      <c r="D95" s="22"/>
-      <c r="E95" s="23"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="20"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2197,10 +2203,10 @@
       <c r="C96" s="8">
         <v>45194</v>
       </c>
-      <c r="D96" s="19">
+      <c r="D96" s="24">
         <v>14</v>
       </c>
-      <c r="E96" s="24" t="s">
+      <c r="E96" s="21" t="s">
         <v>48</v>
       </c>
       <c r="F96" s="5"/>
@@ -2215,8 +2221,8 @@
       <c r="C97" s="8">
         <v>45195</v>
       </c>
-      <c r="D97" s="20"/>
-      <c r="E97" s="26"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="22"/>
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,8 +2235,8 @@
       <c r="C98" s="11">
         <v>45196</v>
       </c>
-      <c r="D98" s="20"/>
-      <c r="E98" s="26"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="22"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2243,8 +2249,8 @@
       <c r="C99" s="8">
         <v>45197</v>
       </c>
-      <c r="D99" s="20"/>
-      <c r="E99" s="26"/>
+      <c r="D99" s="25"/>
+      <c r="E99" s="22"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2257,8 +2263,8 @@
       <c r="C100" s="8">
         <v>45201</v>
       </c>
-      <c r="D100" s="20"/>
-      <c r="E100" s="26"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="22"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,8 +2277,8 @@
       <c r="C101" s="8">
         <v>45202</v>
       </c>
-      <c r="D101" s="20"/>
-      <c r="E101" s="26"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="22"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2285,8 +2291,8 @@
       <c r="C102" s="8">
         <v>45203</v>
       </c>
-      <c r="D102" s="20"/>
-      <c r="E102" s="26"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="22"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2299,8 +2305,8 @@
       <c r="C103" s="8">
         <v>45204</v>
       </c>
-      <c r="D103" s="20"/>
-      <c r="E103" s="26"/>
+      <c r="D103" s="25"/>
+      <c r="E103" s="22"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2313,8 +2319,8 @@
       <c r="C104" s="8">
         <v>45208</v>
       </c>
-      <c r="D104" s="21"/>
-      <c r="E104" s="25"/>
+      <c r="D104" s="26"/>
+      <c r="E104" s="23"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2345,10 +2351,10 @@
       <c r="C106" s="8">
         <v>45210</v>
       </c>
-      <c r="D106" s="19">
+      <c r="D106" s="24">
         <v>15</v>
       </c>
-      <c r="E106" s="24" t="s">
+      <c r="E106" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F106" s="5"/>
@@ -2363,8 +2369,8 @@
       <c r="C107" s="8">
         <v>45211</v>
       </c>
-      <c r="D107" s="20"/>
-      <c r="E107" s="26"/>
+      <c r="D107" s="25"/>
+      <c r="E107" s="22"/>
       <c r="F107" s="5"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2377,8 +2383,8 @@
       <c r="C108" s="8">
         <v>45216</v>
       </c>
-      <c r="D108" s="20"/>
-      <c r="E108" s="26"/>
+      <c r="D108" s="25"/>
+      <c r="E108" s="22"/>
       <c r="F108" s="5"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -2391,8 +2397,8 @@
       <c r="C109" s="8">
         <v>45217</v>
       </c>
-      <c r="D109" s="21"/>
-      <c r="E109" s="25"/>
+      <c r="D109" s="26"/>
+      <c r="E109" s="23"/>
       <c r="F109" s="5"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -2405,10 +2411,10 @@
       <c r="C110" s="8">
         <v>45218</v>
       </c>
-      <c r="D110" s="19">
+      <c r="D110" s="24">
         <v>16</v>
       </c>
-      <c r="E110" s="24" t="s">
+      <c r="E110" s="21" t="s">
         <v>51</v>
       </c>
       <c r="F110" s="5"/>
@@ -2423,8 +2429,8 @@
       <c r="C111" s="8">
         <v>45222</v>
       </c>
-      <c r="D111" s="20"/>
-      <c r="E111" s="26"/>
+      <c r="D111" s="25"/>
+      <c r="E111" s="22"/>
       <c r="F111" s="5"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -2437,8 +2443,8 @@
       <c r="C112" s="8">
         <v>45223</v>
       </c>
-      <c r="D112" s="20"/>
-      <c r="E112" s="26"/>
+      <c r="D112" s="25"/>
+      <c r="E112" s="22"/>
       <c r="F112" s="5"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2451,8 +2457,8 @@
       <c r="C113" s="8">
         <v>45224</v>
       </c>
-      <c r="D113" s="20"/>
-      <c r="E113" s="26"/>
+      <c r="D113" s="25"/>
+      <c r="E113" s="22"/>
       <c r="F113" s="5"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2465,8 +2471,8 @@
       <c r="C114" s="8">
         <v>45225</v>
       </c>
-      <c r="D114" s="20"/>
-      <c r="E114" s="26"/>
+      <c r="D114" s="25"/>
+      <c r="E114" s="22"/>
       <c r="F114" s="5"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -2479,8 +2485,8 @@
       <c r="C115" s="8">
         <v>45229</v>
       </c>
-      <c r="D115" s="20"/>
-      <c r="E115" s="26"/>
+      <c r="D115" s="25"/>
+      <c r="E115" s="22"/>
       <c r="F115" s="5"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -2490,12 +2496,14 @@
       <c r="B116" s="5">
         <v>7</v>
       </c>
-      <c r="C116" s="9">
+      <c r="C116" s="8">
         <v>45230</v>
       </c>
-      <c r="D116" s="20"/>
-      <c r="E116" s="26"/>
-      <c r="F116" s="5"/>
+      <c r="D116" s="25"/>
+      <c r="E116" s="22"/>
+      <c r="F116" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
@@ -2507,15 +2515,17 @@
       <c r="C117" s="9">
         <v>45231</v>
       </c>
-      <c r="D117" s="21"/>
-      <c r="E117" s="25"/>
+      <c r="D117" s="26"/>
+      <c r="E117" s="23"/>
       <c r="F117" s="5"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>117</v>
       </c>
-      <c r="B118" s="5"/>
+      <c r="B118" s="5">
+        <v>1</v>
+      </c>
       <c r="C118" s="9">
         <v>45232</v>
       </c>
@@ -2531,156 +2541,186 @@
       <c r="A119" s="5">
         <v>118</v>
       </c>
-      <c r="B119" s="5"/>
+      <c r="B119" s="5">
+        <v>1</v>
+      </c>
       <c r="C119" s="9">
         <v>45236</v>
       </c>
-      <c r="D119" s="6"/>
-      <c r="E119" s="14"/>
+      <c r="D119" s="24">
+        <v>18</v>
+      </c>
+      <c r="E119" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="F119" s="5"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>119</v>
       </c>
-      <c r="B120" s="5"/>
+      <c r="B120" s="5">
+        <v>2</v>
+      </c>
       <c r="C120" s="9">
         <v>45237</v>
       </c>
-      <c r="D120" s="6"/>
-      <c r="E120" s="14"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="22"/>
       <c r="F120" s="5"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>120</v>
       </c>
-      <c r="B121" s="5"/>
+      <c r="B121" s="5">
+        <v>3</v>
+      </c>
       <c r="C121" s="9">
         <v>45238</v>
       </c>
-      <c r="D121" s="6"/>
-      <c r="E121" s="14"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="22"/>
       <c r="F121" s="5"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>121</v>
       </c>
-      <c r="B122" s="5"/>
+      <c r="B122" s="5">
+        <v>4</v>
+      </c>
       <c r="C122" s="9">
         <v>45239</v>
       </c>
-      <c r="D122" s="6"/>
-      <c r="E122" s="14"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="22"/>
       <c r="F122" s="5"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>122</v>
       </c>
-      <c r="B123" s="5"/>
+      <c r="B123" s="5">
+        <v>5</v>
+      </c>
       <c r="C123" s="9">
         <v>45243</v>
       </c>
-      <c r="D123" s="6"/>
-      <c r="E123" s="14"/>
+      <c r="D123" s="25"/>
+      <c r="E123" s="22"/>
       <c r="F123" s="5"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>123</v>
       </c>
-      <c r="B124" s="5"/>
+      <c r="B124" s="5">
+        <v>6</v>
+      </c>
       <c r="C124" s="9">
         <v>45244</v>
       </c>
-      <c r="D124" s="6"/>
-      <c r="E124" s="14"/>
+      <c r="D124" s="25"/>
+      <c r="E124" s="22"/>
       <c r="F124" s="5"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>124</v>
       </c>
-      <c r="B125" s="5"/>
+      <c r="B125" s="5">
+        <v>7</v>
+      </c>
       <c r="C125" s="9">
         <v>45245</v>
       </c>
-      <c r="D125" s="6"/>
-      <c r="E125" s="14"/>
+      <c r="D125" s="25"/>
+      <c r="E125" s="22"/>
       <c r="F125" s="5"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>125</v>
       </c>
-      <c r="B126" s="5"/>
+      <c r="B126" s="5">
+        <v>8</v>
+      </c>
       <c r="C126" s="9">
         <v>45246</v>
       </c>
-      <c r="D126" s="6"/>
-      <c r="E126" s="14"/>
+      <c r="D126" s="25"/>
+      <c r="E126" s="22"/>
       <c r="F126" s="5"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>126</v>
       </c>
-      <c r="B127" s="5"/>
+      <c r="B127" s="5">
+        <v>9</v>
+      </c>
       <c r="C127" s="9">
         <v>45251</v>
       </c>
-      <c r="D127" s="6"/>
-      <c r="E127" s="14"/>
+      <c r="D127" s="25"/>
+      <c r="E127" s="22"/>
       <c r="F127" s="5"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>127</v>
       </c>
-      <c r="B128" s="5"/>
+      <c r="B128" s="5">
+        <v>10</v>
+      </c>
       <c r="C128" s="9">
         <v>45252</v>
       </c>
-      <c r="D128" s="6"/>
-      <c r="E128" s="14"/>
+      <c r="D128" s="25"/>
+      <c r="E128" s="22"/>
       <c r="F128" s="5"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>128</v>
       </c>
-      <c r="B129" s="5"/>
+      <c r="B129" s="5">
+        <v>11</v>
+      </c>
       <c r="C129" s="9">
         <v>45253</v>
       </c>
-      <c r="D129" s="6"/>
-      <c r="E129" s="14"/>
+      <c r="D129" s="25"/>
+      <c r="E129" s="22"/>
       <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>129</v>
       </c>
-      <c r="B130" s="5"/>
+      <c r="B130" s="5">
+        <v>12</v>
+      </c>
       <c r="C130" s="9">
         <v>45257</v>
       </c>
-      <c r="D130" s="6"/>
-      <c r="E130" s="14"/>
+      <c r="D130" s="25"/>
+      <c r="E130" s="22"/>
       <c r="F130" s="5"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>130</v>
       </c>
-      <c r="B131" s="5"/>
+      <c r="B131" s="5">
+        <v>13</v>
+      </c>
       <c r="C131" s="9">
         <v>45258</v>
       </c>
-      <c r="D131" s="6"/>
-      <c r="E131" s="14"/>
+      <c r="D131" s="26"/>
+      <c r="E131" s="23"/>
       <c r="F131" s="5"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -2947,7 +2987,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="24" t="s">
+      <c r="E153" s="21" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -2963,7 +3003,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="26"/>
+      <c r="E154" s="22"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -2977,7 +3017,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="26"/>
+      <c r="E155" s="22"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -2991,7 +3031,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="26"/>
+      <c r="E156" s="22"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -3005,7 +3045,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="26"/>
+      <c r="E157" s="22"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -3019,7 +3059,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="26"/>
+      <c r="E158" s="22"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -3033,7 +3073,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="26"/>
+      <c r="E159" s="22"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3047,7 +3087,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="26"/>
+      <c r="E160" s="22"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3061,7 +3101,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="26"/>
+      <c r="E161" s="22"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3075,7 +3115,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="26"/>
+      <c r="E162" s="22"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3089,7 +3129,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="26"/>
+      <c r="E163" s="22"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3103,7 +3143,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="26"/>
+      <c r="E164" s="22"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3117,7 +3157,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="26"/>
+      <c r="E165" s="22"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3131,7 +3171,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="26"/>
+      <c r="E166" s="22"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3145,7 +3185,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="26"/>
+      <c r="E167" s="22"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3159,7 +3199,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="26"/>
+      <c r="E168" s="22"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3173,7 +3213,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="26"/>
+      <c r="E169" s="22"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3187,7 +3227,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="26"/>
+      <c r="E170" s="22"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3201,7 +3241,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="26"/>
+      <c r="E171" s="22"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3215,7 +3255,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="26"/>
+      <c r="E172" s="22"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3229,7 +3269,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="26"/>
+      <c r="E173" s="22"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3243,7 +3283,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="26"/>
+      <c r="E174" s="22"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3257,7 +3297,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="26"/>
+      <c r="E175" s="22"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3271,7 +3311,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="26"/>
+      <c r="E176" s="22"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3285,7 +3325,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="26"/>
+      <c r="E177" s="22"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3299,7 +3339,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="26"/>
+      <c r="E178" s="22"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3313,31 +3353,19 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="25"/>
+      <c r="E179" s="23"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
   <sortState columnSort="1" ref="D3:J3">
     <sortCondition ref="D3:J3"/>
   </sortState>
-  <mergeCells count="37">
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="E96:E104"/>
-    <mergeCell ref="D96:D104"/>
-    <mergeCell ref="E153:E179"/>
-    <mergeCell ref="D106:D109"/>
-    <mergeCell ref="E106:E109"/>
-    <mergeCell ref="D110:D117"/>
-    <mergeCell ref="E110:E117"/>
-    <mergeCell ref="E71:E80"/>
-    <mergeCell ref="E81:E91"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="F51:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F57:F58"/>
+  <mergeCells count="39">
+    <mergeCell ref="D71:D80"/>
+    <mergeCell ref="D81:D91"/>
+    <mergeCell ref="D30:D39"/>
+    <mergeCell ref="D40:D59"/>
+    <mergeCell ref="D60:D61"/>
     <mergeCell ref="E30:E39"/>
     <mergeCell ref="D62:D70"/>
     <mergeCell ref="D3:D4"/>
@@ -3353,11 +3381,25 @@
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="E62:E70"/>
-    <mergeCell ref="D71:D80"/>
-    <mergeCell ref="D81:D91"/>
-    <mergeCell ref="D30:D39"/>
-    <mergeCell ref="D40:D59"/>
-    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E71:E80"/>
+    <mergeCell ref="E81:E91"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="E96:E104"/>
+    <mergeCell ref="D96:D104"/>
+    <mergeCell ref="E153:E179"/>
+    <mergeCell ref="D106:D109"/>
+    <mergeCell ref="E106:E109"/>
+    <mergeCell ref="D110:D117"/>
+    <mergeCell ref="E110:E117"/>
+    <mergeCell ref="D119:D131"/>
+    <mergeCell ref="E119:E131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
armando biblioteca con los videos
</commit_message>
<xml_diff>
--- a/Encuentros.xlsx
+++ b/Encuentros.xlsx
@@ -422,6 +422,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -431,20 +440,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -806,7 +806,7 @@
         <v>56</v>
       </c>
       <c r="H1" s="21">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>57</v>
@@ -825,7 +825,7 @@
       </c>
       <c r="N1" s="24">
         <f>+H1+J1+L1</f>
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -856,10 +856,10 @@
       <c r="C3" s="8">
         <v>45019</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="28">
         <v>1</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="32" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5"/>
@@ -874,8 +874,8 @@
       <c r="C4" s="8">
         <v>45020</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
@@ -890,10 +890,10 @@
       <c r="C5" s="8">
         <v>45021</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="28">
         <v>2</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -910,8 +910,8 @@
       <c r="C6" s="8">
         <v>45026</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
@@ -926,8 +926,8 @@
       <c r="C7" s="8">
         <v>45027</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="12" t="s">
         <v>31</v>
       </c>
@@ -942,10 +942,10 @@
       <c r="C8" s="8">
         <v>45028</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="28">
         <v>3</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="32" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -962,8 +962,8 @@
       <c r="C9" s="8">
         <v>45029</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
@@ -978,8 +978,8 @@
       <c r="C10" s="8">
         <v>45033</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="12" t="s">
         <v>32</v>
       </c>
@@ -994,8 +994,8 @@
       <c r="C11" s="8">
         <v>45034</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
@@ -1030,10 +1030,10 @@
       <c r="C13" s="8">
         <v>45036</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="28">
         <v>4</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="32" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1050,8 +1050,8 @@
       <c r="C14" s="8">
         <v>45040</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
@@ -1066,8 +1066,8 @@
       <c r="C15" s="8">
         <v>45041</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
@@ -1082,8 +1082,8 @@
       <c r="C16" s="8">
         <v>45042</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
@@ -1098,8 +1098,8 @@
       <c r="C17" s="8">
         <v>45043</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="C18" s="8">
         <v>45048</v>
       </c>
-      <c r="D18" s="35"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="14" t="s">
         <v>8</v>
       </c>
@@ -1132,10 +1132,10 @@
       <c r="C19" s="8">
         <v>45049</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="28">
         <v>5</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="32" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1152,8 +1152,8 @@
       <c r="C20" s="8">
         <v>45050</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1168,8 +1168,8 @@
       <c r="C21" s="8">
         <v>45054</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1184,8 +1184,8 @@
       <c r="C22" s="8">
         <v>45055</v>
       </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1200,8 +1200,8 @@
       <c r="C23" s="8">
         <v>45056</v>
       </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="12" t="s">
         <v>36</v>
       </c>
@@ -1216,8 +1216,8 @@
       <c r="C24" s="8">
         <v>45057</v>
       </c>
-      <c r="D24" s="34"/>
-      <c r="E24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="32"/>
       <c r="F24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1232,8 +1232,8 @@
       <c r="C25" s="8">
         <v>45062</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="12" t="s">
         <v>36</v>
       </c>
@@ -1248,8 +1248,8 @@
       <c r="C26" s="8">
         <v>45062</v>
       </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="32"/>
       <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="C27" s="8">
         <v>45063</v>
       </c>
-      <c r="D27" s="34"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="14" t="s">
         <v>8</v>
       </c>
@@ -1282,7 +1282,7 @@
       <c r="C28" s="8">
         <v>45064</v>
       </c>
-      <c r="D28" s="35"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="14" t="s">
         <v>9</v>
       </c>
@@ -1320,10 +1320,10 @@
       <c r="C30" s="8">
         <v>45069</v>
       </c>
-      <c r="D30" s="33">
+      <c r="D30" s="28">
         <v>7</v>
       </c>
-      <c r="E30" s="29" t="s">
+      <c r="E30" s="32" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1340,8 +1340,8 @@
       <c r="C31" s="8">
         <v>45070</v>
       </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
@@ -1356,8 +1356,8 @@
       <c r="C32" s="8">
         <v>45075</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="32"/>
       <c r="F32" s="12" t="s">
         <v>40</v>
       </c>
@@ -1372,8 +1372,8 @@
       <c r="C33" s="8">
         <v>45076</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="12" t="s">
         <v>40</v>
       </c>
@@ -1388,8 +1388,8 @@
       <c r="C34" s="8">
         <v>45077</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="12" t="s">
         <v>40</v>
       </c>
@@ -1404,8 +1404,8 @@
       <c r="C35" s="8">
         <v>45078</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
@@ -1420,8 +1420,8 @@
       <c r="C36" s="8">
         <v>45082</v>
       </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="32"/>
       <c r="F36" s="12" t="s">
         <v>40</v>
       </c>
@@ -1436,8 +1436,8 @@
       <c r="C37" s="8">
         <v>45083</v>
       </c>
-      <c r="D37" s="34"/>
-      <c r="E37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="32"/>
       <c r="F37" s="12" t="s">
         <v>40</v>
       </c>
@@ -1452,8 +1452,8 @@
       <c r="C38" s="8">
         <v>45084</v>
       </c>
-      <c r="D38" s="34"/>
-      <c r="E38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="32"/>
       <c r="F38" s="12" t="s">
         <v>40</v>
       </c>
@@ -1468,8 +1468,8 @@
       <c r="C39" s="8">
         <v>45085</v>
       </c>
-      <c r="D39" s="35"/>
-      <c r="E39" s="29"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="12" t="s">
         <v>40</v>
       </c>
@@ -1484,10 +1484,10 @@
       <c r="C40" s="8">
         <v>45089</v>
       </c>
-      <c r="D40" s="33">
+      <c r="D40" s="28">
         <v>8</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="32" t="s">
         <v>3</v>
       </c>
       <c r="F40" s="38" t="s">
@@ -1504,8 +1504,8 @@
       <c r="C41" s="8">
         <v>45090</v>
       </c>
-      <c r="D41" s="34"/>
-      <c r="E41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="32"/>
       <c r="F41" s="38"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1518,8 +1518,8 @@
       <c r="C42" s="8">
         <v>45091</v>
       </c>
-      <c r="D42" s="34"/>
-      <c r="E42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="32"/>
       <c r="F42" s="38"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,8 +1532,8 @@
       <c r="C43" s="8">
         <v>45092</v>
       </c>
-      <c r="D43" s="34"/>
-      <c r="E43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="38"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1546,8 +1546,8 @@
       <c r="C44" s="8">
         <v>45098</v>
       </c>
-      <c r="D44" s="34"/>
-      <c r="E44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="32"/>
       <c r="F44" s="10" t="s">
         <v>23</v>
       </c>
@@ -1562,8 +1562,8 @@
       <c r="C45" s="8">
         <v>45099</v>
       </c>
-      <c r="D45" s="34"/>
-      <c r="E45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="5" t="s">
         <v>21</v>
       </c>
@@ -1578,8 +1578,8 @@
       <c r="C46" s="8">
         <v>45103</v>
       </c>
-      <c r="D46" s="34"/>
-      <c r="E46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="32"/>
       <c r="F46" s="38" t="s">
         <v>20</v>
       </c>
@@ -1594,8 +1594,8 @@
       <c r="C47" s="8">
         <v>45104</v>
       </c>
-      <c r="D47" s="34"/>
-      <c r="E47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="32"/>
       <c r="F47" s="38"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,8 +1608,8 @@
       <c r="C48" s="8">
         <v>45105</v>
       </c>
-      <c r="D48" s="34"/>
-      <c r="E48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="32"/>
       <c r="F48" s="38"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1622,8 +1622,8 @@
       <c r="C49" s="8">
         <v>45106</v>
       </c>
-      <c r="D49" s="34"/>
-      <c r="E49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="32"/>
       <c r="F49" s="38"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1636,8 +1636,8 @@
       <c r="C50" s="8">
         <v>45110</v>
       </c>
-      <c r="D50" s="34"/>
-      <c r="E50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="32"/>
       <c r="F50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1652,8 +1652,8 @@
       <c r="C51" s="11">
         <v>45111</v>
       </c>
-      <c r="D51" s="34"/>
-      <c r="E51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="32"/>
       <c r="F51" s="39" t="s">
         <v>18</v>
       </c>
@@ -1668,8 +1668,8 @@
       <c r="C52" s="8">
         <v>45112</v>
       </c>
-      <c r="D52" s="34"/>
-      <c r="E52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="32"/>
       <c r="F52" s="39"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1682,8 +1682,8 @@
       <c r="C53" s="8">
         <v>45113</v>
       </c>
-      <c r="D53" s="34"/>
-      <c r="E53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="32"/>
       <c r="F53" s="39"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,8 +1696,8 @@
       <c r="C54" s="8">
         <v>45117</v>
       </c>
-      <c r="D54" s="34"/>
-      <c r="E54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="39"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1710,8 +1710,8 @@
       <c r="C55" s="8">
         <v>45118</v>
       </c>
-      <c r="D55" s="34"/>
-      <c r="E55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="32"/>
       <c r="F55" s="38" t="s">
         <v>15</v>
       </c>
@@ -1726,8 +1726,8 @@
       <c r="C56" s="8">
         <v>45119</v>
       </c>
-      <c r="D56" s="34"/>
-      <c r="E56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="32"/>
       <c r="F56" s="38"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1740,8 +1740,8 @@
       <c r="C57" s="8">
         <v>45120</v>
       </c>
-      <c r="D57" s="34"/>
-      <c r="E57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="32"/>
       <c r="F57" s="38" t="s">
         <v>16</v>
       </c>
@@ -1756,8 +1756,8 @@
       <c r="C58" s="8">
         <v>45124</v>
       </c>
-      <c r="D58" s="34"/>
-      <c r="E58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="32"/>
       <c r="F58" s="38"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1770,8 +1770,8 @@
       <c r="C59" s="8">
         <v>45125</v>
       </c>
-      <c r="D59" s="35"/>
-      <c r="E59" s="29"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="32"/>
       <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
@@ -1786,10 +1786,10 @@
       <c r="C60" s="8">
         <v>45126</v>
       </c>
-      <c r="D60" s="33">
+      <c r="D60" s="28">
         <v>9</v>
       </c>
-      <c r="E60" s="30" t="s">
+      <c r="E60" s="33" t="s">
         <v>41</v>
       </c>
       <c r="F60" s="36" t="s">
@@ -1806,8 +1806,8 @@
       <c r="C61" s="8">
         <v>45127</v>
       </c>
-      <c r="D61" s="35"/>
-      <c r="E61" s="32"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="34"/>
       <c r="F61" s="37"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,10 +1820,10 @@
       <c r="C62" s="8">
         <v>45131</v>
       </c>
-      <c r="D62" s="33">
+      <c r="D62" s="28">
         <v>10</v>
       </c>
-      <c r="E62" s="30" t="s">
+      <c r="E62" s="33" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -1838,8 +1838,8 @@
       <c r="C63" s="8">
         <v>45132</v>
       </c>
-      <c r="D63" s="34"/>
-      <c r="E63" s="31"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="35"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,8 +1852,8 @@
       <c r="C64" s="8">
         <v>45133</v>
       </c>
-      <c r="D64" s="34"/>
-      <c r="E64" s="31"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="35"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,8 +1866,8 @@
       <c r="C65" s="8">
         <v>45134</v>
       </c>
-      <c r="D65" s="34"/>
-      <c r="E65" s="31"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="35"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1880,8 +1880,8 @@
       <c r="C66" s="8">
         <v>45138</v>
       </c>
-      <c r="D66" s="34"/>
-      <c r="E66" s="31"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="35"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1894,8 +1894,8 @@
       <c r="C67" s="11">
         <v>45139</v>
       </c>
-      <c r="D67" s="34"/>
-      <c r="E67" s="31"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="35"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1908,8 +1908,8 @@
       <c r="C68" s="8">
         <v>45140</v>
       </c>
-      <c r="D68" s="34"/>
-      <c r="E68" s="31"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="35"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1922,8 +1922,8 @@
       <c r="C69" s="8">
         <v>45141</v>
       </c>
-      <c r="D69" s="34"/>
-      <c r="E69" s="31"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="35"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,8 +1936,8 @@
       <c r="C70" s="8">
         <v>45146</v>
       </c>
-      <c r="D70" s="35"/>
-      <c r="E70" s="31"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="35"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1950,10 +1950,10 @@
       <c r="C71" s="8">
         <v>45147</v>
       </c>
-      <c r="D71" s="33">
+      <c r="D71" s="28">
         <v>11</v>
       </c>
-      <c r="E71" s="30" t="s">
+      <c r="E71" s="33" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="5"/>
@@ -1968,8 +1968,8 @@
       <c r="C72" s="11">
         <v>45148</v>
       </c>
-      <c r="D72" s="34"/>
-      <c r="E72" s="31"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="35"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1982,8 +1982,8 @@
       <c r="C73" s="8">
         <v>45152</v>
       </c>
-      <c r="D73" s="34"/>
-      <c r="E73" s="31"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="35"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1996,8 +1996,8 @@
       <c r="C74" s="8">
         <v>45153</v>
       </c>
-      <c r="D74" s="34"/>
-      <c r="E74" s="31"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="35"/>
       <c r="F74" s="5" t="s">
         <v>45</v>
       </c>
@@ -2012,8 +2012,8 @@
       <c r="C75" s="8">
         <v>45154</v>
       </c>
-      <c r="D75" s="34"/>
-      <c r="E75" s="31"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="35"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,8 +2026,8 @@
       <c r="C76" s="8">
         <v>45155</v>
       </c>
-      <c r="D76" s="34"/>
-      <c r="E76" s="31"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="35"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,8 +2040,8 @@
       <c r="C77" s="8">
         <v>45160</v>
       </c>
-      <c r="D77" s="34"/>
-      <c r="E77" s="31"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="35"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2054,8 +2054,8 @@
       <c r="C78" s="8">
         <v>45161</v>
       </c>
-      <c r="D78" s="34"/>
-      <c r="E78" s="31"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="35"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2068,8 +2068,8 @@
       <c r="C79" s="8">
         <v>45162</v>
       </c>
-      <c r="D79" s="34"/>
-      <c r="E79" s="31"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="35"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,8 +2082,8 @@
       <c r="C80" s="8">
         <v>45166</v>
       </c>
-      <c r="D80" s="35"/>
-      <c r="E80" s="32"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="34"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2096,10 +2096,10 @@
       <c r="C81" s="8">
         <v>45167</v>
       </c>
-      <c r="D81" s="28">
+      <c r="D81" s="31">
         <v>12</v>
       </c>
-      <c r="E81" s="29" t="s">
+      <c r="E81" s="32" t="s">
         <v>46</v>
       </c>
       <c r="F81" s="5"/>
@@ -2114,8 +2114,8 @@
       <c r="C82" s="8">
         <v>45168</v>
       </c>
-      <c r="D82" s="28"/>
-      <c r="E82" s="29"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="32"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2128,8 +2128,8 @@
       <c r="C83" s="8">
         <v>45169</v>
       </c>
-      <c r="D83" s="28"/>
-      <c r="E83" s="29"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="32"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2142,8 +2142,8 @@
       <c r="C84" s="8">
         <v>45173</v>
       </c>
-      <c r="D84" s="28"/>
-      <c r="E84" s="29"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="32"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2156,8 +2156,8 @@
       <c r="C85" s="8">
         <v>45174</v>
       </c>
-      <c r="D85" s="28"/>
-      <c r="E85" s="29"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="32"/>
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2170,8 +2170,8 @@
       <c r="C86" s="8">
         <v>45175</v>
       </c>
-      <c r="D86" s="28"/>
-      <c r="E86" s="29"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="32"/>
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2184,8 +2184,8 @@
       <c r="C87" s="8">
         <v>45176</v>
       </c>
-      <c r="D87" s="28"/>
-      <c r="E87" s="29"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="32"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,8 +2198,8 @@
       <c r="C88" s="8">
         <v>45180</v>
       </c>
-      <c r="D88" s="28"/>
-      <c r="E88" s="29"/>
+      <c r="D88" s="31"/>
+      <c r="E88" s="32"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2212,8 +2212,8 @@
       <c r="C89" s="8">
         <v>45181</v>
       </c>
-      <c r="D89" s="28"/>
-      <c r="E89" s="29"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="32"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2226,8 +2226,8 @@
       <c r="C90" s="8">
         <v>45182</v>
       </c>
-      <c r="D90" s="28"/>
-      <c r="E90" s="29"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="32"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2240,8 +2240,8 @@
       <c r="C91" s="8">
         <v>45183</v>
       </c>
-      <c r="D91" s="28"/>
-      <c r="E91" s="29"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="32"/>
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2254,10 +2254,10 @@
       <c r="C92" s="8">
         <v>45187</v>
       </c>
-      <c r="D92" s="28">
+      <c r="D92" s="31">
         <v>13</v>
       </c>
-      <c r="E92" s="29" t="s">
+      <c r="E92" s="32" t="s">
         <v>47</v>
       </c>
       <c r="F92" s="5"/>
@@ -2272,8 +2272,8 @@
       <c r="C93" s="8">
         <v>45188</v>
       </c>
-      <c r="D93" s="28"/>
-      <c r="E93" s="29"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="32"/>
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2286,8 +2286,8 @@
       <c r="C94" s="8">
         <v>45189</v>
       </c>
-      <c r="D94" s="28"/>
-      <c r="E94" s="29"/>
+      <c r="D94" s="31"/>
+      <c r="E94" s="32"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2300,8 +2300,8 @@
       <c r="C95" s="8">
         <v>45190</v>
       </c>
-      <c r="D95" s="28"/>
-      <c r="E95" s="29"/>
+      <c r="D95" s="31"/>
+      <c r="E95" s="32"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2314,10 +2314,10 @@
       <c r="C96" s="8">
         <v>45194</v>
       </c>
-      <c r="D96" s="33">
+      <c r="D96" s="28">
         <v>14</v>
       </c>
-      <c r="E96" s="30" t="s">
+      <c r="E96" s="33" t="s">
         <v>48</v>
       </c>
       <c r="F96" s="5"/>
@@ -2332,8 +2332,8 @@
       <c r="C97" s="8">
         <v>45195</v>
       </c>
-      <c r="D97" s="34"/>
-      <c r="E97" s="31"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="35"/>
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2346,8 +2346,8 @@
       <c r="C98" s="11">
         <v>45196</v>
       </c>
-      <c r="D98" s="34"/>
-      <c r="E98" s="31"/>
+      <c r="D98" s="29"/>
+      <c r="E98" s="35"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2360,8 +2360,8 @@
       <c r="C99" s="8">
         <v>45197</v>
       </c>
-      <c r="D99" s="34"/>
-      <c r="E99" s="31"/>
+      <c r="D99" s="29"/>
+      <c r="E99" s="35"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2374,8 +2374,8 @@
       <c r="C100" s="8">
         <v>45201</v>
       </c>
-      <c r="D100" s="34"/>
-      <c r="E100" s="31"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="35"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2388,8 +2388,8 @@
       <c r="C101" s="8">
         <v>45202</v>
       </c>
-      <c r="D101" s="34"/>
-      <c r="E101" s="31"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="35"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2402,8 +2402,8 @@
       <c r="C102" s="8">
         <v>45203</v>
       </c>
-      <c r="D102" s="34"/>
-      <c r="E102" s="31"/>
+      <c r="D102" s="29"/>
+      <c r="E102" s="35"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2416,8 +2416,8 @@
       <c r="C103" s="8">
         <v>45204</v>
       </c>
-      <c r="D103" s="34"/>
-      <c r="E103" s="31"/>
+      <c r="D103" s="29"/>
+      <c r="E103" s="35"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2430,8 +2430,8 @@
       <c r="C104" s="8">
         <v>45208</v>
       </c>
-      <c r="D104" s="35"/>
-      <c r="E104" s="32"/>
+      <c r="D104" s="30"/>
+      <c r="E104" s="34"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2462,10 +2462,10 @@
       <c r="C106" s="8">
         <v>45210</v>
       </c>
-      <c r="D106" s="33">
+      <c r="D106" s="28">
         <v>15</v>
       </c>
-      <c r="E106" s="30" t="s">
+      <c r="E106" s="33" t="s">
         <v>50</v>
       </c>
       <c r="F106" s="5"/>
@@ -2480,8 +2480,8 @@
       <c r="C107" s="8">
         <v>45211</v>
       </c>
-      <c r="D107" s="34"/>
-      <c r="E107" s="31"/>
+      <c r="D107" s="29"/>
+      <c r="E107" s="35"/>
       <c r="F107" s="5"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2494,8 +2494,8 @@
       <c r="C108" s="8">
         <v>45216</v>
       </c>
-      <c r="D108" s="34"/>
-      <c r="E108" s="31"/>
+      <c r="D108" s="29"/>
+      <c r="E108" s="35"/>
       <c r="F108" s="5"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,8 +2508,8 @@
       <c r="C109" s="8">
         <v>45217</v>
       </c>
-      <c r="D109" s="35"/>
-      <c r="E109" s="32"/>
+      <c r="D109" s="30"/>
+      <c r="E109" s="34"/>
       <c r="F109" s="5"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -2522,10 +2522,10 @@
       <c r="C110" s="8">
         <v>45218</v>
       </c>
-      <c r="D110" s="33">
+      <c r="D110" s="28">
         <v>16</v>
       </c>
-      <c r="E110" s="30" t="s">
+      <c r="E110" s="33" t="s">
         <v>51</v>
       </c>
       <c r="F110" s="5"/>
@@ -2540,8 +2540,8 @@
       <c r="C111" s="8">
         <v>45222</v>
       </c>
-      <c r="D111" s="34"/>
-      <c r="E111" s="31"/>
+      <c r="D111" s="29"/>
+      <c r="E111" s="35"/>
       <c r="F111" s="5"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -2554,8 +2554,8 @@
       <c r="C112" s="8">
         <v>45223</v>
       </c>
-      <c r="D112" s="34"/>
-      <c r="E112" s="31"/>
+      <c r="D112" s="29"/>
+      <c r="E112" s="35"/>
       <c r="F112" s="5"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2568,8 +2568,8 @@
       <c r="C113" s="8">
         <v>45224</v>
       </c>
-      <c r="D113" s="34"/>
-      <c r="E113" s="31"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="35"/>
       <c r="F113" s="5"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2582,8 +2582,8 @@
       <c r="C114" s="8">
         <v>45225</v>
       </c>
-      <c r="D114" s="34"/>
-      <c r="E114" s="31"/>
+      <c r="D114" s="29"/>
+      <c r="E114" s="35"/>
       <c r="F114" s="5"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -2596,8 +2596,8 @@
       <c r="C115" s="8">
         <v>45229</v>
       </c>
-      <c r="D115" s="34"/>
-      <c r="E115" s="31"/>
+      <c r="D115" s="29"/>
+      <c r="E115" s="35"/>
       <c r="F115" s="5"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -2610,8 +2610,8 @@
       <c r="C116" s="8">
         <v>45230</v>
       </c>
-      <c r="D116" s="34"/>
-      <c r="E116" s="31"/>
+      <c r="D116" s="29"/>
+      <c r="E116" s="35"/>
       <c r="F116" s="5" t="s">
         <v>54</v>
       </c>
@@ -2626,8 +2626,8 @@
       <c r="C117" s="8">
         <v>45231</v>
       </c>
-      <c r="D117" s="35"/>
-      <c r="E117" s="32"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="34"/>
       <c r="F117" s="5"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -2658,10 +2658,10 @@
       <c r="C119" s="8">
         <v>45236</v>
       </c>
-      <c r="D119" s="33">
+      <c r="D119" s="28">
         <v>18</v>
       </c>
-      <c r="E119" s="30" t="s">
+      <c r="E119" s="33" t="s">
         <v>52</v>
       </c>
       <c r="F119" s="5" t="s">
@@ -2678,8 +2678,8 @@
       <c r="C120" s="8">
         <v>45237</v>
       </c>
-      <c r="D120" s="34"/>
-      <c r="E120" s="31"/>
+      <c r="D120" s="29"/>
+      <c r="E120" s="35"/>
       <c r="F120" s="5"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -2692,8 +2692,8 @@
       <c r="C121" s="8">
         <v>45238</v>
       </c>
-      <c r="D121" s="34"/>
-      <c r="E121" s="31"/>
+      <c r="D121" s="29"/>
+      <c r="E121" s="35"/>
       <c r="F121" s="5"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -2703,11 +2703,11 @@
       <c r="B122" s="5">
         <v>4</v>
       </c>
-      <c r="C122" s="9">
+      <c r="C122" s="8">
         <v>45239</v>
       </c>
-      <c r="D122" s="34"/>
-      <c r="E122" s="31"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="35"/>
       <c r="F122" s="5"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -2720,8 +2720,8 @@
       <c r="C123" s="9">
         <v>45243</v>
       </c>
-      <c r="D123" s="34"/>
-      <c r="E123" s="31"/>
+      <c r="D123" s="29"/>
+      <c r="E123" s="35"/>
       <c r="F123" s="5"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -2734,8 +2734,8 @@
       <c r="C124" s="9">
         <v>45244</v>
       </c>
-      <c r="D124" s="34"/>
-      <c r="E124" s="31"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="35"/>
       <c r="F124" s="5"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -2748,8 +2748,8 @@
       <c r="C125" s="9">
         <v>45245</v>
       </c>
-      <c r="D125" s="34"/>
-      <c r="E125" s="31"/>
+      <c r="D125" s="29"/>
+      <c r="E125" s="35"/>
       <c r="F125" s="5"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -2762,8 +2762,8 @@
       <c r="C126" s="9">
         <v>45246</v>
       </c>
-      <c r="D126" s="34"/>
-      <c r="E126" s="31"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="35"/>
       <c r="F126" s="5"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -2776,8 +2776,8 @@
       <c r="C127" s="9">
         <v>45251</v>
       </c>
-      <c r="D127" s="34"/>
-      <c r="E127" s="31"/>
+      <c r="D127" s="29"/>
+      <c r="E127" s="35"/>
       <c r="F127" s="5"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -2790,8 +2790,8 @@
       <c r="C128" s="9">
         <v>45252</v>
       </c>
-      <c r="D128" s="34"/>
-      <c r="E128" s="31"/>
+      <c r="D128" s="29"/>
+      <c r="E128" s="35"/>
       <c r="F128" s="5"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -2804,8 +2804,8 @@
       <c r="C129" s="9">
         <v>45253</v>
       </c>
-      <c r="D129" s="34"/>
-      <c r="E129" s="31"/>
+      <c r="D129" s="29"/>
+      <c r="E129" s="35"/>
       <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -2818,8 +2818,8 @@
       <c r="C130" s="9">
         <v>45257</v>
       </c>
-      <c r="D130" s="34"/>
-      <c r="E130" s="31"/>
+      <c r="D130" s="29"/>
+      <c r="E130" s="35"/>
       <c r="F130" s="5"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -2832,8 +2832,8 @@
       <c r="C131" s="9">
         <v>45258</v>
       </c>
-      <c r="D131" s="35"/>
-      <c r="E131" s="32"/>
+      <c r="D131" s="30"/>
+      <c r="E131" s="34"/>
       <c r="F131" s="5"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -2864,10 +2864,10 @@
       <c r="C133" s="9">
         <v>45260</v>
       </c>
-      <c r="D133" s="33">
+      <c r="D133" s="28">
         <v>20</v>
       </c>
-      <c r="E133" s="30" t="s">
+      <c r="E133" s="33" t="s">
         <v>53</v>
       </c>
       <c r="F133" s="5"/>
@@ -2882,8 +2882,8 @@
       <c r="C134" s="9">
         <v>45264</v>
       </c>
-      <c r="D134" s="34"/>
-      <c r="E134" s="31"/>
+      <c r="D134" s="29"/>
+      <c r="E134" s="35"/>
       <c r="F134" s="5"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -2896,8 +2896,8 @@
       <c r="C135" s="9">
         <v>45265</v>
       </c>
-      <c r="D135" s="34"/>
-      <c r="E135" s="31"/>
+      <c r="D135" s="29"/>
+      <c r="E135" s="35"/>
       <c r="F135" s="5"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -2910,8 +2910,8 @@
       <c r="C136" s="9">
         <v>45266</v>
       </c>
-      <c r="D136" s="34"/>
-      <c r="E136" s="31"/>
+      <c r="D136" s="29"/>
+      <c r="E136" s="35"/>
       <c r="F136" s="5"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -2924,8 +2924,8 @@
       <c r="C137" s="9">
         <v>45267</v>
       </c>
-      <c r="D137" s="34"/>
-      <c r="E137" s="31"/>
+      <c r="D137" s="29"/>
+      <c r="E137" s="35"/>
       <c r="F137" s="5"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -2938,8 +2938,8 @@
       <c r="C138" s="9">
         <v>45271</v>
       </c>
-      <c r="D138" s="34"/>
-      <c r="E138" s="31"/>
+      <c r="D138" s="29"/>
+      <c r="E138" s="35"/>
       <c r="F138" s="5"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -2952,8 +2952,8 @@
       <c r="C139" s="9">
         <v>45272</v>
       </c>
-      <c r="D139" s="34"/>
-      <c r="E139" s="31"/>
+      <c r="D139" s="29"/>
+      <c r="E139" s="35"/>
       <c r="F139" s="5"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -2966,8 +2966,8 @@
       <c r="C140" s="9">
         <v>45273</v>
       </c>
-      <c r="D140" s="34"/>
-      <c r="E140" s="31"/>
+      <c r="D140" s="29"/>
+      <c r="E140" s="35"/>
       <c r="F140" s="5"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -2980,8 +2980,8 @@
       <c r="C141" s="9">
         <v>45274</v>
       </c>
-      <c r="D141" s="34"/>
-      <c r="E141" s="31"/>
+      <c r="D141" s="29"/>
+      <c r="E141" s="35"/>
       <c r="F141" s="5"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -2994,8 +2994,8 @@
       <c r="C142" s="9">
         <v>45278</v>
       </c>
-      <c r="D142" s="34"/>
-      <c r="E142" s="31"/>
+      <c r="D142" s="29"/>
+      <c r="E142" s="35"/>
       <c r="F142" s="5"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -3008,8 +3008,8 @@
       <c r="C143" s="9">
         <v>45279</v>
       </c>
-      <c r="D143" s="34"/>
-      <c r="E143" s="31"/>
+      <c r="D143" s="29"/>
+      <c r="E143" s="35"/>
       <c r="F143" s="5"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -3022,8 +3022,8 @@
       <c r="C144" s="9">
         <v>45280</v>
       </c>
-      <c r="D144" s="35"/>
-      <c r="E144" s="32"/>
+      <c r="D144" s="30"/>
+      <c r="E144" s="34"/>
       <c r="F144" s="5" t="s">
         <v>63</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>45299</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="30" t="s">
+      <c r="E153" s="33" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="5"/>
@@ -3161,7 +3161,7 @@
         <v>45300</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="31"/>
+      <c r="E154" s="35"/>
       <c r="F154" s="5"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -3175,7 +3175,7 @@
         <v>45301</v>
       </c>
       <c r="D155" s="6"/>
-      <c r="E155" s="31"/>
+      <c r="E155" s="35"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -3189,7 +3189,7 @@
         <v>45302</v>
       </c>
       <c r="D156" s="6"/>
-      <c r="E156" s="31"/>
+      <c r="E156" s="35"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -3203,7 +3203,7 @@
         <v>45306</v>
       </c>
       <c r="D157" s="6"/>
-      <c r="E157" s="31"/>
+      <c r="E157" s="35"/>
       <c r="F157" s="5"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -3217,7 +3217,7 @@
         <v>45307</v>
       </c>
       <c r="D158" s="6"/>
-      <c r="E158" s="31"/>
+      <c r="E158" s="35"/>
       <c r="F158" s="5"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>45308</v>
       </c>
       <c r="D159" s="6"/>
-      <c r="E159" s="31"/>
+      <c r="E159" s="35"/>
       <c r="F159" s="5"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3245,7 +3245,7 @@
         <v>45309</v>
       </c>
       <c r="D160" s="6"/>
-      <c r="E160" s="31"/>
+      <c r="E160" s="35"/>
       <c r="F160" s="5"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
         <v>45313</v>
       </c>
       <c r="D161" s="6"/>
-      <c r="E161" s="31"/>
+      <c r="E161" s="35"/>
       <c r="F161" s="5"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3273,7 +3273,7 @@
         <v>45314</v>
       </c>
       <c r="D162" s="6"/>
-      <c r="E162" s="31"/>
+      <c r="E162" s="35"/>
       <c r="F162" s="12"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3287,7 +3287,7 @@
         <v>45315</v>
       </c>
       <c r="D163" s="6"/>
-      <c r="E163" s="31"/>
+      <c r="E163" s="35"/>
       <c r="F163" s="12"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3301,7 +3301,7 @@
         <v>45316</v>
       </c>
       <c r="D164" s="6"/>
-      <c r="E164" s="31"/>
+      <c r="E164" s="35"/>
       <c r="F164" s="12"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3315,7 +3315,7 @@
         <v>45320</v>
       </c>
       <c r="D165" s="6"/>
-      <c r="E165" s="31"/>
+      <c r="E165" s="35"/>
       <c r="F165" s="12"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3329,7 +3329,7 @@
         <v>45321</v>
       </c>
       <c r="D166" s="6"/>
-      <c r="E166" s="31"/>
+      <c r="E166" s="35"/>
       <c r="F166" s="12"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
         <v>45322</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="31"/>
+      <c r="E167" s="35"/>
       <c r="F167" s="12"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3357,7 +3357,7 @@
         <v>45323</v>
       </c>
       <c r="D168" s="6"/>
-      <c r="E168" s="31"/>
+      <c r="E168" s="35"/>
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3371,7 +3371,7 @@
         <v>45327</v>
       </c>
       <c r="D169" s="6"/>
-      <c r="E169" s="31"/>
+      <c r="E169" s="35"/>
       <c r="F169" s="12"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3385,7 +3385,7 @@
         <v>45328</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="31"/>
+      <c r="E170" s="35"/>
       <c r="F170" s="12"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -3399,7 +3399,7 @@
         <v>45329</v>
       </c>
       <c r="D171" s="6"/>
-      <c r="E171" s="31"/>
+      <c r="E171" s="35"/>
       <c r="F171" s="12"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3413,7 +3413,7 @@
         <v>45330</v>
       </c>
       <c r="D172" s="6"/>
-      <c r="E172" s="31"/>
+      <c r="E172" s="35"/>
       <c r="F172" s="12"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3427,7 +3427,7 @@
         <v>45334</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="31"/>
+      <c r="E173" s="35"/>
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3441,7 +3441,7 @@
         <v>45335</v>
       </c>
       <c r="D174" s="6"/>
-      <c r="E174" s="31"/>
+      <c r="E174" s="35"/>
       <c r="F174" s="12"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3455,7 +3455,7 @@
         <v>45336</v>
       </c>
       <c r="D175" s="6"/>
-      <c r="E175" s="31"/>
+      <c r="E175" s="35"/>
       <c r="F175" s="12"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3469,7 +3469,7 @@
         <v>45337</v>
       </c>
       <c r="D176" s="6"/>
-      <c r="E176" s="31"/>
+      <c r="E176" s="35"/>
       <c r="F176" s="12"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -3483,7 +3483,7 @@
         <v>45341</v>
       </c>
       <c r="D177" s="6"/>
-      <c r="E177" s="31"/>
+      <c r="E177" s="35"/>
       <c r="F177" s="12"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -3497,7 +3497,7 @@
         <v>45342</v>
       </c>
       <c r="D178" s="6"/>
-      <c r="E178" s="31"/>
+      <c r="E178" s="35"/>
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -3511,7 +3511,7 @@
         <v>45343</v>
       </c>
       <c r="D179" s="6"/>
-      <c r="E179" s="32"/>
+      <c r="E179" s="34"/>
       <c r="F179" s="12"/>
     </row>
   </sheetData>
@@ -3519,11 +3519,27 @@
     <sortCondition ref="D3:J3"/>
   </sortState>
   <mergeCells count="41">
-    <mergeCell ref="D71:D80"/>
-    <mergeCell ref="D81:D91"/>
-    <mergeCell ref="D30:D39"/>
-    <mergeCell ref="D40:D59"/>
-    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="E96:E104"/>
+    <mergeCell ref="D96:D104"/>
+    <mergeCell ref="E153:E179"/>
+    <mergeCell ref="D106:D109"/>
+    <mergeCell ref="E106:E109"/>
+    <mergeCell ref="D110:D117"/>
+    <mergeCell ref="E110:E117"/>
+    <mergeCell ref="D119:D131"/>
+    <mergeCell ref="E119:E131"/>
+    <mergeCell ref="E133:E144"/>
+    <mergeCell ref="D133:D144"/>
+    <mergeCell ref="E71:E80"/>
+    <mergeCell ref="E81:E91"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F57:F58"/>
     <mergeCell ref="E30:E39"/>
     <mergeCell ref="D62:D70"/>
     <mergeCell ref="D3:D4"/>
@@ -3539,27 +3555,11 @@
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="E40:E59"/>
     <mergeCell ref="E62:E70"/>
-    <mergeCell ref="E71:E80"/>
-    <mergeCell ref="E81:E91"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="F51:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="E96:E104"/>
-    <mergeCell ref="D96:D104"/>
-    <mergeCell ref="E153:E179"/>
-    <mergeCell ref="D106:D109"/>
-    <mergeCell ref="E106:E109"/>
-    <mergeCell ref="D110:D117"/>
-    <mergeCell ref="E110:E117"/>
-    <mergeCell ref="D119:D131"/>
-    <mergeCell ref="E119:E131"/>
-    <mergeCell ref="E133:E144"/>
-    <mergeCell ref="D133:D144"/>
+    <mergeCell ref="D71:D80"/>
+    <mergeCell ref="D81:D91"/>
+    <mergeCell ref="D30:D39"/>
+    <mergeCell ref="D40:D59"/>
+    <mergeCell ref="D60:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>